<commit_message>
document within run pooling
</commit_message>
<xml_diff>
--- a/documentation/config_explained.xlsx
+++ b/documentation/config_explained.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/heintzbu/Documents/Programs/myOwn/dadasnake/documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E95A545-5648-C04B-8A04-C640CD1FCE1C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C49CB1C-8870-C349-A469-2EB3FCE9F04B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="460" windowWidth="16980" windowHeight="17040" xr2:uid="{F207B228-D75F-344A-ADB6-4CA41A47821F}"/>
+    <workbookView xWindow="380" yWindow="460" windowWidth="22800" windowHeight="16900" xr2:uid="{F207B228-D75F-344A-ADB6-4CA41A47821F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -498,15 +498,9 @@
     <t xml:space="preserve"> false</t>
   </si>
   <si>
-    <t>true, false or "pseudo"</t>
-  </si>
-  <si>
     <t>Should DADA2 be run per sample (default) or in a pool, or should pseudo-pooling be done?</t>
   </si>
   <si>
-    <t xml:space="preserve"> default is good for Illumina and much more efficient for large data sets; set to true for 454, pacbio and nanopore; set to pseudo for non-huge datasets, if you're interested in rare ASVs.</t>
-  </si>
-  <si>
     <t xml:space="preserve">  omega_A</t>
   </si>
   <si>
@@ -1234,6 +1228,12 @@
   </si>
   <si>
     <t>"../DBs/functions/funguild_db.json"</t>
+  </si>
+  <si>
+    <t>true, false, "pseudo", or "within_run"</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> default is good for Illumina and much more efficient for large data sets; set to true for 454, pacbio and nanopore; set to pseudo for non-huge datasets, if you're interested in rare ASVs. You can also run pooling run-wise, which will increase sensitivity towards rare ASVs - however, take care with this setting, because run-specific biases can be strengthened and it's not advisable, if runs have vastly different sizes.</t>
   </si>
 </sst>
 </file>
@@ -1278,13 +1278,13 @@
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1601,8 +1601,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{61B259DD-FAC6-FB4A-84F8-11B4141970E7}">
   <dimension ref="A1:H138"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A121" workbookViewId="0">
-      <selection activeCell="D134" sqref="D134"/>
+    <sheetView tabSelected="1" topLeftCell="D50" workbookViewId="0">
+      <selection activeCell="E56" sqref="E56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1619,28 +1619,28 @@
   <sheetData>
     <row r="1" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>344</v>
+      </c>
+      <c r="B1" t="s">
+        <v>345</v>
+      </c>
+      <c r="C1" t="s">
         <v>346</v>
       </c>
-      <c r="B1" t="s">
+      <c r="D1" t="s">
         <v>347</v>
       </c>
-      <c r="C1" t="s">
+      <c r="E1" s="2" t="s">
         <v>348</v>
       </c>
-      <c r="D1" t="s">
+      <c r="F1" t="s">
         <v>349</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="G1" s="2" t="s">
         <v>350</v>
       </c>
-      <c r="F1" t="s">
+      <c r="H1" s="2" t="s">
         <v>351</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>352</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>353</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="34" x14ac:dyDescent="0.2">
@@ -1666,147 +1666,147 @@
         <v>6</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
+        <v>354</v>
+      </c>
+      <c r="D3" t="s">
+        <v>281</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>355</v>
+      </c>
+      <c r="F3" t="s">
         <v>356</v>
       </c>
-      <c r="D3" t="s">
-        <v>283</v>
-      </c>
-      <c r="E3" s="2" t="s">
+      <c r="G3" s="2" t="s">
         <v>357</v>
       </c>
-      <c r="F3" t="s">
+      <c r="H3" s="2" t="s">
         <v>358</v>
-      </c>
-      <c r="G3" s="2" t="s">
-        <v>359</v>
-      </c>
-      <c r="H3" s="2" t="s">
-        <v>360</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
       <c r="D4" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
       <c r="F4" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="H4" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="D5" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
       <c r="F5" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
       <c r="G5" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
       <c r="H5" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
       <c r="D6" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
       <c r="F6" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
       <c r="G6" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="H6" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
       <c r="D7" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="F7" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
       <c r="G7" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
       <c r="H7" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>365</v>
-      </c>
-      <c r="D8" s="6" t="s">
-        <v>366</v>
+        <v>363</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>364</v>
       </c>
       <c r="E8" s="2" t="s">
         <v>63</v>
       </c>
       <c r="F8" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
       <c r="G8" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
       <c r="H8" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
     </row>
     <row r="9" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>378</v>
-      </c>
-      <c r="D9" s="6" t="s">
-        <v>366</v>
+        <v>376</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>364</v>
       </c>
       <c r="E9" s="2" t="s">
         <v>63</v>
       </c>
       <c r="F9" t="s">
+        <v>377</v>
+      </c>
+      <c r="G9" t="s">
+        <v>378</v>
+      </c>
+      <c r="H9" t="s">
         <v>379</v>
-      </c>
-      <c r="G9" t="s">
-        <v>380</v>
-      </c>
-      <c r="H9" t="s">
-        <v>381</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="34" x14ac:dyDescent="0.2">
@@ -2015,7 +2015,7 @@
       </c>
     </row>
     <row r="18" spans="1:8" ht="17" x14ac:dyDescent="0.2">
-      <c r="A18" s="4" t="s">
+      <c r="A18" s="5" t="s">
         <v>36</v>
       </c>
       <c r="B18" t="s">
@@ -2041,8 +2041,8 @@
       </c>
     </row>
     <row r="19" spans="1:8" ht="17" x14ac:dyDescent="0.2">
-      <c r="A19" s="4"/>
-      <c r="B19" s="5" t="s">
+      <c r="A19" s="5"/>
+      <c r="B19" s="6" t="s">
         <v>39</v>
       </c>
       <c r="C19" t="s">
@@ -2065,8 +2065,8 @@
       </c>
     </row>
     <row r="20" spans="1:8" ht="17" x14ac:dyDescent="0.2">
-      <c r="A20" s="4"/>
-      <c r="B20" s="5"/>
+      <c r="A20" s="5"/>
+      <c r="B20" s="6"/>
       <c r="C20" t="s">
         <v>41</v>
       </c>
@@ -2084,8 +2084,8 @@
       </c>
     </row>
     <row r="21" spans="1:8" ht="17" x14ac:dyDescent="0.2">
-      <c r="A21" s="4"/>
-      <c r="B21" s="5"/>
+      <c r="A21" s="5"/>
+      <c r="B21" s="6"/>
       <c r="C21" t="s">
         <v>45</v>
       </c>
@@ -2106,8 +2106,8 @@
       </c>
     </row>
     <row r="22" spans="1:8" ht="17" x14ac:dyDescent="0.2">
-      <c r="A22" s="4"/>
-      <c r="B22" s="4" t="s">
+      <c r="A22" s="5"/>
+      <c r="B22" s="5" t="s">
         <v>50</v>
       </c>
       <c r="C22" t="s">
@@ -2130,8 +2130,8 @@
       </c>
     </row>
     <row r="23" spans="1:8" ht="17" x14ac:dyDescent="0.2">
-      <c r="A23" s="4"/>
-      <c r="B23" s="4"/>
+      <c r="A23" s="5"/>
+      <c r="B23" s="5"/>
       <c r="C23" t="s">
         <v>52</v>
       </c>
@@ -2149,8 +2149,8 @@
       </c>
     </row>
     <row r="24" spans="1:8" ht="17" x14ac:dyDescent="0.2">
-      <c r="A24" s="4"/>
-      <c r="B24" s="4"/>
+      <c r="A24" s="5"/>
+      <c r="B24" s="5"/>
       <c r="C24" t="s">
         <v>57</v>
       </c>
@@ -2211,7 +2211,7 @@
       </c>
     </row>
     <row r="27" spans="1:8" ht="17" x14ac:dyDescent="0.2">
-      <c r="A27" s="4" t="s">
+      <c r="A27" s="5" t="s">
         <v>72</v>
       </c>
       <c r="F27" t="s">
@@ -2222,7 +2222,7 @@
       </c>
     </row>
     <row r="28" spans="1:8" ht="17" x14ac:dyDescent="0.2">
-      <c r="A28" s="4"/>
+      <c r="A28" s="5"/>
       <c r="B28" t="s">
         <v>74</v>
       </c>
@@ -2240,7 +2240,7 @@
       </c>
     </row>
     <row r="29" spans="1:8" ht="34" x14ac:dyDescent="0.2">
-      <c r="A29" s="4"/>
+      <c r="A29" s="5"/>
       <c r="B29" t="s">
         <v>77</v>
       </c>
@@ -2258,7 +2258,7 @@
       </c>
     </row>
     <row r="30" spans="1:8" ht="34" x14ac:dyDescent="0.2">
-      <c r="A30" s="4"/>
+      <c r="A30" s="5"/>
       <c r="B30" t="s">
         <v>80</v>
       </c>
@@ -2279,7 +2279,7 @@
       </c>
     </row>
     <row r="31" spans="1:8" ht="17" x14ac:dyDescent="0.2">
-      <c r="A31" s="4"/>
+      <c r="A31" s="5"/>
       <c r="B31" t="s">
         <v>85</v>
       </c>
@@ -2300,7 +2300,7 @@
       </c>
     </row>
     <row r="32" spans="1:8" ht="34" x14ac:dyDescent="0.2">
-      <c r="A32" s="4"/>
+      <c r="A32" s="5"/>
       <c r="B32" t="s">
         <v>89</v>
       </c>
@@ -2318,7 +2318,7 @@
       </c>
     </row>
     <row r="33" spans="1:8" ht="34" x14ac:dyDescent="0.2">
-      <c r="A33" s="4"/>
+      <c r="A33" s="5"/>
       <c r="B33" t="s">
         <v>93</v>
       </c>
@@ -2339,7 +2339,7 @@
       </c>
     </row>
     <row r="34" spans="1:8" ht="102" x14ac:dyDescent="0.2">
-      <c r="A34" s="4" t="s">
+      <c r="A34" s="5" t="s">
         <v>97</v>
       </c>
       <c r="B34" t="s">
@@ -2365,8 +2365,8 @@
       </c>
     </row>
     <row r="35" spans="1:8" ht="17" x14ac:dyDescent="0.2">
-      <c r="A35" s="4"/>
-      <c r="B35" s="4" t="s">
+      <c r="A35" s="5"/>
+      <c r="B35" s="5" t="s">
         <v>100</v>
       </c>
       <c r="F35" t="s">
@@ -2377,8 +2377,8 @@
       </c>
     </row>
     <row r="36" spans="1:8" ht="51" x14ac:dyDescent="0.2">
-      <c r="A36" s="4"/>
-      <c r="B36" s="4"/>
+      <c r="A36" s="5"/>
+      <c r="B36" s="5"/>
       <c r="C36" t="s">
         <v>103</v>
       </c>
@@ -2399,8 +2399,8 @@
       </c>
     </row>
     <row r="37" spans="1:8" ht="51" x14ac:dyDescent="0.2">
-      <c r="A37" s="4"/>
-      <c r="B37" s="4"/>
+      <c r="A37" s="5"/>
+      <c r="B37" s="5"/>
       <c r="C37" t="s">
         <v>106</v>
       </c>
@@ -2421,7 +2421,7 @@
       </c>
     </row>
     <row r="38" spans="1:8" ht="34" x14ac:dyDescent="0.2">
-      <c r="A38" s="4"/>
+      <c r="A38" s="5"/>
       <c r="B38" t="s">
         <v>109</v>
       </c>
@@ -2439,8 +2439,8 @@
       </c>
     </row>
     <row r="39" spans="1:8" ht="51" x14ac:dyDescent="0.2">
-      <c r="A39" s="4"/>
-      <c r="B39" s="4" t="s">
+      <c r="A39" s="5"/>
+      <c r="B39" s="5" t="s">
         <v>112</v>
       </c>
       <c r="F39" t="s">
@@ -2451,8 +2451,8 @@
       </c>
     </row>
     <row r="40" spans="1:8" ht="51" x14ac:dyDescent="0.2">
-      <c r="A40" s="4"/>
-      <c r="B40" s="4"/>
+      <c r="A40" s="5"/>
+      <c r="B40" s="5"/>
       <c r="C40" t="s">
         <v>114</v>
       </c>
@@ -2473,8 +2473,8 @@
       </c>
     </row>
     <row r="41" spans="1:8" ht="68" x14ac:dyDescent="0.2">
-      <c r="A41" s="4"/>
-      <c r="B41" s="4"/>
+      <c r="A41" s="5"/>
+      <c r="B41" s="5"/>
       <c r="C41" t="s">
         <v>106</v>
       </c>
@@ -2495,8 +2495,8 @@
       </c>
     </row>
     <row r="42" spans="1:8" ht="17" x14ac:dyDescent="0.2">
-      <c r="A42" s="4"/>
-      <c r="B42" s="4" t="s">
+      <c r="A42" s="5"/>
+      <c r="B42" s="5" t="s">
         <v>121</v>
       </c>
       <c r="F42" t="s">
@@ -2507,8 +2507,8 @@
       </c>
     </row>
     <row r="43" spans="1:8" ht="51" x14ac:dyDescent="0.2">
-      <c r="A43" s="4"/>
-      <c r="B43" s="4"/>
+      <c r="A43" s="5"/>
+      <c r="B43" s="5"/>
       <c r="C43" t="s">
         <v>103</v>
       </c>
@@ -2529,8 +2529,8 @@
       </c>
     </row>
     <row r="44" spans="1:8" ht="51" x14ac:dyDescent="0.2">
-      <c r="A44" s="4"/>
-      <c r="B44" s="4"/>
+      <c r="A44" s="5"/>
+      <c r="B44" s="5"/>
       <c r="C44" t="s">
         <v>106</v>
       </c>
@@ -2551,8 +2551,8 @@
       </c>
     </row>
     <row r="45" spans="1:8" ht="17" x14ac:dyDescent="0.2">
-      <c r="A45" s="4"/>
-      <c r="B45" s="4" t="s">
+      <c r="A45" s="5"/>
+      <c r="B45" s="5" t="s">
         <v>127</v>
       </c>
       <c r="F45" t="s">
@@ -2563,8 +2563,8 @@
       </c>
     </row>
     <row r="46" spans="1:8" ht="51" x14ac:dyDescent="0.2">
-      <c r="A46" s="4"/>
-      <c r="B46" s="4"/>
+      <c r="A46" s="5"/>
+      <c r="B46" s="5"/>
       <c r="C46" t="s">
         <v>103</v>
       </c>
@@ -2582,8 +2582,8 @@
       </c>
     </row>
     <row r="47" spans="1:8" ht="51" x14ac:dyDescent="0.2">
-      <c r="A47" s="4"/>
-      <c r="B47" s="4"/>
+      <c r="A47" s="5"/>
+      <c r="B47" s="5"/>
       <c r="C47" t="s">
         <v>106</v>
       </c>
@@ -2604,8 +2604,8 @@
       </c>
     </row>
     <row r="48" spans="1:8" ht="17" x14ac:dyDescent="0.2">
-      <c r="A48" s="4"/>
-      <c r="B48" s="4" t="s">
+      <c r="A48" s="5"/>
+      <c r="B48" s="5" t="s">
         <v>134</v>
       </c>
       <c r="F48" t="s">
@@ -2616,8 +2616,8 @@
       </c>
     </row>
     <row r="49" spans="1:8" ht="51" x14ac:dyDescent="0.2">
-      <c r="A49" s="4"/>
-      <c r="B49" s="4"/>
+      <c r="A49" s="5"/>
+      <c r="B49" s="5"/>
       <c r="C49" t="s">
         <v>103</v>
       </c>
@@ -2638,8 +2638,8 @@
       </c>
     </row>
     <row r="50" spans="1:8" ht="51" x14ac:dyDescent="0.2">
-      <c r="A50" s="4"/>
-      <c r="B50" s="4"/>
+      <c r="A50" s="5"/>
+      <c r="B50" s="5"/>
       <c r="C50" t="s">
         <v>106</v>
       </c>
@@ -2691,7 +2691,7 @@
       </c>
     </row>
     <row r="53" spans="1:8" ht="51" x14ac:dyDescent="0.2">
-      <c r="A53" s="4"/>
+      <c r="A53" s="5"/>
       <c r="B53" t="s">
         <v>146</v>
       </c>
@@ -2712,7 +2712,7 @@
       </c>
     </row>
     <row r="54" spans="1:8" ht="68" x14ac:dyDescent="0.2">
-      <c r="A54" s="4"/>
+      <c r="A54" s="5"/>
       <c r="B54" t="s">
         <v>149</v>
       </c>
@@ -2732,8 +2732,8 @@
         <v>153</v>
       </c>
     </row>
-    <row r="55" spans="1:8" ht="68" x14ac:dyDescent="0.2">
-      <c r="A55" s="4"/>
+    <row r="55" spans="1:8" ht="136" x14ac:dyDescent="0.2">
+      <c r="A55" s="5"/>
       <c r="B55" t="s">
         <v>154</v>
       </c>
@@ -2741,106 +2741,106 @@
         <v>155</v>
       </c>
       <c r="E55" s="2" t="s">
+        <v>400</v>
+      </c>
+      <c r="F55" t="s">
+        <v>101</v>
+      </c>
+      <c r="G55" s="2" t="s">
         <v>156</v>
       </c>
-      <c r="F55" t="s">
-        <v>101</v>
-      </c>
-      <c r="G55" s="2" t="s">
+      <c r="H55" s="2" t="s">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="56" spans="1:8" ht="51" x14ac:dyDescent="0.2">
+      <c r="A56" s="5"/>
+      <c r="B56" t="s">
         <v>157</v>
-      </c>
-      <c r="H55" s="2" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="56" spans="1:8" ht="51" x14ac:dyDescent="0.2">
-      <c r="A56" s="4"/>
-      <c r="B56" t="s">
-        <v>159</v>
       </c>
       <c r="D56" s="1">
         <v>9.9999999999999993E-41</v>
       </c>
       <c r="E56" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="F56" t="s">
+        <v>101</v>
+      </c>
+      <c r="G56" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="H56" s="2" t="s">
         <v>160</v>
       </c>
-      <c r="F56" t="s">
-        <v>101</v>
-      </c>
-      <c r="G56" s="2" t="s">
+    </row>
+    <row r="57" spans="1:8" ht="34" x14ac:dyDescent="0.2">
+      <c r="A57" s="5"/>
+      <c r="B57" t="s">
         <v>161</v>
       </c>
-      <c r="H56" s="2" t="s">
+      <c r="D57" t="s">
         <v>162</v>
       </c>
-    </row>
-    <row r="57" spans="1:8" ht="34" x14ac:dyDescent="0.2">
-      <c r="A57" s="4"/>
-      <c r="B57" t="s">
+      <c r="E57" s="2" t="s">
         <v>163</v>
       </c>
-      <c r="D57" t="s">
+      <c r="F57" t="s">
+        <v>101</v>
+      </c>
+      <c r="G57" s="2" t="s">
         <v>164</v>
       </c>
-      <c r="E57" s="2" t="s">
+      <c r="H57" s="2" t="s">
         <v>165</v>
       </c>
-      <c r="F57" t="s">
-        <v>101</v>
-      </c>
-      <c r="G57" s="2" t="s">
+    </row>
+    <row r="58" spans="1:8" ht="34" x14ac:dyDescent="0.2">
+      <c r="A58" s="5"/>
+      <c r="B58" t="s">
         <v>166</v>
-      </c>
-      <c r="H57" s="2" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="58" spans="1:8" ht="34" x14ac:dyDescent="0.2">
-      <c r="A58" s="4"/>
-      <c r="B58" t="s">
-        <v>168</v>
       </c>
       <c r="D58" s="1">
         <v>1E-4</v>
       </c>
       <c r="E58" s="2" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="F58" t="s">
         <v>101</v>
       </c>
       <c r="G58" s="2" t="s">
+        <v>167</v>
+      </c>
+      <c r="H58" s="2" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="59" spans="1:8" ht="34" x14ac:dyDescent="0.2">
+      <c r="A59" s="5"/>
+      <c r="B59" t="s">
         <v>169</v>
-      </c>
-      <c r="H58" s="2" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="59" spans="1:8" ht="34" x14ac:dyDescent="0.2">
-      <c r="A59" s="4"/>
-      <c r="B59" t="s">
-        <v>171</v>
       </c>
       <c r="D59" s="1">
         <v>9.9999999999999993E-41</v>
       </c>
       <c r="E59" s="2" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="F59" t="s">
         <v>101</v>
       </c>
       <c r="G59" s="2" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="H59" s="2" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
     </row>
     <row r="60" spans="1:8" ht="51" x14ac:dyDescent="0.2">
-      <c r="A60" s="4"/>
+      <c r="A60" s="5"/>
       <c r="B60" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="D60" t="s">
         <v>155</v>
@@ -2852,16 +2852,16 @@
         <v>101</v>
       </c>
       <c r="G60" s="2" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="H60" s="2" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
     </row>
     <row r="61" spans="1:8" ht="51" x14ac:dyDescent="0.2">
-      <c r="A61" s="4"/>
+      <c r="A61" s="5"/>
       <c r="B61" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="D61" t="s">
         <v>155</v>
@@ -2873,37 +2873,37 @@
         <v>101</v>
       </c>
       <c r="G61" s="2" t="s">
+        <v>174</v>
+      </c>
+      <c r="H61" s="2" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="62" spans="1:8" ht="51" x14ac:dyDescent="0.2">
+      <c r="A62" s="5"/>
+      <c r="B62" t="s">
+        <v>175</v>
+      </c>
+      <c r="D62" t="s">
         <v>176</v>
       </c>
-      <c r="H61" s="2" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="62" spans="1:8" ht="51" x14ac:dyDescent="0.2">
-      <c r="A62" s="4"/>
-      <c r="B62" t="s">
+      <c r="E62" s="2" t="s">
         <v>177</v>
       </c>
-      <c r="D62" t="s">
+      <c r="F62" t="s">
+        <v>101</v>
+      </c>
+      <c r="G62" s="2" t="s">
         <v>178</v>
       </c>
-      <c r="E62" s="2" t="s">
+      <c r="H62" s="2" t="s">
         <v>179</v>
       </c>
-      <c r="F62" t="s">
-        <v>101</v>
-      </c>
-      <c r="G62" s="2" t="s">
+    </row>
+    <row r="63" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="A63" s="5"/>
+      <c r="B63" t="s">
         <v>180</v>
-      </c>
-      <c r="H62" s="2" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="63" spans="1:8" ht="17" x14ac:dyDescent="0.2">
-      <c r="A63" s="4"/>
-      <c r="B63" t="s">
-        <v>182</v>
       </c>
       <c r="D63" t="s">
         <v>62</v>
@@ -2915,16 +2915,16 @@
         <v>101</v>
       </c>
       <c r="G63" s="2" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="H63" s="2" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
     </row>
     <row r="64" spans="1:8" ht="34" x14ac:dyDescent="0.2">
-      <c r="A64" s="4"/>
+      <c r="A64" s="5"/>
       <c r="B64" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="D64" t="s">
         <v>62</v>
@@ -2936,111 +2936,111 @@
         <v>101</v>
       </c>
       <c r="G64" s="2" t="s">
+        <v>183</v>
+      </c>
+      <c r="H64" s="2" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="65" spans="1:8" ht="51" x14ac:dyDescent="0.2">
+      <c r="A65" s="5"/>
+      <c r="B65" t="s">
         <v>185</v>
-      </c>
-      <c r="H64" s="2" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="65" spans="1:8" ht="51" x14ac:dyDescent="0.2">
-      <c r="A65" s="4"/>
-      <c r="B65" t="s">
-        <v>187</v>
       </c>
       <c r="D65">
         <v>0.42</v>
       </c>
       <c r="E65" s="2" t="s">
+        <v>186</v>
+      </c>
+      <c r="F65" t="s">
+        <v>101</v>
+      </c>
+      <c r="G65" s="2" t="s">
+        <v>187</v>
+      </c>
+      <c r="H65" s="2" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="66" spans="1:8" ht="34" x14ac:dyDescent="0.2">
+      <c r="A66" s="5"/>
+      <c r="B66" t="s">
         <v>188</v>
-      </c>
-      <c r="F65" t="s">
-        <v>101</v>
-      </c>
-      <c r="G65" s="2" t="s">
-        <v>189</v>
-      </c>
-      <c r="H65" s="2" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="66" spans="1:8" ht="34" x14ac:dyDescent="0.2">
-      <c r="A66" s="4"/>
-      <c r="B66" t="s">
-        <v>190</v>
       </c>
       <c r="D66">
         <v>4</v>
       </c>
       <c r="E66" s="2" t="s">
+        <v>189</v>
+      </c>
+      <c r="F66" t="s">
+        <v>101</v>
+      </c>
+      <c r="G66" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="H66" s="2" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="67" spans="1:8" ht="34" x14ac:dyDescent="0.2">
+      <c r="A67" s="5"/>
+      <c r="B67" t="s">
         <v>191</v>
-      </c>
-      <c r="F66" t="s">
-        <v>101</v>
-      </c>
-      <c r="G66" s="2" t="s">
-        <v>192</v>
-      </c>
-      <c r="H66" s="2" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="67" spans="1:8" ht="34" x14ac:dyDescent="0.2">
-      <c r="A67" s="4"/>
-      <c r="B67" t="s">
-        <v>193</v>
       </c>
       <c r="D67">
         <v>-5</v>
       </c>
       <c r="E67" s="2" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="F67" t="s">
         <v>101</v>
       </c>
       <c r="G67" s="2" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="H67" s="2" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
     </row>
     <row r="68" spans="1:8" ht="85" x14ac:dyDescent="0.2">
-      <c r="A68" s="4"/>
+      <c r="A68" s="5"/>
       <c r="B68" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="D68">
         <v>-8</v>
       </c>
       <c r="E68" s="2" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="F68" t="s">
         <v>101</v>
       </c>
       <c r="G68" s="2" t="s">
+        <v>194</v>
+      </c>
+      <c r="H68" s="2" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="69" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="A69" s="5" t="s">
+        <v>195</v>
+      </c>
+      <c r="F69" t="s">
+        <v>101</v>
+      </c>
+      <c r="H69" s="2" t="s">
         <v>196</v>
       </c>
-      <c r="H68" s="2" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="69" spans="1:8" ht="17" x14ac:dyDescent="0.2">
-      <c r="A69" s="4" t="s">
+    </row>
+    <row r="70" spans="1:8" ht="34" x14ac:dyDescent="0.2">
+      <c r="A70" s="5"/>
+      <c r="B70" t="s">
         <v>197</v>
-      </c>
-      <c r="F69" t="s">
-        <v>101</v>
-      </c>
-      <c r="H69" s="2" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="70" spans="1:8" ht="34" x14ac:dyDescent="0.2">
-      <c r="A70" s="4"/>
-      <c r="B70" t="s">
-        <v>199</v>
       </c>
       <c r="D70">
         <v>12</v>
@@ -3052,37 +3052,37 @@
         <v>101</v>
       </c>
       <c r="G70" s="2" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="H70" s="2" t="s">
         <v>133</v>
       </c>
     </row>
     <row r="71" spans="1:8" ht="34" x14ac:dyDescent="0.2">
-      <c r="A71" s="4"/>
+      <c r="A71" s="5"/>
       <c r="B71" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="D71">
         <v>0</v>
       </c>
       <c r="E71" s="2" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="F71" t="s">
         <v>101</v>
       </c>
       <c r="G71" s="2" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="H71" s="2" t="s">
         <v>133</v>
       </c>
     </row>
     <row r="72" spans="1:8" ht="68" x14ac:dyDescent="0.2">
-      <c r="A72" s="4"/>
+      <c r="A72" s="5"/>
       <c r="B72" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="D72" t="s">
         <v>155</v>
@@ -3094,16 +3094,16 @@
         <v>101</v>
       </c>
       <c r="G72" s="2" t="s">
+        <v>203</v>
+      </c>
+      <c r="H72" s="2" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="73" spans="1:8" ht="34" x14ac:dyDescent="0.2">
+      <c r="A73" s="5"/>
+      <c r="B73" t="s">
         <v>205</v>
-      </c>
-      <c r="H72" s="2" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="73" spans="1:8" ht="34" x14ac:dyDescent="0.2">
-      <c r="A73" s="4"/>
-      <c r="B73" t="s">
-        <v>207</v>
       </c>
       <c r="D73" t="s">
         <v>62</v>
@@ -3115,27 +3115,27 @@
         <v>101</v>
       </c>
       <c r="G73" s="2" t="s">
+        <v>206</v>
+      </c>
+      <c r="H73" s="2" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="74" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="A74" s="5" t="s">
         <v>208</v>
       </c>
-      <c r="H73" s="2" t="s">
+      <c r="F74" t="s">
+        <v>101</v>
+      </c>
+      <c r="H74" s="2" t="s">
         <v>209</v>
       </c>
     </row>
-    <row r="74" spans="1:8" ht="17" x14ac:dyDescent="0.2">
-      <c r="A74" s="4" t="s">
+    <row r="75" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="A75" s="5"/>
+      <c r="B75" t="s">
         <v>210</v>
-      </c>
-      <c r="F74" t="s">
-        <v>101</v>
-      </c>
-      <c r="H74" s="2" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="75" spans="1:8" ht="17" x14ac:dyDescent="0.2">
-      <c r="A75" s="4"/>
-      <c r="B75" t="s">
-        <v>212</v>
       </c>
       <c r="D75" t="s">
         <v>62</v>
@@ -3147,76 +3147,76 @@
         <v>101</v>
       </c>
       <c r="G75" s="2" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="76" spans="1:8" ht="85" x14ac:dyDescent="0.2">
+      <c r="A76" s="5"/>
+      <c r="B76" t="s">
+        <v>212</v>
+      </c>
+      <c r="D76" t="s">
         <v>213</v>
       </c>
-    </row>
-    <row r="76" spans="1:8" ht="85" x14ac:dyDescent="0.2">
-      <c r="A76" s="4"/>
-      <c r="B76" t="s">
+      <c r="E76" s="2" t="s">
         <v>214</v>
       </c>
-      <c r="D76" t="s">
+      <c r="F76" t="s">
+        <v>101</v>
+      </c>
+      <c r="G76" s="2" t="s">
         <v>215</v>
       </c>
-      <c r="E76" s="2" t="s">
+      <c r="H76" s="2" t="s">
         <v>216</v>
       </c>
-      <c r="F76" t="s">
-        <v>101</v>
-      </c>
-      <c r="G76" s="2" t="s">
+    </row>
+    <row r="77" spans="1:8" ht="34" x14ac:dyDescent="0.2">
+      <c r="A77" s="5"/>
+      <c r="B77" t="s">
         <v>217</v>
-      </c>
-      <c r="H76" s="2" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="77" spans="1:8" ht="34" x14ac:dyDescent="0.2">
-      <c r="A77" s="4"/>
-      <c r="B77" t="s">
-        <v>219</v>
       </c>
       <c r="D77">
         <v>2</v>
       </c>
       <c r="E77" s="2" t="s">
+        <v>218</v>
+      </c>
+      <c r="F77" t="s">
+        <v>101</v>
+      </c>
+      <c r="G77" s="2" t="s">
+        <v>219</v>
+      </c>
+      <c r="H77" s="2" t="s">
         <v>220</v>
       </c>
-      <c r="F77" t="s">
-        <v>101</v>
-      </c>
-      <c r="G77" s="2" t="s">
+    </row>
+    <row r="78" spans="1:8" ht="34" x14ac:dyDescent="0.2">
+      <c r="A78" s="5"/>
+      <c r="B78" t="s">
         <v>221</v>
-      </c>
-      <c r="H77" s="2" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="78" spans="1:8" ht="34" x14ac:dyDescent="0.2">
-      <c r="A78" s="4"/>
-      <c r="B78" t="s">
-        <v>223</v>
       </c>
       <c r="D78">
         <v>8</v>
       </c>
       <c r="E78" s="2" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="F78" t="s">
         <v>101</v>
       </c>
       <c r="G78" s="2" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="H78" s="2" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
     </row>
     <row r="79" spans="1:8" ht="34" x14ac:dyDescent="0.2">
-      <c r="A79" s="4"/>
+      <c r="A79" s="5"/>
       <c r="B79" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="D79" t="s">
         <v>155</v>
@@ -3228,82 +3228,82 @@
         <v>101</v>
       </c>
       <c r="G79" s="2" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="H79" s="2" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
     </row>
     <row r="80" spans="1:8" ht="51" x14ac:dyDescent="0.2">
-      <c r="A80" s="4"/>
+      <c r="A80" s="5"/>
       <c r="B80" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="D80">
         <v>4</v>
       </c>
       <c r="E80" s="2" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="F80" t="s">
         <v>101</v>
       </c>
       <c r="G80" s="2" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="H80" s="2" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
     </row>
     <row r="81" spans="1:8" ht="34" x14ac:dyDescent="0.2">
-      <c r="A81" s="4"/>
+      <c r="A81" s="5"/>
       <c r="B81" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="D81">
         <v>16</v>
       </c>
       <c r="E81" s="2" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="F81" t="s">
         <v>101</v>
       </c>
       <c r="G81" s="2" t="s">
+        <v>228</v>
+      </c>
+      <c r="H81" s="2" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="82" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="A82" s="5" t="s">
+        <v>229</v>
+      </c>
+      <c r="F82" t="s">
+        <v>229</v>
+      </c>
+      <c r="H82" s="2" t="s">
         <v>230</v>
       </c>
-      <c r="H81" s="2" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="82" spans="1:8" ht="17" x14ac:dyDescent="0.2">
-      <c r="A82" s="4" t="s">
-        <v>231</v>
-      </c>
-      <c r="F82" t="s">
-        <v>231</v>
-      </c>
-      <c r="H82" s="2" t="s">
+    </row>
+    <row r="83" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="A83" s="5"/>
+      <c r="B83" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="F83" t="s">
+        <v>229</v>
+      </c>
+      <c r="H83" s="2" t="s">
         <v>232</v>
       </c>
     </row>
-    <row r="83" spans="1:8" ht="17" x14ac:dyDescent="0.2">
-      <c r="A83" s="4"/>
-      <c r="B83" s="4" t="s">
-        <v>101</v>
-      </c>
-      <c r="F83" t="s">
-        <v>231</v>
-      </c>
-      <c r="H83" s="2" t="s">
-        <v>234</v>
-      </c>
-    </row>
     <row r="84" spans="1:8" ht="51" x14ac:dyDescent="0.2">
-      <c r="A84" s="4"/>
-      <c r="B84" s="4"/>
+      <c r="A84" s="5"/>
+      <c r="B84" s="5"/>
       <c r="C84" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="D84" t="s">
         <v>155</v>
@@ -3312,20 +3312,20 @@
         <v>63</v>
       </c>
       <c r="F84" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="G84" s="2" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
       <c r="H84" s="2" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
     </row>
     <row r="85" spans="1:8" ht="51" x14ac:dyDescent="0.2">
-      <c r="A85" s="4"/>
-      <c r="B85" s="4"/>
+      <c r="A85" s="5"/>
+      <c r="B85" s="5"/>
       <c r="C85" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="D85" t="s">
         <v>155</v>
@@ -3334,77 +3334,77 @@
         <v>63</v>
       </c>
       <c r="F85" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="G85" s="2" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="H85" s="2" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
     </row>
     <row r="86" spans="1:8" ht="17" x14ac:dyDescent="0.2">
-      <c r="A86" s="4"/>
-      <c r="B86" s="4"/>
+      <c r="A86" s="5"/>
+      <c r="B86" s="5"/>
       <c r="C86" t="s">
+        <v>239</v>
+      </c>
+      <c r="D86" t="s">
+        <v>393</v>
+      </c>
+      <c r="F86" t="s">
+        <v>229</v>
+      </c>
+      <c r="G86" s="2" t="s">
         <v>241</v>
       </c>
-      <c r="D86" t="s">
-        <v>395</v>
-      </c>
-      <c r="F86" t="s">
-        <v>231</v>
-      </c>
-      <c r="G86" s="2" t="s">
-        <v>243</v>
-      </c>
       <c r="H86" s="2" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="87" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="A87" s="5"/>
+      <c r="B87" s="5"/>
+      <c r="C87" t="s">
+        <v>385</v>
+      </c>
+      <c r="D87" t="s">
+        <v>394</v>
+      </c>
+      <c r="F87" t="s">
+        <v>229</v>
+      </c>
+      <c r="G87" s="2" t="s">
         <v>244</v>
       </c>
     </row>
-    <row r="87" spans="1:8" ht="17" x14ac:dyDescent="0.2">
-      <c r="A87" s="4"/>
-      <c r="B87" s="4"/>
-      <c r="C87" t="s">
-        <v>387</v>
-      </c>
-      <c r="D87" t="s">
-        <v>396</v>
-      </c>
-      <c r="F87" t="s">
-        <v>231</v>
-      </c>
-      <c r="G87" s="2" t="s">
-        <v>246</v>
-      </c>
-    </row>
     <row r="88" spans="1:8" ht="34" x14ac:dyDescent="0.2">
-      <c r="A88" s="4"/>
-      <c r="B88" s="4"/>
+      <c r="A88" s="5"/>
+      <c r="B88" s="5"/>
       <c r="C88" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
       <c r="D88">
         <v>50</v>
       </c>
       <c r="E88" s="2" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="F88" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="G88" s="2" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="H88" s="2" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
     </row>
     <row r="89" spans="1:8" ht="51" x14ac:dyDescent="0.2">
-      <c r="A89" s="4"/>
-      <c r="B89" s="4"/>
+      <c r="A89" s="5"/>
+      <c r="B89" s="5"/>
       <c r="C89" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
       <c r="D89" t="s">
         <v>155</v>
@@ -3413,20 +3413,20 @@
         <v>63</v>
       </c>
       <c r="F89" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="G89" s="2" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
       <c r="H89" s="2" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
     </row>
     <row r="90" spans="1:8" ht="34" x14ac:dyDescent="0.2">
-      <c r="A90" s="4"/>
-      <c r="B90" s="4"/>
+      <c r="A90" s="5"/>
+      <c r="B90" s="5"/>
       <c r="C90" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="D90">
         <v>100</v>
@@ -3435,20 +3435,20 @@
         <v>78</v>
       </c>
       <c r="F90" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="G90" s="2" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="H90" s="2" t="s">
         <v>144</v>
       </c>
     </row>
     <row r="91" spans="1:8" ht="51" x14ac:dyDescent="0.2">
-      <c r="A91" s="4"/>
-      <c r="B91" s="4"/>
+      <c r="A91" s="5"/>
+      <c r="B91" s="5"/>
       <c r="C91" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="D91" t="s">
         <v>155</v>
@@ -3457,51 +3457,51 @@
         <v>63</v>
       </c>
       <c r="F91" t="s">
+        <v>229</v>
+      </c>
+      <c r="G91" s="2" t="s">
+        <v>384</v>
+      </c>
+      <c r="H91" s="2" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="92" spans="1:8" ht="34" x14ac:dyDescent="0.2">
+      <c r="A92" s="5"/>
+      <c r="B92" s="5"/>
+      <c r="C92" t="s">
+        <v>261</v>
+      </c>
+      <c r="D92" t="s">
+        <v>395</v>
+      </c>
+      <c r="F92" t="s">
+        <v>229</v>
+      </c>
+      <c r="G92" s="2" t="s">
+        <v>262</v>
+      </c>
+      <c r="H92" s="2" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="93" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="A93" s="5"/>
+      <c r="B93" s="5" t="s">
         <v>231</v>
       </c>
-      <c r="G91" s="2" t="s">
-        <v>386</v>
-      </c>
-      <c r="H91" s="2" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="92" spans="1:8" ht="34" x14ac:dyDescent="0.2">
-      <c r="A92" s="4"/>
-      <c r="B92" s="4"/>
-      <c r="C92" t="s">
-        <v>263</v>
-      </c>
-      <c r="D92" t="s">
-        <v>397</v>
-      </c>
-      <c r="F92" t="s">
-        <v>231</v>
-      </c>
-      <c r="G92" s="2" t="s">
-        <v>264</v>
-      </c>
-      <c r="H92" s="2" t="s">
-        <v>244</v>
-      </c>
-    </row>
-    <row r="93" spans="1:8" ht="17" x14ac:dyDescent="0.2">
-      <c r="A93" s="4"/>
-      <c r="B93" s="4" t="s">
+      <c r="F93" t="s">
+        <v>229</v>
+      </c>
+      <c r="H93" s="2" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="94" spans="1:8" ht="68" x14ac:dyDescent="0.2">
+      <c r="A94" s="5"/>
+      <c r="B94" s="5"/>
+      <c r="C94" t="s">
         <v>233</v>
-      </c>
-      <c r="F93" t="s">
-        <v>231</v>
-      </c>
-      <c r="H93" s="2" t="s">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="94" spans="1:8" ht="68" x14ac:dyDescent="0.2">
-      <c r="A94" s="4"/>
-      <c r="B94" s="4"/>
-      <c r="C94" t="s">
-        <v>235</v>
       </c>
       <c r="D94" t="s">
         <v>155</v>
@@ -3510,20 +3510,20 @@
         <v>63</v>
       </c>
       <c r="F94" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="G94" s="2" t="s">
+        <v>234</v>
+      </c>
+      <c r="H94" s="2" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="95" spans="1:8" ht="34" x14ac:dyDescent="0.2">
+      <c r="A95" s="5"/>
+      <c r="B95" s="5"/>
+      <c r="C95" t="s">
         <v>236</v>
-      </c>
-      <c r="H94" s="2" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="95" spans="1:8" ht="34" x14ac:dyDescent="0.2">
-      <c r="A95" s="4"/>
-      <c r="B95" s="4"/>
-      <c r="C95" t="s">
-        <v>238</v>
       </c>
       <c r="D95" t="s">
         <v>155</v>
@@ -3532,99 +3532,99 @@
         <v>63</v>
       </c>
       <c r="F95" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="G95" s="2" t="s">
+        <v>237</v>
+      </c>
+      <c r="H95" s="2" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="96" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="A96" s="5"/>
+      <c r="B96" s="5"/>
+      <c r="C96" t="s">
         <v>239</v>
       </c>
-      <c r="H95" s="2" t="s">
+      <c r="D96" t="s">
         <v>240</v>
       </c>
-    </row>
-    <row r="96" spans="1:8" ht="17" x14ac:dyDescent="0.2">
-      <c r="A96" s="4"/>
-      <c r="B96" s="4"/>
-      <c r="C96" t="s">
+      <c r="F96" t="s">
+        <v>229</v>
+      </c>
+      <c r="G96" s="2" t="s">
         <v>241</v>
       </c>
-      <c r="D96" t="s">
+      <c r="H96" s="2" t="s">
         <v>242</v>
       </c>
-      <c r="F96" t="s">
-        <v>231</v>
-      </c>
-      <c r="G96" s="2" t="s">
+    </row>
+    <row r="97" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="A97" s="5"/>
+      <c r="B97" s="5"/>
+      <c r="C97" t="s">
         <v>243</v>
       </c>
-      <c r="H96" s="2" t="s">
+      <c r="D97" t="s">
+        <v>396</v>
+      </c>
+      <c r="F97" t="s">
+        <v>229</v>
+      </c>
+      <c r="G97" s="2" t="s">
         <v>244</v>
       </c>
     </row>
-    <row r="97" spans="1:8" ht="17" x14ac:dyDescent="0.2">
-      <c r="A97" s="4"/>
-      <c r="B97" s="4"/>
-      <c r="C97" t="s">
+    <row r="98" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="A98" s="5"/>
+      <c r="B98" s="5"/>
+      <c r="C98" t="s">
         <v>245</v>
-      </c>
-      <c r="D97" t="s">
-        <v>398</v>
-      </c>
-      <c r="F97" t="s">
-        <v>231</v>
-      </c>
-      <c r="G97" s="2" t="s">
-        <v>246</v>
-      </c>
-    </row>
-    <row r="98" spans="1:8" ht="17" x14ac:dyDescent="0.2">
-      <c r="A98" s="4"/>
-      <c r="B98" s="4"/>
-      <c r="C98" t="s">
-        <v>247</v>
       </c>
       <c r="D98">
         <v>60</v>
       </c>
       <c r="E98" s="2" t="s">
+        <v>246</v>
+      </c>
+      <c r="F98" t="s">
+        <v>229</v>
+      </c>
+      <c r="G98" s="2" t="s">
+        <v>247</v>
+      </c>
+      <c r="H98" s="2" t="s">
         <v>248</v>
       </c>
-      <c r="F98" t="s">
-        <v>231</v>
-      </c>
-      <c r="G98" s="2" t="s">
+    </row>
+    <row r="99" spans="1:8" ht="51" x14ac:dyDescent="0.2">
+      <c r="A99" s="5"/>
+      <c r="B99" s="5"/>
+      <c r="C99" t="s">
         <v>249</v>
       </c>
-      <c r="H98" s="2" t="s">
+      <c r="D99" t="s">
         <v>250</v>
       </c>
-    </row>
-    <row r="99" spans="1:8" ht="51" x14ac:dyDescent="0.2">
-      <c r="A99" s="4"/>
-      <c r="B99" s="4"/>
-      <c r="C99" t="s">
+      <c r="E99" s="2" t="s">
         <v>251</v>
       </c>
-      <c r="D99" t="s">
+      <c r="F99" t="s">
+        <v>229</v>
+      </c>
+      <c r="G99" s="2" t="s">
         <v>252</v>
       </c>
-      <c r="E99" s="2" t="s">
+      <c r="H99" s="2" t="s">
         <v>253</v>
       </c>
-      <c r="F99" t="s">
-        <v>231</v>
-      </c>
-      <c r="G99" s="2" t="s">
+    </row>
+    <row r="100" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="A100" s="5"/>
+      <c r="B100" s="5"/>
+      <c r="C100" t="s">
         <v>254</v>
-      </c>
-      <c r="H99" s="2" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="100" spans="1:8" ht="17" x14ac:dyDescent="0.2">
-      <c r="A100" s="4"/>
-      <c r="B100" s="4"/>
-      <c r="C100" t="s">
-        <v>256</v>
       </c>
       <c r="D100">
         <v>100</v>
@@ -3633,17 +3633,17 @@
         <v>78</v>
       </c>
       <c r="F100" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="G100" s="2" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
     </row>
     <row r="101" spans="1:8" ht="17" x14ac:dyDescent="0.2">
-      <c r="A101" s="4"/>
-      <c r="B101" s="4"/>
+      <c r="A101" s="5"/>
+      <c r="B101" s="5"/>
       <c r="C101" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="D101">
         <v>100</v>
@@ -3652,20 +3652,20 @@
         <v>78</v>
       </c>
       <c r="F101" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="G101" s="2" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="H101" s="2" t="s">
         <v>144</v>
       </c>
     </row>
     <row r="102" spans="1:8" ht="51" x14ac:dyDescent="0.2">
-      <c r="A102" s="4"/>
-      <c r="B102" s="4"/>
+      <c r="A102" s="5"/>
+      <c r="B102" s="5"/>
       <c r="C102" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="D102" t="s">
         <v>155</v>
@@ -3674,51 +3674,51 @@
         <v>63</v>
       </c>
       <c r="F102" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="G102" s="2" t="s">
+        <v>259</v>
+      </c>
+      <c r="H102" s="2" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="103" spans="1:8" ht="34" x14ac:dyDescent="0.2">
+      <c r="A103" s="5"/>
+      <c r="B103" s="5"/>
+      <c r="C103" t="s">
         <v>261</v>
       </c>
-      <c r="H102" s="2" t="s">
+      <c r="D103" t="s">
+        <v>395</v>
+      </c>
+      <c r="F103" t="s">
+        <v>229</v>
+      </c>
+      <c r="G103" s="2" t="s">
         <v>262</v>
       </c>
-    </row>
-    <row r="103" spans="1:8" ht="34" x14ac:dyDescent="0.2">
-      <c r="A103" s="4"/>
-      <c r="B103" s="4"/>
-      <c r="C103" t="s">
+      <c r="H103" s="2" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="104" spans="1:8" ht="34" x14ac:dyDescent="0.2">
+      <c r="A104" s="5"/>
+      <c r="B104" s="5" t="s">
         <v>263</v>
       </c>
-      <c r="D103" t="s">
-        <v>397</v>
-      </c>
-      <c r="F103" t="s">
-        <v>231</v>
-      </c>
-      <c r="G103" s="2" t="s">
+      <c r="F104" t="s">
+        <v>229</v>
+      </c>
+      <c r="H104" s="2" t="s">
         <v>264</v>
       </c>
-      <c r="H103" s="2" t="s">
-        <v>244</v>
-      </c>
-    </row>
-    <row r="104" spans="1:8" ht="34" x14ac:dyDescent="0.2">
-      <c r="A104" s="4"/>
-      <c r="B104" s="4" t="s">
-        <v>265</v>
-      </c>
-      <c r="F104" t="s">
-        <v>231</v>
-      </c>
-      <c r="H104" s="2" t="s">
-        <v>266</v>
-      </c>
     </row>
     <row r="105" spans="1:8" ht="68" x14ac:dyDescent="0.2">
-      <c r="A105" s="4"/>
-      <c r="B105" s="4"/>
+      <c r="A105" s="5"/>
+      <c r="B105" s="5"/>
       <c r="C105" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="D105" t="s">
         <v>62</v>
@@ -3727,20 +3727,20 @@
         <v>63</v>
       </c>
       <c r="F105" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="G105" s="2" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="H105" s="2" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
     </row>
     <row r="106" spans="1:8" ht="34" x14ac:dyDescent="0.2">
-      <c r="A106" s="4"/>
-      <c r="B106" s="4"/>
+      <c r="A106" s="5"/>
+      <c r="B106" s="5"/>
       <c r="C106" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="D106" t="s">
         <v>155</v>
@@ -3749,84 +3749,84 @@
         <v>63</v>
       </c>
       <c r="F106" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="G106" s="2" t="s">
+        <v>267</v>
+      </c>
+      <c r="H106" s="2" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="107" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="A107" s="5"/>
+      <c r="B107" s="5"/>
+      <c r="C107" t="s">
+        <v>239</v>
+      </c>
+      <c r="D107" t="s">
+        <v>398</v>
+      </c>
+      <c r="F107" t="s">
+        <v>229</v>
+      </c>
+      <c r="G107" s="2" t="s">
+        <v>241</v>
+      </c>
+      <c r="H107" s="2" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="108" spans="1:8" ht="34" x14ac:dyDescent="0.2">
+      <c r="A108" s="5"/>
+      <c r="B108" s="5"/>
+      <c r="C108" t="s">
+        <v>243</v>
+      </c>
+      <c r="D108" t="s">
+        <v>392</v>
+      </c>
+      <c r="F108" t="s">
+        <v>229</v>
+      </c>
+      <c r="G108" s="2" t="s">
         <v>269</v>
       </c>
-      <c r="H106" s="2" t="s">
+      <c r="H108" s="2" t="s">
         <v>270</v>
       </c>
     </row>
-    <row r="107" spans="1:8" ht="17" x14ac:dyDescent="0.2">
-      <c r="A107" s="4"/>
-      <c r="B107" s="4"/>
-      <c r="C107" t="s">
-        <v>241</v>
-      </c>
-      <c r="D107" t="s">
-        <v>400</v>
-      </c>
-      <c r="F107" t="s">
-        <v>231</v>
-      </c>
-      <c r="G107" s="2" t="s">
-        <v>243</v>
-      </c>
-      <c r="H107" s="2" t="s">
-        <v>244</v>
-      </c>
-    </row>
-    <row r="108" spans="1:8" ht="34" x14ac:dyDescent="0.2">
-      <c r="A108" s="4"/>
-      <c r="B108" s="4"/>
-      <c r="C108" t="s">
-        <v>245</v>
-      </c>
-      <c r="D108" t="s">
-        <v>394</v>
-      </c>
-      <c r="F108" t="s">
-        <v>231</v>
-      </c>
-      <c r="G108" s="2" t="s">
+    <row r="109" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="A109" s="5"/>
+      <c r="B109" s="5"/>
+      <c r="C109" t="s">
         <v>271</v>
-      </c>
-      <c r="H108" s="2" t="s">
-        <v>272</v>
-      </c>
-    </row>
-    <row r="109" spans="1:8" ht="17" x14ac:dyDescent="0.2">
-      <c r="A109" s="4"/>
-      <c r="B109" s="4"/>
-      <c r="C109" t="s">
-        <v>273</v>
       </c>
       <c r="D109">
         <v>60</v>
       </c>
       <c r="E109" s="2" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="F109" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="G109" s="2" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
     </row>
     <row r="110" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A110" s="4" t="s">
-        <v>275</v>
+      <c r="A110" s="5" t="s">
+        <v>273</v>
       </c>
       <c r="F110" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
     </row>
     <row r="111" spans="1:8" ht="17" x14ac:dyDescent="0.2">
-      <c r="A111" s="4"/>
+      <c r="A111" s="5"/>
       <c r="B111" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="C111" t="b">
         <v>0</v>
@@ -3835,111 +3835,111 @@
         <v>63</v>
       </c>
       <c r="F111" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="G111" s="2" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="112" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="A112" s="5"/>
+      <c r="B112" t="s">
+        <v>239</v>
+      </c>
+      <c r="C112" t="s">
+        <v>397</v>
+      </c>
+      <c r="F112" t="s">
+        <v>229</v>
+      </c>
+      <c r="G112" s="2" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="113" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="A113" s="5"/>
+      <c r="B113" t="s">
+        <v>243</v>
+      </c>
+      <c r="C113" t="s">
         <v>276</v>
       </c>
-    </row>
-    <row r="112" spans="1:8" ht="17" x14ac:dyDescent="0.2">
-      <c r="A112" s="4"/>
-      <c r="B112" t="s">
-        <v>241</v>
-      </c>
-      <c r="C112" t="s">
-        <v>399</v>
-      </c>
-      <c r="F112" t="s">
-        <v>231</v>
-      </c>
-      <c r="G112" s="2" t="s">
+      <c r="F113" t="s">
+        <v>229</v>
+      </c>
+      <c r="G113" s="2" t="s">
         <v>277</v>
       </c>
     </row>
-    <row r="113" spans="1:8" ht="17" x14ac:dyDescent="0.2">
-      <c r="A113" s="4"/>
-      <c r="B113" t="s">
-        <v>245</v>
-      </c>
-      <c r="C113" t="s">
+    <row r="114" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="A114" s="5"/>
+      <c r="B114" t="s">
         <v>278</v>
-      </c>
-      <c r="F113" t="s">
-        <v>231</v>
-      </c>
-      <c r="G113" s="2" t="s">
-        <v>279</v>
-      </c>
-    </row>
-    <row r="114" spans="1:8" ht="17" x14ac:dyDescent="0.2">
-      <c r="A114" s="4"/>
-      <c r="B114" t="s">
-        <v>280</v>
       </c>
       <c r="C114">
         <v>0.01</v>
       </c>
       <c r="F114" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="G114" s="2" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="115" spans="1:8" ht="34" x14ac:dyDescent="0.2">
+      <c r="A115" s="5"/>
+      <c r="B115" t="s">
+        <v>280</v>
+      </c>
+      <c r="C115" t="s">
         <v>281</v>
       </c>
-    </row>
-    <row r="115" spans="1:8" ht="34" x14ac:dyDescent="0.2">
-      <c r="A115" s="4"/>
-      <c r="B115" t="s">
+      <c r="E115" s="2" t="s">
         <v>282</v>
       </c>
-      <c r="C115" t="s">
+      <c r="F115" t="s">
+        <v>229</v>
+      </c>
+      <c r="G115" s="2" t="s">
         <v>283</v>
       </c>
-      <c r="E115" s="2" t="s">
+      <c r="H115" s="2" t="s">
         <v>284</v>
       </c>
-      <c r="F115" t="s">
-        <v>231</v>
-      </c>
-      <c r="G115" s="2" t="s">
+    </row>
+    <row r="116" spans="1:8" ht="34" x14ac:dyDescent="0.2">
+      <c r="A116" s="5"/>
+      <c r="B116" t="s">
         <v>285</v>
-      </c>
-      <c r="H115" s="2" t="s">
-        <v>286</v>
-      </c>
-    </row>
-    <row r="116" spans="1:8" ht="34" x14ac:dyDescent="0.2">
-      <c r="A116" s="4"/>
-      <c r="B116" t="s">
-        <v>287</v>
       </c>
       <c r="C116" t="b">
         <v>0</v>
       </c>
       <c r="F116" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="G116" s="2" t="s">
+        <v>286</v>
+      </c>
+      <c r="H116" s="2" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="117" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="A117" s="5" t="s">
         <v>288</v>
       </c>
-      <c r="H116" s="2" t="s">
+      <c r="F117" t="s">
+        <v>229</v>
+      </c>
+      <c r="H117" s="2" t="s">
         <v>289</v>
       </c>
     </row>
-    <row r="117" spans="1:8" ht="17" x14ac:dyDescent="0.2">
-      <c r="A117" s="4" t="s">
+    <row r="118" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="A118" s="5"/>
+      <c r="B118" t="s">
         <v>290</v>
-      </c>
-      <c r="F117" t="s">
-        <v>231</v>
-      </c>
-      <c r="H117" s="2" t="s">
-        <v>291</v>
-      </c>
-    </row>
-    <row r="118" spans="1:8" ht="17" x14ac:dyDescent="0.2">
-      <c r="A118" s="4"/>
-      <c r="B118" t="s">
-        <v>292</v>
       </c>
       <c r="D118" t="s">
         <v>155</v>
@@ -3948,19 +3948,19 @@
         <v>63</v>
       </c>
       <c r="F118" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="G118" s="2" t="s">
+        <v>291</v>
+      </c>
+      <c r="H118" s="2" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="119" spans="1:8" ht="34" x14ac:dyDescent="0.2">
+      <c r="A119" s="5"/>
+      <c r="B119" t="s">
         <v>293</v>
-      </c>
-      <c r="H118" s="2" t="s">
-        <v>294</v>
-      </c>
-    </row>
-    <row r="119" spans="1:8" ht="34" x14ac:dyDescent="0.2">
-      <c r="A119" s="4"/>
-      <c r="B119" t="s">
-        <v>295</v>
       </c>
       <c r="D119">
         <v>1</v>
@@ -3969,37 +3969,37 @@
         <v>43922</v>
       </c>
       <c r="F119" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="G119" s="2" t="s">
+        <v>294</v>
+      </c>
+      <c r="H119" s="2" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="120" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="A120" s="5"/>
+      <c r="B120" t="s">
         <v>296</v>
       </c>
-      <c r="H119" s="2" t="s">
+      <c r="D120" t="s">
         <v>297</v>
       </c>
-    </row>
-    <row r="120" spans="1:8" ht="17" x14ac:dyDescent="0.2">
-      <c r="A120" s="4"/>
-      <c r="B120" t="s">
+      <c r="E120" s="2" t="s">
         <v>298</v>
       </c>
-      <c r="D120" t="s">
+      <c r="F120" t="s">
+        <v>229</v>
+      </c>
+      <c r="G120" s="2" t="s">
         <v>299</v>
       </c>
-      <c r="E120" s="2" t="s">
+    </row>
+    <row r="121" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="A121" s="5"/>
+      <c r="B121" t="s">
         <v>300</v>
-      </c>
-      <c r="F120" t="s">
-        <v>231</v>
-      </c>
-      <c r="G120" s="2" t="s">
-        <v>301</v>
-      </c>
-    </row>
-    <row r="121" spans="1:8" ht="17" x14ac:dyDescent="0.2">
-      <c r="A121" s="4"/>
-      <c r="B121" t="s">
-        <v>302</v>
       </c>
       <c r="D121" s="1">
         <v>1.0000000000000001E-5</v>
@@ -4008,302 +4008,312 @@
         <v>86</v>
       </c>
       <c r="F121" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="G121" s="2" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="122" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="A122" s="5" t="s">
+        <v>302</v>
+      </c>
+      <c r="F122" t="s">
         <v>303</v>
       </c>
-    </row>
-    <row r="122" spans="1:8" ht="17" x14ac:dyDescent="0.2">
-      <c r="A122" s="4" t="s">
+      <c r="H122" s="2" t="s">
         <v>304</v>
       </c>
-      <c r="F122" t="s">
+    </row>
+    <row r="123" spans="1:8" ht="34" x14ac:dyDescent="0.2">
+      <c r="A123" s="5"/>
+      <c r="B123" t="s">
         <v>305</v>
       </c>
-      <c r="H122" s="2" t="s">
-        <v>306</v>
-      </c>
-    </row>
-    <row r="123" spans="1:8" ht="34" x14ac:dyDescent="0.2">
-      <c r="A123" s="4"/>
-      <c r="B123" t="s">
-        <v>307</v>
-      </c>
-      <c r="D123" s="6" t="s">
-        <v>393</v>
+      <c r="D123" s="4" t="s">
+        <v>391</v>
       </c>
       <c r="E123" s="2" t="s">
         <v>63</v>
       </c>
       <c r="F123" t="s">
+        <v>306</v>
+      </c>
+      <c r="G123" s="2" t="s">
+        <v>307</v>
+      </c>
+      <c r="H123" s="2" t="s">
         <v>308</v>
       </c>
-      <c r="G123" s="2" t="s">
+    </row>
+    <row r="124" spans="1:8" ht="51" x14ac:dyDescent="0.2">
+      <c r="A124" s="5"/>
+      <c r="B124" t="s">
         <v>309</v>
       </c>
-      <c r="H123" s="2" t="s">
-        <v>310</v>
-      </c>
-    </row>
-    <row r="124" spans="1:8" ht="51" x14ac:dyDescent="0.2">
-      <c r="A124" s="4"/>
-      <c r="B124" t="s">
-        <v>311</v>
-      </c>
-      <c r="D124" s="6" t="s">
-        <v>366</v>
+      <c r="D124" s="4" t="s">
+        <v>364</v>
       </c>
       <c r="E124" s="2" t="s">
         <v>63</v>
       </c>
       <c r="F124" t="s">
+        <v>310</v>
+      </c>
+      <c r="G124" s="2" t="s">
+        <v>311</v>
+      </c>
+      <c r="H124" s="2" t="s">
         <v>312</v>
       </c>
-      <c r="G124" s="2" t="s">
+    </row>
+    <row r="125" spans="1:8" ht="34" x14ac:dyDescent="0.2">
+      <c r="A125" s="5" t="s">
         <v>313</v>
       </c>
-      <c r="H124" s="2" t="s">
+      <c r="F125" t="s">
         <v>314</v>
       </c>
-    </row>
-    <row r="125" spans="1:8" ht="34" x14ac:dyDescent="0.2">
-      <c r="A125" s="4" t="s">
+      <c r="H125" s="2" t="s">
         <v>315</v>
       </c>
-      <c r="F125" t="s">
+    </row>
+    <row r="126" spans="1:8" ht="51" x14ac:dyDescent="0.2">
+      <c r="A126" s="5"/>
+      <c r="B126" t="s">
         <v>316</v>
       </c>
-      <c r="H125" s="2" t="s">
-        <v>317</v>
-      </c>
-    </row>
-    <row r="126" spans="1:8" ht="51" x14ac:dyDescent="0.2">
-      <c r="A126" s="4"/>
-      <c r="B126" t="s">
-        <v>318</v>
-      </c>
-      <c r="D126" s="6" t="s">
-        <v>393</v>
+      <c r="D126" s="4" t="s">
+        <v>391</v>
       </c>
       <c r="E126" s="2" t="s">
         <v>63</v>
       </c>
       <c r="F126" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="G126" s="2" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="127" spans="1:8" ht="51" x14ac:dyDescent="0.2">
+      <c r="A127" s="5"/>
+      <c r="B127" t="s">
+        <v>353</v>
+      </c>
+      <c r="D127" t="s">
+        <v>318</v>
+      </c>
+      <c r="E127" s="2" t="s">
         <v>319</v>
       </c>
-    </row>
-    <row r="127" spans="1:8" ht="51" x14ac:dyDescent="0.2">
-      <c r="A127" s="4"/>
-      <c r="B127" t="s">
-        <v>355</v>
-      </c>
-      <c r="D127" t="s">
+      <c r="F127" t="s">
+        <v>314</v>
+      </c>
+      <c r="G127" s="2" t="s">
         <v>320</v>
       </c>
-      <c r="E127" s="2" t="s">
+      <c r="H127" s="2" t="s">
         <v>321</v>
       </c>
-      <c r="F127" t="s">
-        <v>316</v>
-      </c>
-      <c r="G127" s="2" t="s">
+    </row>
+    <row r="128" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="A128" s="5"/>
+      <c r="B128" t="s">
         <v>322</v>
-      </c>
-      <c r="H127" s="2" t="s">
-        <v>323</v>
-      </c>
-    </row>
-    <row r="128" spans="1:8" ht="17" x14ac:dyDescent="0.2">
-      <c r="A128" s="4"/>
-      <c r="B128" t="s">
-        <v>324</v>
       </c>
       <c r="D128">
         <v>1</v>
       </c>
       <c r="F128" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="G128" s="2" t="s">
+        <v>323</v>
+      </c>
+      <c r="H128" s="2" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="129" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="A129" s="5"/>
+      <c r="B129" t="s">
         <v>325</v>
-      </c>
-      <c r="H128" s="2" t="s">
-        <v>326</v>
-      </c>
-    </row>
-    <row r="129" spans="1:8" ht="17" x14ac:dyDescent="0.2">
-      <c r="A129" s="4"/>
-      <c r="B129" t="s">
-        <v>327</v>
       </c>
       <c r="D129">
         <v>10000</v>
       </c>
       <c r="F129" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="G129" s="2" t="s">
+        <v>326</v>
+      </c>
+      <c r="H129" s="2" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="130" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="A130" s="5" t="s">
+        <v>314</v>
+      </c>
+      <c r="F130" t="s">
+        <v>314</v>
+      </c>
+      <c r="H130" s="2" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="131" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="A131" s="5"/>
+      <c r="B131" s="5" t="s">
         <v>328</v>
       </c>
-      <c r="H129" s="2" t="s">
-        <v>326</v>
-      </c>
-    </row>
-    <row r="130" spans="1:8" ht="17" x14ac:dyDescent="0.2">
-      <c r="A130" s="4" t="s">
-        <v>316</v>
-      </c>
-      <c r="F130" t="s">
-        <v>316</v>
-      </c>
-      <c r="H130" s="2" t="s">
+      <c r="F131" t="s">
+        <v>314</v>
+      </c>
+      <c r="H131" s="2" t="s">
         <v>329</v>
       </c>
     </row>
-    <row r="131" spans="1:8" ht="17" x14ac:dyDescent="0.2">
-      <c r="A131" s="4"/>
-      <c r="B131" s="4" t="s">
-        <v>330</v>
-      </c>
-      <c r="F131" t="s">
-        <v>316</v>
-      </c>
-      <c r="H131" s="2" t="s">
-        <v>331</v>
-      </c>
-    </row>
     <row r="132" spans="1:8" ht="17" x14ac:dyDescent="0.2">
-      <c r="A132" s="4"/>
-      <c r="B132" s="4"/>
+      <c r="A132" s="5"/>
+      <c r="B132" s="5"/>
       <c r="C132" t="s">
-        <v>235</v>
-      </c>
-      <c r="D132" s="6" t="s">
-        <v>366</v>
+        <v>233</v>
+      </c>
+      <c r="D132" s="4" t="s">
+        <v>364</v>
       </c>
       <c r="E132" s="2" t="s">
         <v>63</v>
       </c>
       <c r="F132" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="G132" s="2" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="133" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="A133" s="5"/>
+      <c r="B133" s="5"/>
+      <c r="C133" t="s">
+        <v>331</v>
+      </c>
+      <c r="D133" t="s">
+        <v>399</v>
+      </c>
+      <c r="F133" t="s">
+        <v>314</v>
+      </c>
+      <c r="G133" s="2" t="s">
         <v>332</v>
       </c>
-    </row>
-    <row r="133" spans="1:8" ht="17" x14ac:dyDescent="0.2">
-      <c r="A133" s="4"/>
-      <c r="B133" s="4"/>
-      <c r="C133" t="s">
+      <c r="H133" s="2" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="134" spans="1:8" ht="34" x14ac:dyDescent="0.2">
+      <c r="A134" s="5"/>
+      <c r="B134" s="5"/>
+      <c r="C134" t="s">
         <v>333</v>
       </c>
-      <c r="D133" t="s">
-        <v>401</v>
-      </c>
-      <c r="F133" t="s">
-        <v>316</v>
-      </c>
-      <c r="G133" s="2" t="s">
+      <c r="D134" t="s">
         <v>334</v>
       </c>
-      <c r="H133" s="2" t="s">
-        <v>244</v>
-      </c>
-    </row>
-    <row r="134" spans="1:8" ht="34" x14ac:dyDescent="0.2">
-      <c r="A134" s="4"/>
-      <c r="B134" s="4"/>
-      <c r="C134" t="s">
+      <c r="E134" s="2" t="s">
         <v>335</v>
       </c>
-      <c r="D134" t="s">
+      <c r="F134" t="s">
+        <v>314</v>
+      </c>
+      <c r="G134" s="2" t="s">
         <v>336</v>
       </c>
-      <c r="E134" s="2" t="s">
+      <c r="H134" s="2" t="s">
         <v>337</v>
       </c>
-      <c r="F134" t="s">
-        <v>316</v>
-      </c>
-      <c r="G134" s="2" t="s">
+    </row>
+    <row r="135" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="A135" s="5"/>
+      <c r="B135" s="5" t="s">
         <v>338</v>
-      </c>
-      <c r="H134" s="2" t="s">
-        <v>339</v>
-      </c>
-    </row>
-    <row r="135" spans="1:8" ht="17" x14ac:dyDescent="0.2">
-      <c r="A135" s="4"/>
-      <c r="B135" s="4" t="s">
-        <v>340</v>
       </c>
       <c r="E135" s="2" t="s">
         <v>63</v>
       </c>
       <c r="F135" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
     </row>
     <row r="136" spans="1:8" ht="17" x14ac:dyDescent="0.2">
-      <c r="A136" s="4"/>
-      <c r="B136" s="4"/>
+      <c r="A136" s="5"/>
+      <c r="B136" s="5"/>
       <c r="C136" t="s">
-        <v>235</v>
-      </c>
-      <c r="D136" s="6" t="s">
-        <v>393</v>
+        <v>233</v>
+      </c>
+      <c r="D136" s="4" t="s">
+        <v>391</v>
       </c>
       <c r="F136" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="G136" s="2" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="137" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="A137" s="5"/>
+      <c r="B137" s="5"/>
+      <c r="C137" t="s">
+        <v>340</v>
+      </c>
+      <c r="D137" t="s">
+        <v>281</v>
+      </c>
+      <c r="F137" t="s">
+        <v>314</v>
+      </c>
+      <c r="G137" s="2" t="s">
         <v>341</v>
       </c>
-    </row>
-    <row r="137" spans="1:8" ht="17" x14ac:dyDescent="0.2">
-      <c r="A137" s="4"/>
-      <c r="B137" s="4"/>
-      <c r="C137" t="s">
+      <c r="H137" s="2" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="138" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="A138" s="5"/>
+      <c r="B138" t="s">
         <v>342</v>
       </c>
-      <c r="D137" t="s">
-        <v>283</v>
-      </c>
-      <c r="F137" t="s">
-        <v>316</v>
-      </c>
-      <c r="G137" s="2" t="s">
-        <v>343</v>
-      </c>
-      <c r="H137" s="2" t="s">
-        <v>244</v>
-      </c>
-    </row>
-    <row r="138" spans="1:8" ht="17" x14ac:dyDescent="0.2">
-      <c r="A138" s="4"/>
-      <c r="B138" t="s">
-        <v>344</v>
-      </c>
-      <c r="D138" s="6" t="s">
-        <v>393</v>
+      <c r="D138" s="4" t="s">
+        <v>391</v>
       </c>
       <c r="E138" s="2" t="s">
         <v>63</v>
       </c>
       <c r="F138" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="G138" s="2" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
     </row>
   </sheetData>
   <autoFilter ref="A1:H138" xr:uid="{65E3A469-1B8A-364D-8D4D-FD3FF55840DE}"/>
   <mergeCells count="24">
+    <mergeCell ref="A18:A24"/>
+    <mergeCell ref="B19:B21"/>
+    <mergeCell ref="B22:B24"/>
+    <mergeCell ref="A27:A33"/>
+    <mergeCell ref="A34:A50"/>
+    <mergeCell ref="B35:B37"/>
+    <mergeCell ref="B39:B41"/>
+    <mergeCell ref="B42:B44"/>
+    <mergeCell ref="B45:B47"/>
+    <mergeCell ref="B48:B50"/>
     <mergeCell ref="B131:B134"/>
     <mergeCell ref="B135:B137"/>
     <mergeCell ref="A53:A68"/>
@@ -4318,16 +4328,6 @@
     <mergeCell ref="A125:A129"/>
     <mergeCell ref="A130:A138"/>
     <mergeCell ref="B83:B92"/>
-    <mergeCell ref="A18:A24"/>
-    <mergeCell ref="B19:B21"/>
-    <mergeCell ref="B22:B24"/>
-    <mergeCell ref="A27:A33"/>
-    <mergeCell ref="A34:A50"/>
-    <mergeCell ref="B35:B37"/>
-    <mergeCell ref="B39:B41"/>
-    <mergeCell ref="B42:B44"/>
-    <mergeCell ref="B45:B47"/>
-    <mergeCell ref="B48:B50"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
add more config documentation
</commit_message>
<xml_diff>
--- a/documentation/config_explained.xlsx
+++ b/documentation/config_explained.xlsx
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/heintzbu/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FEF5B618-9919-AA4F-AAAA-CD4A0E936B19}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{B42F5B3E-750E-3345-9AD7-37C1E53259F1}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="32380" yWindow="800" windowWidth="31000" windowHeight="20240" xr2:uid="{F207B228-D75F-344A-ADB6-4CA41A47821F}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="config_explained" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$H$149</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">config_explained!$A$1:$H$153</definedName>
   </definedNames>
   <calcPr calcId="181029"/>
   <extLst>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="755" uniqueCount="416">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="774" uniqueCount="423">
   <si>
     <t xml:space="preserve">email </t>
   </si>
@@ -1276,6 +1276,27 @@
   </si>
   <si>
     <t xml:space="preserve">  fungalTraits</t>
+  </si>
+  <si>
+    <t>rm_phix</t>
+  </si>
+  <si>
+    <t>remove phiX</t>
+  </si>
+  <si>
+    <t>trim_left</t>
+  </si>
+  <si>
+    <t xml:space="preserve">this many bases will be cut from the 5' end of fwd reads </t>
+  </si>
+  <si>
+    <t xml:space="preserve">this many bases will be cut from the 5' end of rvs reads </t>
+  </si>
+  <si>
+    <t>filtered reads will have length truncLen-trimLeft</t>
+  </si>
+  <si>
+    <t>useful with Illumina sequencing</t>
   </si>
 </sst>
 </file>
@@ -1311,7 +1332,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1325,8 +1346,12 @@
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1641,10 +1666,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{61B259DD-FAC6-FB4A-84F8-11B4141970E7}">
-  <dimension ref="A1:H149"/>
+  <dimension ref="A1:H153"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A120" workbookViewId="0">
-      <selection activeCell="B142" sqref="B142:B145"/>
+    <sheetView tabSelected="1" topLeftCell="A41" workbookViewId="0">
+      <selection activeCell="H54" sqref="H54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2057,7 +2082,7 @@
       </c>
     </row>
     <row r="18" spans="1:8" ht="17" x14ac:dyDescent="0.2">
-      <c r="A18" s="5" t="s">
+      <c r="A18" s="6" t="s">
         <v>36</v>
       </c>
       <c r="B18" t="s">
@@ -2083,8 +2108,8 @@
       </c>
     </row>
     <row r="19" spans="1:8" ht="17" x14ac:dyDescent="0.2">
-      <c r="A19" s="5"/>
-      <c r="B19" s="6" t="s">
+      <c r="A19" s="6"/>
+      <c r="B19" s="7" t="s">
         <v>39</v>
       </c>
       <c r="C19" t="s">
@@ -2107,8 +2132,8 @@
       </c>
     </row>
     <row r="20" spans="1:8" ht="17" x14ac:dyDescent="0.2">
-      <c r="A20" s="5"/>
-      <c r="B20" s="6"/>
+      <c r="A20" s="6"/>
+      <c r="B20" s="7"/>
       <c r="C20" t="s">
         <v>41</v>
       </c>
@@ -2126,8 +2151,8 @@
       </c>
     </row>
     <row r="21" spans="1:8" ht="17" x14ac:dyDescent="0.2">
-      <c r="A21" s="5"/>
-      <c r="B21" s="6"/>
+      <c r="A21" s="6"/>
+      <c r="B21" s="7"/>
       <c r="C21" t="s">
         <v>45</v>
       </c>
@@ -2148,8 +2173,8 @@
       </c>
     </row>
     <row r="22" spans="1:8" ht="17" x14ac:dyDescent="0.2">
-      <c r="A22" s="5"/>
-      <c r="B22" s="5" t="s">
+      <c r="A22" s="6"/>
+      <c r="B22" s="6" t="s">
         <v>50</v>
       </c>
       <c r="C22" t="s">
@@ -2172,8 +2197,8 @@
       </c>
     </row>
     <row r="23" spans="1:8" ht="17" x14ac:dyDescent="0.2">
-      <c r="A23" s="5"/>
-      <c r="B23" s="5"/>
+      <c r="A23" s="6"/>
+      <c r="B23" s="6"/>
       <c r="C23" t="s">
         <v>52</v>
       </c>
@@ -2191,8 +2216,8 @@
       </c>
     </row>
     <row r="24" spans="1:8" ht="17" x14ac:dyDescent="0.2">
-      <c r="A24" s="5"/>
-      <c r="B24" s="5"/>
+      <c r="A24" s="6"/>
+      <c r="B24" s="6"/>
       <c r="C24" t="s">
         <v>57</v>
       </c>
@@ -2253,7 +2278,7 @@
       </c>
     </row>
     <row r="27" spans="1:8" ht="17" x14ac:dyDescent="0.2">
-      <c r="A27" s="5" t="s">
+      <c r="A27" s="6" t="s">
         <v>72</v>
       </c>
       <c r="F27" t="s">
@@ -2264,7 +2289,7 @@
       </c>
     </row>
     <row r="28" spans="1:8" ht="17" x14ac:dyDescent="0.2">
-      <c r="A28" s="5"/>
+      <c r="A28" s="6"/>
       <c r="B28" t="s">
         <v>74</v>
       </c>
@@ -2282,7 +2307,7 @@
       </c>
     </row>
     <row r="29" spans="1:8" ht="34" x14ac:dyDescent="0.2">
-      <c r="A29" s="5"/>
+      <c r="A29" s="6"/>
       <c r="B29" t="s">
         <v>77</v>
       </c>
@@ -2300,7 +2325,7 @@
       </c>
     </row>
     <row r="30" spans="1:8" ht="34" x14ac:dyDescent="0.2">
-      <c r="A30" s="5"/>
+      <c r="A30" s="6"/>
       <c r="B30" t="s">
         <v>80</v>
       </c>
@@ -2321,7 +2346,7 @@
       </c>
     </row>
     <row r="31" spans="1:8" ht="17" x14ac:dyDescent="0.2">
-      <c r="A31" s="5"/>
+      <c r="A31" s="6"/>
       <c r="B31" t="s">
         <v>85</v>
       </c>
@@ -2342,7 +2367,7 @@
       </c>
     </row>
     <row r="32" spans="1:8" ht="34" x14ac:dyDescent="0.2">
-      <c r="A32" s="5"/>
+      <c r="A32" s="6"/>
       <c r="B32" t="s">
         <v>89</v>
       </c>
@@ -2360,7 +2385,7 @@
       </c>
     </row>
     <row r="33" spans="1:8" ht="34" x14ac:dyDescent="0.2">
-      <c r="A33" s="5"/>
+      <c r="A33" s="6"/>
       <c r="B33" t="s">
         <v>93</v>
       </c>
@@ -2381,7 +2406,7 @@
       </c>
     </row>
     <row r="34" spans="1:8" ht="102" x14ac:dyDescent="0.2">
-      <c r="A34" s="5" t="s">
+      <c r="A34" s="6" t="s">
         <v>97</v>
       </c>
       <c r="B34" t="s">
@@ -2407,8 +2432,8 @@
       </c>
     </row>
     <row r="35" spans="1:8" ht="17" x14ac:dyDescent="0.2">
-      <c r="A35" s="5"/>
-      <c r="B35" s="5" t="s">
+      <c r="A35" s="6"/>
+      <c r="B35" s="6" t="s">
         <v>100</v>
       </c>
       <c r="F35" t="s">
@@ -2419,8 +2444,8 @@
       </c>
     </row>
     <row r="36" spans="1:8" ht="34" x14ac:dyDescent="0.2">
-      <c r="A36" s="5"/>
-      <c r="B36" s="5"/>
+      <c r="A36" s="6"/>
+      <c r="B36" s="6"/>
       <c r="C36" t="s">
         <v>103</v>
       </c>
@@ -2441,8 +2466,8 @@
       </c>
     </row>
     <row r="37" spans="1:8" ht="51" x14ac:dyDescent="0.2">
-      <c r="A37" s="5"/>
-      <c r="B37" s="5"/>
+      <c r="A37" s="6"/>
+      <c r="B37" s="6"/>
       <c r="C37" t="s">
         <v>106</v>
       </c>
@@ -2463,8 +2488,8 @@
       </c>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A38" s="5"/>
-      <c r="B38" s="6" t="s">
+      <c r="A38" s="6"/>
+      <c r="B38" s="7" t="s">
         <v>109</v>
       </c>
       <c r="F38" t="s">
@@ -2475,8 +2500,8 @@
       </c>
     </row>
     <row r="39" spans="1:8" ht="34" x14ac:dyDescent="0.2">
-      <c r="A39" s="5"/>
-      <c r="B39" s="6"/>
+      <c r="A39" s="6"/>
+      <c r="B39" s="7"/>
       <c r="C39" t="s">
         <v>103</v>
       </c>
@@ -2494,8 +2519,8 @@
       </c>
     </row>
     <row r="40" spans="1:8" ht="34" x14ac:dyDescent="0.2">
-      <c r="A40" s="5"/>
-      <c r="B40" s="6"/>
+      <c r="A40" s="6"/>
+      <c r="B40" s="7"/>
       <c r="C40" t="s">
         <v>106</v>
       </c>
@@ -2513,8 +2538,8 @@
       </c>
     </row>
     <row r="41" spans="1:8" ht="51" x14ac:dyDescent="0.2">
-      <c r="A41" s="5"/>
-      <c r="B41" s="5" t="s">
+      <c r="A41" s="6"/>
+      <c r="B41" s="6" t="s">
         <v>112</v>
       </c>
       <c r="F41" t="s">
@@ -2525,8 +2550,8 @@
       </c>
     </row>
     <row r="42" spans="1:8" ht="51" x14ac:dyDescent="0.2">
-      <c r="A42" s="5"/>
-      <c r="B42" s="5"/>
+      <c r="A42" s="6"/>
+      <c r="B42" s="6"/>
       <c r="C42" t="s">
         <v>114</v>
       </c>
@@ -2547,8 +2572,8 @@
       </c>
     </row>
     <row r="43" spans="1:8" ht="68" x14ac:dyDescent="0.2">
-      <c r="A43" s="5"/>
-      <c r="B43" s="5"/>
+      <c r="A43" s="6"/>
+      <c r="B43" s="6"/>
       <c r="C43" t="s">
         <v>106</v>
       </c>
@@ -2569,8 +2594,8 @@
       </c>
     </row>
     <row r="44" spans="1:8" ht="17" x14ac:dyDescent="0.2">
-      <c r="A44" s="5"/>
-      <c r="B44" s="5" t="s">
+      <c r="A44" s="6"/>
+      <c r="B44" s="6" t="s">
         <v>121</v>
       </c>
       <c r="F44" t="s">
@@ -2581,8 +2606,8 @@
       </c>
     </row>
     <row r="45" spans="1:8" ht="51" x14ac:dyDescent="0.2">
-      <c r="A45" s="5"/>
-      <c r="B45" s="5"/>
+      <c r="A45" s="6"/>
+      <c r="B45" s="6"/>
       <c r="C45" t="s">
         <v>103</v>
       </c>
@@ -2603,8 +2628,8 @@
       </c>
     </row>
     <row r="46" spans="1:8" ht="51" x14ac:dyDescent="0.2">
-      <c r="A46" s="5"/>
-      <c r="B46" s="5"/>
+      <c r="A46" s="6"/>
+      <c r="B46" s="6"/>
       <c r="C46" t="s">
         <v>106</v>
       </c>
@@ -2625,8 +2650,8 @@
       </c>
     </row>
     <row r="47" spans="1:8" ht="17" x14ac:dyDescent="0.2">
-      <c r="A47" s="5"/>
-      <c r="B47" s="5" t="s">
+      <c r="A47" s="6"/>
+      <c r="B47" s="6" t="s">
         <v>127</v>
       </c>
       <c r="F47" t="s">
@@ -2637,8 +2662,8 @@
       </c>
     </row>
     <row r="48" spans="1:8" ht="51" x14ac:dyDescent="0.2">
-      <c r="A48" s="5"/>
-      <c r="B48" s="5"/>
+      <c r="A48" s="6"/>
+      <c r="B48" s="6"/>
       <c r="C48" t="s">
         <v>103</v>
       </c>
@@ -2656,8 +2681,8 @@
       </c>
     </row>
     <row r="49" spans="1:8" ht="51" x14ac:dyDescent="0.2">
-      <c r="A49" s="5"/>
-      <c r="B49" s="5"/>
+      <c r="A49" s="6"/>
+      <c r="B49" s="6"/>
       <c r="C49" t="s">
         <v>106</v>
       </c>
@@ -2678,8 +2703,8 @@
       </c>
     </row>
     <row r="50" spans="1:8" ht="17" x14ac:dyDescent="0.2">
-      <c r="A50" s="5"/>
-      <c r="B50" s="5" t="s">
+      <c r="A50" s="6"/>
+      <c r="B50" s="6" t="s">
         <v>134</v>
       </c>
       <c r="F50" t="s">
@@ -2690,8 +2715,8 @@
       </c>
     </row>
     <row r="51" spans="1:8" ht="51" x14ac:dyDescent="0.2">
-      <c r="A51" s="5"/>
-      <c r="B51" s="5"/>
+      <c r="A51" s="6"/>
+      <c r="B51" s="6"/>
       <c r="C51" t="s">
         <v>103</v>
       </c>
@@ -2712,8 +2737,8 @@
       </c>
     </row>
     <row r="52" spans="1:8" ht="51" x14ac:dyDescent="0.2">
-      <c r="A52" s="5"/>
-      <c r="B52" s="5"/>
+      <c r="A52" s="6"/>
+      <c r="B52" s="6"/>
       <c r="C52" t="s">
         <v>106</v>
       </c>
@@ -2734,123 +2759,135 @@
       </c>
     </row>
     <row r="53" spans="1:8" ht="17" x14ac:dyDescent="0.2">
-      <c r="A53" t="s">
+      <c r="A53" s="6"/>
+      <c r="B53" s="6" t="s">
+        <v>418</v>
+      </c>
+      <c r="F53" t="s">
+        <v>101</v>
+      </c>
+      <c r="H53" s="2" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="54" spans="1:8" ht="34" x14ac:dyDescent="0.2">
+      <c r="A54" s="6"/>
+      <c r="B54" s="6"/>
+      <c r="C54" t="s">
+        <v>103</v>
+      </c>
+      <c r="D54">
+        <v>0</v>
+      </c>
+      <c r="E54" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="F54" t="s">
+        <v>101</v>
+      </c>
+      <c r="G54" s="2" t="s">
+        <v>419</v>
+      </c>
+      <c r="H54" s="8" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="55" spans="1:8" ht="34" x14ac:dyDescent="0.2">
+      <c r="A55" s="6"/>
+      <c r="B55" s="6"/>
+      <c r="C55" t="s">
+        <v>106</v>
+      </c>
+      <c r="D55">
+        <v>0</v>
+      </c>
+      <c r="E55" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="F55" t="s">
+        <v>101</v>
+      </c>
+      <c r="G55" s="2" t="s">
+        <v>420</v>
+      </c>
+      <c r="H55" s="8" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="56" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="A56" s="6"/>
+      <c r="B56" s="5" t="s">
+        <v>416</v>
+      </c>
+      <c r="D56" s="4" t="s">
+        <v>391</v>
+      </c>
+      <c r="E56" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="F56" t="s">
+        <v>101</v>
+      </c>
+      <c r="G56" s="2" t="s">
+        <v>417</v>
+      </c>
+      <c r="H56" s="2" t="s">
+        <v>422</v>
+      </c>
+    </row>
+    <row r="57" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="A57" t="s">
         <v>141</v>
       </c>
-      <c r="D53">
+      <c r="D57">
         <v>100</v>
       </c>
-      <c r="E53" s="2" t="s">
+      <c r="E57" s="2" t="s">
         <v>142</v>
       </c>
-      <c r="F53" t="s">
-        <v>101</v>
-      </c>
-      <c r="G53" s="2" t="s">
+      <c r="F57" t="s">
+        <v>101</v>
+      </c>
+      <c r="G57" s="2" t="s">
         <v>143</v>
       </c>
-      <c r="H53" s="2" t="s">
+      <c r="H57" s="2" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A54" s="5" t="s">
+    <row r="58" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A58" s="6" t="s">
         <v>404</v>
       </c>
-      <c r="F54" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="55" spans="1:8" ht="34" x14ac:dyDescent="0.2">
-      <c r="A55" s="5"/>
-      <c r="B55" t="s">
+      <c r="F58" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="59" spans="1:8" ht="34" x14ac:dyDescent="0.2">
+      <c r="A59" s="6"/>
+      <c r="B59" t="s">
         <v>316</v>
       </c>
-      <c r="D55" s="4" t="s">
+      <c r="D59" s="4" t="s">
         <v>364</v>
       </c>
-      <c r="E55" s="2" t="s">
+      <c r="E59" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="F55" t="s">
-        <v>101</v>
-      </c>
-      <c r="G55" s="2" t="s">
+      <c r="F59" t="s">
+        <v>101</v>
+      </c>
+      <c r="G59" s="2" t="s">
         <v>405</v>
       </c>
     </row>
-    <row r="56" spans="1:8" ht="17" x14ac:dyDescent="0.2">
-      <c r="A56" s="5"/>
-      <c r="B56" t="s">
+    <row r="60" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="A60" s="6"/>
+      <c r="B60" t="s">
         <v>406</v>
       </c>
-      <c r="D56">
+      <c r="D60">
         <v>50000</v>
-      </c>
-      <c r="E56" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="F56" t="s">
-        <v>101</v>
-      </c>
-      <c r="G56" s="2" t="s">
-        <v>409</v>
-      </c>
-    </row>
-    <row r="57" spans="1:8" ht="34" x14ac:dyDescent="0.2">
-      <c r="A57" s="5"/>
-      <c r="B57" t="s">
-        <v>408</v>
-      </c>
-      <c r="D57" s="4" t="s">
-        <v>391</v>
-      </c>
-      <c r="E57" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="F57" t="s">
-        <v>101</v>
-      </c>
-      <c r="G57" s="2" t="s">
-        <v>411</v>
-      </c>
-      <c r="H57" s="2" t="s">
-        <v>410</v>
-      </c>
-    </row>
-    <row r="58" spans="1:8" ht="17" x14ac:dyDescent="0.2">
-      <c r="A58" s="5"/>
-      <c r="B58" t="s">
-        <v>407</v>
-      </c>
-      <c r="D58">
-        <v>123</v>
-      </c>
-      <c r="E58" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="F58" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="59" spans="1:8" ht="17" x14ac:dyDescent="0.2">
-      <c r="A59" t="s">
-        <v>101</v>
-      </c>
-      <c r="F59" t="s">
-        <v>101</v>
-      </c>
-      <c r="H59" s="2" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="60" spans="1:8" ht="34" x14ac:dyDescent="0.2">
-      <c r="A60" s="5"/>
-      <c r="B60" t="s">
-        <v>146</v>
-      </c>
-      <c r="D60">
-        <v>16</v>
       </c>
       <c r="E60" s="2" t="s">
         <v>78</v>
@@ -2859,229 +2896,210 @@
         <v>101</v>
       </c>
       <c r="G60" s="2" t="s">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="61" spans="1:8" ht="34" x14ac:dyDescent="0.2">
+      <c r="A61" s="6"/>
+      <c r="B61" t="s">
+        <v>408</v>
+      </c>
+      <c r="D61" s="4" t="s">
+        <v>391</v>
+      </c>
+      <c r="E61" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="F61" t="s">
+        <v>101</v>
+      </c>
+      <c r="G61" s="2" t="s">
+        <v>411</v>
+      </c>
+      <c r="H61" s="2" t="s">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="62" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="A62" s="6"/>
+      <c r="B62" t="s">
+        <v>407</v>
+      </c>
+      <c r="D62">
+        <v>123</v>
+      </c>
+      <c r="E62" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="F62" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="63" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="A63" t="s">
+        <v>101</v>
+      </c>
+      <c r="F63" t="s">
+        <v>101</v>
+      </c>
+      <c r="H63" s="2" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="64" spans="1:8" ht="34" x14ac:dyDescent="0.2">
+      <c r="A64" s="6"/>
+      <c r="B64" t="s">
+        <v>146</v>
+      </c>
+      <c r="D64">
+        <v>16</v>
+      </c>
+      <c r="E64" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="F64" t="s">
+        <v>101</v>
+      </c>
+      <c r="G64" s="2" t="s">
         <v>147</v>
       </c>
-      <c r="H60" s="2" t="s">
+      <c r="H64" s="2" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="61" spans="1:8" ht="68" x14ac:dyDescent="0.2">
-      <c r="A61" s="5"/>
-      <c r="B61" t="s">
+    <row r="65" spans="1:8" ht="68" x14ac:dyDescent="0.2">
+      <c r="A65" s="6"/>
+      <c r="B65" t="s">
         <v>149</v>
       </c>
-      <c r="D61" t="s">
+      <c r="D65" t="s">
         <v>150</v>
       </c>
-      <c r="E61" s="2" t="s">
+      <c r="E65" s="2" t="s">
         <v>151</v>
       </c>
-      <c r="F61" t="s">
-        <v>101</v>
-      </c>
-      <c r="G61" s="2" t="s">
+      <c r="F65" t="s">
+        <v>101</v>
+      </c>
+      <c r="G65" s="2" t="s">
         <v>152</v>
       </c>
-      <c r="H61" s="2" t="s">
+      <c r="H65" s="2" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="62" spans="1:8" ht="136" x14ac:dyDescent="0.2">
-      <c r="A62" s="5"/>
-      <c r="B62" t="s">
+    <row r="66" spans="1:8" ht="136" x14ac:dyDescent="0.2">
+      <c r="A66" s="6"/>
+      <c r="B66" t="s">
         <v>154</v>
       </c>
-      <c r="D62" t="s">
+      <c r="D66" t="s">
         <v>155</v>
       </c>
-      <c r="E62" s="2" t="s">
+      <c r="E66" s="2" t="s">
         <v>400</v>
       </c>
-      <c r="F62" t="s">
-        <v>101</v>
-      </c>
-      <c r="G62" s="2" t="s">
+      <c r="F66" t="s">
+        <v>101</v>
+      </c>
+      <c r="G66" s="2" t="s">
         <v>156</v>
       </c>
-      <c r="H62" s="2" t="s">
+      <c r="H66" s="2" t="s">
         <v>401</v>
       </c>
     </row>
-    <row r="63" spans="1:8" ht="51" x14ac:dyDescent="0.2">
-      <c r="A63" s="5"/>
-      <c r="B63" t="s">
+    <row r="67" spans="1:8" ht="51" x14ac:dyDescent="0.2">
+      <c r="A67" s="6"/>
+      <c r="B67" t="s">
         <v>157</v>
       </c>
-      <c r="D63" s="1">
+      <c r="D67" s="1">
         <v>9.9999999999999993E-41</v>
       </c>
-      <c r="E63" s="2" t="s">
+      <c r="E67" s="2" t="s">
         <v>158</v>
       </c>
-      <c r="F63" t="s">
-        <v>101</v>
-      </c>
-      <c r="G63" s="2" t="s">
+      <c r="F67" t="s">
+        <v>101</v>
+      </c>
+      <c r="G67" s="2" t="s">
         <v>159</v>
       </c>
-      <c r="H63" s="2" t="s">
+      <c r="H67" s="2" t="s">
         <v>160</v>
       </c>
     </row>
-    <row r="64" spans="1:8" ht="34" x14ac:dyDescent="0.2">
-      <c r="A64" s="5"/>
-      <c r="B64" t="s">
+    <row r="68" spans="1:8" ht="34" x14ac:dyDescent="0.2">
+      <c r="A68" s="6"/>
+      <c r="B68" t="s">
         <v>161</v>
       </c>
-      <c r="D64" t="s">
+      <c r="D68" t="s">
         <v>162</v>
       </c>
-      <c r="E64" s="2" t="s">
+      <c r="E68" s="2" t="s">
         <v>163</v>
       </c>
-      <c r="F64" t="s">
-        <v>101</v>
-      </c>
-      <c r="G64" s="2" t="s">
+      <c r="F68" t="s">
+        <v>101</v>
+      </c>
+      <c r="G68" s="2" t="s">
         <v>164</v>
-      </c>
-      <c r="H64" s="2" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="65" spans="1:8" ht="34" x14ac:dyDescent="0.2">
-      <c r="A65" s="5"/>
-      <c r="B65" t="s">
-        <v>166</v>
-      </c>
-      <c r="D65" s="1">
-        <v>1E-4</v>
-      </c>
-      <c r="E65" s="2" t="s">
-        <v>158</v>
-      </c>
-      <c r="F65" t="s">
-        <v>101</v>
-      </c>
-      <c r="G65" s="2" t="s">
-        <v>167</v>
-      </c>
-      <c r="H65" s="2" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="66" spans="1:8" ht="34" x14ac:dyDescent="0.2">
-      <c r="A66" s="5"/>
-      <c r="B66" t="s">
-        <v>169</v>
-      </c>
-      <c r="D66" s="1">
-        <v>9.9999999999999993E-41</v>
-      </c>
-      <c r="E66" s="2" t="s">
-        <v>158</v>
-      </c>
-      <c r="F66" t="s">
-        <v>101</v>
-      </c>
-      <c r="G66" s="2" t="s">
-        <v>170</v>
-      </c>
-      <c r="H66" s="2" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="67" spans="1:8" ht="51" x14ac:dyDescent="0.2">
-      <c r="A67" s="5"/>
-      <c r="B67" t="s">
-        <v>171</v>
-      </c>
-      <c r="D67" t="s">
-        <v>155</v>
-      </c>
-      <c r="E67" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="F67" t="s">
-        <v>101</v>
-      </c>
-      <c r="G67" s="2" t="s">
-        <v>172</v>
-      </c>
-      <c r="H67" s="2" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="68" spans="1:8" ht="51" x14ac:dyDescent="0.2">
-      <c r="A68" s="5"/>
-      <c r="B68" t="s">
-        <v>173</v>
-      </c>
-      <c r="D68" t="s">
-        <v>155</v>
-      </c>
-      <c r="E68" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="F68" t="s">
-        <v>101</v>
-      </c>
-      <c r="G68" s="2" t="s">
-        <v>174</v>
       </c>
       <c r="H68" s="2" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="69" spans="1:8" ht="51" x14ac:dyDescent="0.2">
-      <c r="A69" s="5"/>
+    <row r="69" spans="1:8" ht="34" x14ac:dyDescent="0.2">
+      <c r="A69" s="6"/>
       <c r="B69" t="s">
-        <v>175</v>
-      </c>
-      <c r="D69" t="s">
-        <v>176</v>
+        <v>166</v>
+      </c>
+      <c r="D69" s="1">
+        <v>1E-4</v>
       </c>
       <c r="E69" s="2" t="s">
-        <v>177</v>
+        <v>158</v>
       </c>
       <c r="F69" t="s">
         <v>101</v>
       </c>
       <c r="G69" s="2" t="s">
-        <v>178</v>
+        <v>167</v>
       </c>
       <c r="H69" s="2" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="70" spans="1:8" ht="17" x14ac:dyDescent="0.2">
-      <c r="A70" s="5"/>
+        <v>168</v>
+      </c>
+    </row>
+    <row r="70" spans="1:8" ht="34" x14ac:dyDescent="0.2">
+      <c r="A70" s="6"/>
       <c r="B70" t="s">
-        <v>180</v>
-      </c>
-      <c r="D70" t="s">
-        <v>62</v>
+        <v>169</v>
+      </c>
+      <c r="D70" s="1">
+        <v>9.9999999999999993E-41</v>
       </c>
       <c r="E70" s="2" t="s">
-        <v>63</v>
+        <v>158</v>
       </c>
       <c r="F70" t="s">
         <v>101</v>
       </c>
       <c r="G70" s="2" t="s">
-        <v>181</v>
+        <v>170</v>
       </c>
       <c r="H70" s="2" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="71" spans="1:8" ht="34" x14ac:dyDescent="0.2">
-      <c r="A71" s="5"/>
+    <row r="71" spans="1:8" ht="51" x14ac:dyDescent="0.2">
+      <c r="A71" s="6"/>
       <c r="B71" t="s">
-        <v>182</v>
+        <v>171</v>
       </c>
       <c r="D71" t="s">
-        <v>62</v>
+        <v>155</v>
       </c>
       <c r="E71" s="2" t="s">
         <v>63</v>
@@ -3090,290 +3108,293 @@
         <v>101</v>
       </c>
       <c r="G71" s="2" t="s">
-        <v>183</v>
+        <v>172</v>
       </c>
       <c r="H71" s="2" t="s">
-        <v>184</v>
+        <v>165</v>
       </c>
     </row>
     <row r="72" spans="1:8" ht="51" x14ac:dyDescent="0.2">
-      <c r="A72" s="5"/>
+      <c r="A72" s="6"/>
       <c r="B72" t="s">
-        <v>185</v>
-      </c>
-      <c r="D72">
-        <v>0.42</v>
+        <v>173</v>
+      </c>
+      <c r="D72" t="s">
+        <v>155</v>
       </c>
       <c r="E72" s="2" t="s">
-        <v>186</v>
+        <v>63</v>
       </c>
       <c r="F72" t="s">
         <v>101</v>
       </c>
       <c r="G72" s="2" t="s">
-        <v>187</v>
+        <v>174</v>
       </c>
       <c r="H72" s="2" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="73" spans="1:8" ht="34" x14ac:dyDescent="0.2">
-      <c r="A73" s="5"/>
+    <row r="73" spans="1:8" ht="51" x14ac:dyDescent="0.2">
+      <c r="A73" s="6"/>
       <c r="B73" t="s">
-        <v>188</v>
-      </c>
-      <c r="D73">
-        <v>4</v>
+        <v>175</v>
+      </c>
+      <c r="D73" t="s">
+        <v>176</v>
       </c>
       <c r="E73" s="2" t="s">
-        <v>189</v>
+        <v>177</v>
       </c>
       <c r="F73" t="s">
         <v>101</v>
       </c>
       <c r="G73" s="2" t="s">
-        <v>190</v>
+        <v>178</v>
       </c>
       <c r="H73" s="2" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="74" spans="1:8" ht="34" x14ac:dyDescent="0.2">
-      <c r="A74" s="5"/>
+        <v>179</v>
+      </c>
+    </row>
+    <row r="74" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="A74" s="6"/>
       <c r="B74" t="s">
-        <v>191</v>
-      </c>
-      <c r="D74">
-        <v>-5</v>
+        <v>180</v>
+      </c>
+      <c r="D74" t="s">
+        <v>62</v>
       </c>
       <c r="E74" s="2" t="s">
-        <v>189</v>
+        <v>63</v>
       </c>
       <c r="F74" t="s">
         <v>101</v>
       </c>
       <c r="G74" s="2" t="s">
-        <v>192</v>
+        <v>181</v>
       </c>
       <c r="H74" s="2" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="75" spans="1:8" ht="68" x14ac:dyDescent="0.2">
-      <c r="A75" s="5"/>
+    <row r="75" spans="1:8" ht="34" x14ac:dyDescent="0.2">
+      <c r="A75" s="6"/>
       <c r="B75" t="s">
+        <v>182</v>
+      </c>
+      <c r="D75" t="s">
+        <v>62</v>
+      </c>
+      <c r="E75" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="F75" t="s">
+        <v>101</v>
+      </c>
+      <c r="G75" s="2" t="s">
+        <v>183</v>
+      </c>
+      <c r="H75" s="2" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="76" spans="1:8" ht="51" x14ac:dyDescent="0.2">
+      <c r="A76" s="6"/>
+      <c r="B76" t="s">
+        <v>185</v>
+      </c>
+      <c r="D76">
+        <v>0.42</v>
+      </c>
+      <c r="E76" s="2" t="s">
+        <v>186</v>
+      </c>
+      <c r="F76" t="s">
+        <v>101</v>
+      </c>
+      <c r="G76" s="2" t="s">
+        <v>187</v>
+      </c>
+      <c r="H76" s="2" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="77" spans="1:8" ht="34" x14ac:dyDescent="0.2">
+      <c r="A77" s="6"/>
+      <c r="B77" t="s">
+        <v>188</v>
+      </c>
+      <c r="D77">
+        <v>4</v>
+      </c>
+      <c r="E77" s="2" t="s">
+        <v>189</v>
+      </c>
+      <c r="F77" t="s">
+        <v>101</v>
+      </c>
+      <c r="G77" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="H77" s="2" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="78" spans="1:8" ht="34" x14ac:dyDescent="0.2">
+      <c r="A78" s="6"/>
+      <c r="B78" t="s">
+        <v>191</v>
+      </c>
+      <c r="D78">
+        <v>-5</v>
+      </c>
+      <c r="E78" s="2" t="s">
+        <v>189</v>
+      </c>
+      <c r="F78" t="s">
+        <v>101</v>
+      </c>
+      <c r="G78" s="2" t="s">
+        <v>192</v>
+      </c>
+      <c r="H78" s="2" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="79" spans="1:8" ht="68" x14ac:dyDescent="0.2">
+      <c r="A79" s="6"/>
+      <c r="B79" t="s">
         <v>193</v>
       </c>
-      <c r="D75">
+      <c r="D79">
         <v>-8</v>
       </c>
-      <c r="E75" s="2" t="s">
+      <c r="E79" s="2" t="s">
         <v>189</v>
       </c>
-      <c r="F75" t="s">
-        <v>101</v>
-      </c>
-      <c r="G75" s="2" t="s">
+      <c r="F79" t="s">
+        <v>101</v>
+      </c>
+      <c r="G79" s="2" t="s">
         <v>194</v>
       </c>
-      <c r="H75" s="2" t="s">
+      <c r="H79" s="2" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="76" spans="1:8" ht="17" x14ac:dyDescent="0.2">
-      <c r="A76" s="5" t="s">
+    <row r="80" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="A80" s="6" t="s">
         <v>195</v>
       </c>
-      <c r="F76" t="s">
-        <v>101</v>
-      </c>
-      <c r="H76" s="2" t="s">
+      <c r="F80" t="s">
+        <v>101</v>
+      </c>
+      <c r="H80" s="2" t="s">
         <v>196</v>
       </c>
     </row>
-    <row r="77" spans="1:8" ht="34" x14ac:dyDescent="0.2">
-      <c r="A77" s="5"/>
-      <c r="B77" t="s">
+    <row r="81" spans="1:8" ht="34" x14ac:dyDescent="0.2">
+      <c r="A81" s="6"/>
+      <c r="B81" t="s">
         <v>197</v>
       </c>
-      <c r="D77">
+      <c r="D81">
         <v>12</v>
       </c>
-      <c r="E77" s="2" t="s">
+      <c r="E81" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="F77" t="s">
-        <v>101</v>
-      </c>
-      <c r="G77" s="2" t="s">
+      <c r="F81" t="s">
+        <v>101</v>
+      </c>
+      <c r="G81" s="2" t="s">
         <v>198</v>
       </c>
-      <c r="H77" s="2" t="s">
+      <c r="H81" s="2" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="78" spans="1:8" ht="34" x14ac:dyDescent="0.2">
-      <c r="A78" s="5"/>
-      <c r="B78" t="s">
+    <row r="82" spans="1:8" ht="34" x14ac:dyDescent="0.2">
+      <c r="A82" s="6"/>
+      <c r="B82" t="s">
         <v>199</v>
       </c>
-      <c r="D78">
+      <c r="D82">
         <v>0</v>
       </c>
-      <c r="E78" s="2" t="s">
+      <c r="E82" s="2" t="s">
         <v>200</v>
       </c>
-      <c r="F78" t="s">
-        <v>101</v>
-      </c>
-      <c r="G78" s="2" t="s">
+      <c r="F82" t="s">
+        <v>101</v>
+      </c>
+      <c r="G82" s="2" t="s">
         <v>201</v>
       </c>
-      <c r="H78" s="2" t="s">
+      <c r="H82" s="2" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="79" spans="1:8" ht="68" x14ac:dyDescent="0.2">
-      <c r="A79" s="5"/>
-      <c r="B79" t="s">
+    <row r="83" spans="1:8" ht="68" x14ac:dyDescent="0.2">
+      <c r="A83" s="6"/>
+      <c r="B83" t="s">
         <v>202</v>
       </c>
-      <c r="D79" t="s">
+      <c r="D83" t="s">
         <v>155</v>
       </c>
-      <c r="E79" s="2" t="s">
+      <c r="E83" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="F79" t="s">
-        <v>101</v>
-      </c>
-      <c r="G79" s="2" t="s">
+      <c r="F83" t="s">
+        <v>101</v>
+      </c>
+      <c r="G83" s="2" t="s">
         <v>203</v>
       </c>
-      <c r="H79" s="2" t="s">
+      <c r="H83" s="2" t="s">
         <v>204</v>
       </c>
     </row>
-    <row r="80" spans="1:8" ht="34" x14ac:dyDescent="0.2">
-      <c r="A80" s="5"/>
-      <c r="B80" t="s">
+    <row r="84" spans="1:8" ht="34" x14ac:dyDescent="0.2">
+      <c r="A84" s="6"/>
+      <c r="B84" t="s">
         <v>205</v>
       </c>
-      <c r="D80" t="s">
+      <c r="D84" t="s">
         <v>62</v>
       </c>
-      <c r="E80" s="2" t="s">
+      <c r="E84" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="F80" t="s">
-        <v>101</v>
-      </c>
-      <c r="G80" s="2" t="s">
+      <c r="F84" t="s">
+        <v>101</v>
+      </c>
+      <c r="G84" s="2" t="s">
         <v>206</v>
       </c>
-      <c r="H80" s="2" t="s">
+      <c r="H84" s="2" t="s">
         <v>207</v>
       </c>
     </row>
-    <row r="81" spans="1:8" ht="17" x14ac:dyDescent="0.2">
-      <c r="A81" s="5" t="s">
+    <row r="85" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="A85" s="6" t="s">
         <v>208</v>
       </c>
-      <c r="F81" t="s">
-        <v>101</v>
-      </c>
-      <c r="H81" s="2" t="s">
+      <c r="F85" t="s">
+        <v>101</v>
+      </c>
+      <c r="H85" s="2" t="s">
         <v>209</v>
       </c>
     </row>
-    <row r="82" spans="1:8" ht="17" x14ac:dyDescent="0.2">
-      <c r="A82" s="5"/>
-      <c r="B82" t="s">
+    <row r="86" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="A86" s="6"/>
+      <c r="B86" t="s">
         <v>210</v>
       </c>
-      <c r="D82" t="s">
+      <c r="D86" t="s">
         <v>62</v>
-      </c>
-      <c r="E82" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="F82" t="s">
-        <v>101</v>
-      </c>
-      <c r="G82" s="2" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="83" spans="1:8" ht="85" x14ac:dyDescent="0.2">
-      <c r="A83" s="5"/>
-      <c r="B83" t="s">
-        <v>212</v>
-      </c>
-      <c r="D83" t="s">
-        <v>213</v>
-      </c>
-      <c r="E83" s="2" t="s">
-        <v>214</v>
-      </c>
-      <c r="F83" t="s">
-        <v>101</v>
-      </c>
-      <c r="G83" s="2" t="s">
-        <v>215</v>
-      </c>
-      <c r="H83" s="2" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="84" spans="1:8" ht="34" x14ac:dyDescent="0.2">
-      <c r="A84" s="5"/>
-      <c r="B84" t="s">
-        <v>217</v>
-      </c>
-      <c r="D84">
-        <v>2</v>
-      </c>
-      <c r="E84" s="2" t="s">
-        <v>218</v>
-      </c>
-      <c r="F84" t="s">
-        <v>101</v>
-      </c>
-      <c r="G84" s="2" t="s">
-        <v>219</v>
-      </c>
-      <c r="H84" s="2" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="85" spans="1:8" ht="34" x14ac:dyDescent="0.2">
-      <c r="A85" s="5"/>
-      <c r="B85" t="s">
-        <v>221</v>
-      </c>
-      <c r="D85">
-        <v>8</v>
-      </c>
-      <c r="E85" s="2" t="s">
-        <v>218</v>
-      </c>
-      <c r="F85" t="s">
-        <v>101</v>
-      </c>
-      <c r="G85" s="2" t="s">
-        <v>222</v>
-      </c>
-      <c r="H85" s="2" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="86" spans="1:8" ht="34" x14ac:dyDescent="0.2">
-      <c r="A86" s="5"/>
-      <c r="B86" t="s">
-        <v>223</v>
-      </c>
-      <c r="D86" t="s">
-        <v>155</v>
       </c>
       <c r="E86" s="2" t="s">
         <v>63</v>
@@ -3382,183 +3403,185 @@
         <v>101</v>
       </c>
       <c r="G86" s="2" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="87" spans="1:8" ht="85" x14ac:dyDescent="0.2">
+      <c r="A87" s="6"/>
+      <c r="B87" t="s">
+        <v>212</v>
+      </c>
+      <c r="D87" t="s">
+        <v>213</v>
+      </c>
+      <c r="E87" s="2" t="s">
+        <v>214</v>
+      </c>
+      <c r="F87" t="s">
+        <v>101</v>
+      </c>
+      <c r="G87" s="2" t="s">
+        <v>215</v>
+      </c>
+      <c r="H87" s="2" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="88" spans="1:8" ht="34" x14ac:dyDescent="0.2">
+      <c r="A88" s="6"/>
+      <c r="B88" t="s">
+        <v>217</v>
+      </c>
+      <c r="D88">
+        <v>2</v>
+      </c>
+      <c r="E88" s="2" t="s">
+        <v>218</v>
+      </c>
+      <c r="F88" t="s">
+        <v>101</v>
+      </c>
+      <c r="G88" s="2" t="s">
+        <v>219</v>
+      </c>
+      <c r="H88" s="2" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="89" spans="1:8" ht="34" x14ac:dyDescent="0.2">
+      <c r="A89" s="6"/>
+      <c r="B89" t="s">
+        <v>221</v>
+      </c>
+      <c r="D89">
+        <v>8</v>
+      </c>
+      <c r="E89" s="2" t="s">
+        <v>218</v>
+      </c>
+      <c r="F89" t="s">
+        <v>101</v>
+      </c>
+      <c r="G89" s="2" t="s">
+        <v>222</v>
+      </c>
+      <c r="H89" s="2" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="90" spans="1:8" ht="34" x14ac:dyDescent="0.2">
+      <c r="A90" s="6"/>
+      <c r="B90" t="s">
+        <v>223</v>
+      </c>
+      <c r="D90" t="s">
+        <v>155</v>
+      </c>
+      <c r="E90" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="F90" t="s">
+        <v>101</v>
+      </c>
+      <c r="G90" s="2" t="s">
         <v>224</v>
       </c>
-      <c r="H86" s="2" t="s">
+      <c r="H90" s="2" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="87" spans="1:8" ht="51" x14ac:dyDescent="0.2">
-      <c r="A87" s="5"/>
-      <c r="B87" t="s">
+    <row r="91" spans="1:8" ht="51" x14ac:dyDescent="0.2">
+      <c r="A91" s="6"/>
+      <c r="B91" t="s">
         <v>225</v>
       </c>
-      <c r="D87">
+      <c r="D91">
         <v>4</v>
       </c>
-      <c r="E87" s="2" t="s">
+      <c r="E91" s="2" t="s">
         <v>218</v>
       </c>
-      <c r="F87" t="s">
-        <v>101</v>
-      </c>
-      <c r="G87" s="2" t="s">
+      <c r="F91" t="s">
+        <v>101</v>
+      </c>
+      <c r="G91" s="2" t="s">
         <v>226</v>
       </c>
-      <c r="H87" s="2" t="s">
+      <c r="H91" s="2" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="88" spans="1:8" ht="34" x14ac:dyDescent="0.2">
-      <c r="A88" s="5"/>
-      <c r="B88" t="s">
+    <row r="92" spans="1:8" ht="34" x14ac:dyDescent="0.2">
+      <c r="A92" s="6"/>
+      <c r="B92" t="s">
         <v>227</v>
       </c>
-      <c r="D88">
+      <c r="D92">
         <v>16</v>
       </c>
-      <c r="E88" s="2" t="s">
+      <c r="E92" s="2" t="s">
         <v>189</v>
       </c>
-      <c r="F88" t="s">
-        <v>101</v>
-      </c>
-      <c r="G88" s="2" t="s">
+      <c r="F92" t="s">
+        <v>101</v>
+      </c>
+      <c r="G92" s="2" t="s">
         <v>228</v>
       </c>
-      <c r="H88" s="2" t="s">
+      <c r="H92" s="2" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="89" spans="1:8" ht="17" x14ac:dyDescent="0.2">
-      <c r="A89" s="5" t="s">
+    <row r="93" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="A93" s="6" t="s">
         <v>229</v>
-      </c>
-      <c r="F89" t="s">
-        <v>229</v>
-      </c>
-      <c r="H89" s="2" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="90" spans="1:8" ht="17" x14ac:dyDescent="0.2">
-      <c r="A90" s="5"/>
-      <c r="B90" s="5" t="s">
-        <v>101</v>
-      </c>
-      <c r="F90" t="s">
-        <v>229</v>
-      </c>
-      <c r="H90" s="2" t="s">
-        <v>232</v>
-      </c>
-    </row>
-    <row r="91" spans="1:8" ht="51" x14ac:dyDescent="0.2">
-      <c r="A91" s="5"/>
-      <c r="B91" s="5"/>
-      <c r="C91" t="s">
-        <v>233</v>
-      </c>
-      <c r="D91" t="s">
-        <v>155</v>
-      </c>
-      <c r="E91" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="F91" t="s">
-        <v>229</v>
-      </c>
-      <c r="G91" s="2" t="s">
-        <v>380</v>
-      </c>
-      <c r="H91" s="2" t="s">
-        <v>390</v>
-      </c>
-    </row>
-    <row r="92" spans="1:8" ht="51" x14ac:dyDescent="0.2">
-      <c r="A92" s="5"/>
-      <c r="B92" s="5"/>
-      <c r="C92" t="s">
-        <v>236</v>
-      </c>
-      <c r="D92" t="s">
-        <v>155</v>
-      </c>
-      <c r="E92" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="F92" t="s">
-        <v>229</v>
-      </c>
-      <c r="G92" s="2" t="s">
-        <v>381</v>
-      </c>
-      <c r="H92" s="2" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="93" spans="1:8" ht="17" x14ac:dyDescent="0.2">
-      <c r="A93" s="5"/>
-      <c r="B93" s="5"/>
-      <c r="C93" t="s">
-        <v>239</v>
-      </c>
-      <c r="D93" t="s">
-        <v>393</v>
       </c>
       <c r="F93" t="s">
         <v>229</v>
       </c>
-      <c r="G93" s="2" t="s">
-        <v>241</v>
-      </c>
       <c r="H93" s="2" t="s">
-        <v>242</v>
+        <v>230</v>
       </c>
     </row>
     <row r="94" spans="1:8" ht="17" x14ac:dyDescent="0.2">
-      <c r="A94" s="5"/>
-      <c r="B94" s="5"/>
-      <c r="C94" t="s">
-        <v>385</v>
-      </c>
-      <c r="D94" t="s">
-        <v>394</v>
+      <c r="A94" s="6"/>
+      <c r="B94" s="6" t="s">
+        <v>101</v>
       </c>
       <c r="F94" t="s">
         <v>229</v>
       </c>
-      <c r="G94" s="2" t="s">
-        <v>244</v>
-      </c>
-    </row>
-    <row r="95" spans="1:8" ht="34" x14ac:dyDescent="0.2">
-      <c r="A95" s="5"/>
-      <c r="B95" s="5"/>
+      <c r="H94" s="2" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="95" spans="1:8" ht="51" x14ac:dyDescent="0.2">
+      <c r="A95" s="6"/>
+      <c r="B95" s="6"/>
       <c r="C95" t="s">
-        <v>386</v>
-      </c>
-      <c r="D95">
-        <v>50</v>
+        <v>233</v>
+      </c>
+      <c r="D95" t="s">
+        <v>155</v>
       </c>
       <c r="E95" s="2" t="s">
-        <v>246</v>
+        <v>63</v>
       </c>
       <c r="F95" t="s">
         <v>229</v>
       </c>
       <c r="G95" s="2" t="s">
-        <v>247</v>
+        <v>380</v>
       </c>
       <c r="H95" s="2" t="s">
-        <v>382</v>
+        <v>390</v>
       </c>
     </row>
     <row r="96" spans="1:8" ht="51" x14ac:dyDescent="0.2">
-      <c r="A96" s="5"/>
-      <c r="B96" s="5"/>
+      <c r="A96" s="6"/>
+      <c r="B96" s="6"/>
       <c r="C96" t="s">
-        <v>387</v>
+        <v>236</v>
       </c>
       <c r="D96" t="s">
         <v>155</v>
@@ -3570,114 +3593,118 @@
         <v>229</v>
       </c>
       <c r="G96" s="2" t="s">
-        <v>388</v>
+        <v>381</v>
       </c>
       <c r="H96" s="2" t="s">
-        <v>389</v>
-      </c>
-    </row>
-    <row r="97" spans="1:8" ht="34" x14ac:dyDescent="0.2">
-      <c r="A97" s="5"/>
-      <c r="B97" s="5"/>
+        <v>238</v>
+      </c>
+    </row>
+    <row r="97" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="A97" s="6"/>
+      <c r="B97" s="6"/>
       <c r="C97" t="s">
-        <v>256</v>
-      </c>
-      <c r="D97">
-        <v>100</v>
-      </c>
-      <c r="E97" s="2" t="s">
-        <v>78</v>
+        <v>239</v>
+      </c>
+      <c r="D97" t="s">
+        <v>393</v>
       </c>
       <c r="F97" t="s">
         <v>229</v>
       </c>
       <c r="G97" s="2" t="s">
-        <v>383</v>
+        <v>241</v>
       </c>
       <c r="H97" s="2" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="98" spans="1:8" ht="51" x14ac:dyDescent="0.2">
-      <c r="A98" s="5"/>
-      <c r="B98" s="5"/>
+        <v>242</v>
+      </c>
+    </row>
+    <row r="98" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="A98" s="6"/>
+      <c r="B98" s="6"/>
       <c r="C98" t="s">
-        <v>258</v>
+        <v>385</v>
       </c>
       <c r="D98" t="s">
-        <v>155</v>
-      </c>
-      <c r="E98" s="2" t="s">
-        <v>63</v>
+        <v>394</v>
       </c>
       <c r="F98" t="s">
         <v>229</v>
       </c>
       <c r="G98" s="2" t="s">
-        <v>384</v>
-      </c>
-      <c r="H98" s="2" t="s">
-        <v>260</v>
+        <v>244</v>
       </c>
     </row>
     <row r="99" spans="1:8" ht="34" x14ac:dyDescent="0.2">
-      <c r="A99" s="5"/>
-      <c r="B99" s="5"/>
+      <c r="A99" s="6"/>
+      <c r="B99" s="6"/>
       <c r="C99" t="s">
-        <v>261</v>
-      </c>
-      <c r="D99" t="s">
-        <v>395</v>
+        <v>386</v>
+      </c>
+      <c r="D99">
+        <v>50</v>
+      </c>
+      <c r="E99" s="2" t="s">
+        <v>246</v>
       </c>
       <c r="F99" t="s">
         <v>229</v>
       </c>
       <c r="G99" s="2" t="s">
-        <v>262</v>
+        <v>247</v>
       </c>
       <c r="H99" s="2" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="100" spans="1:8" ht="17" x14ac:dyDescent="0.2">
-      <c r="A100" s="5"/>
-      <c r="B100" s="5" t="s">
-        <v>231</v>
+        <v>382</v>
+      </c>
+    </row>
+    <row r="100" spans="1:8" ht="51" x14ac:dyDescent="0.2">
+      <c r="A100" s="6"/>
+      <c r="B100" s="6"/>
+      <c r="C100" t="s">
+        <v>387</v>
+      </c>
+      <c r="D100" t="s">
+        <v>155</v>
+      </c>
+      <c r="E100" s="2" t="s">
+        <v>63</v>
       </c>
       <c r="F100" t="s">
         <v>229</v>
       </c>
+      <c r="G100" s="2" t="s">
+        <v>388</v>
+      </c>
       <c r="H100" s="2" t="s">
-        <v>232</v>
-      </c>
-    </row>
-    <row r="101" spans="1:8" ht="68" x14ac:dyDescent="0.2">
-      <c r="A101" s="5"/>
-      <c r="B101" s="5"/>
+        <v>389</v>
+      </c>
+    </row>
+    <row r="101" spans="1:8" ht="34" x14ac:dyDescent="0.2">
+      <c r="A101" s="6"/>
+      <c r="B101" s="6"/>
       <c r="C101" t="s">
-        <v>233</v>
-      </c>
-      <c r="D101" t="s">
-        <v>155</v>
+        <v>256</v>
+      </c>
+      <c r="D101">
+        <v>100</v>
       </c>
       <c r="E101" s="2" t="s">
-        <v>63</v>
+        <v>78</v>
       </c>
       <c r="F101" t="s">
         <v>229</v>
       </c>
       <c r="G101" s="2" t="s">
-        <v>234</v>
+        <v>383</v>
       </c>
       <c r="H101" s="2" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="102" spans="1:8" ht="34" x14ac:dyDescent="0.2">
-      <c r="A102" s="5"/>
-      <c r="B102" s="5"/>
+        <v>144</v>
+      </c>
+    </row>
+    <row r="102" spans="1:8" ht="51" x14ac:dyDescent="0.2">
+      <c r="A102" s="6"/>
+      <c r="B102" s="6"/>
       <c r="C102" t="s">
-        <v>236</v>
+        <v>258</v>
       </c>
       <c r="D102" t="s">
         <v>155</v>
@@ -3689,212 +3716,212 @@
         <v>229</v>
       </c>
       <c r="G102" s="2" t="s">
-        <v>237</v>
+        <v>384</v>
       </c>
       <c r="H102" s="2" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="103" spans="1:8" ht="17" x14ac:dyDescent="0.2">
-      <c r="A103" s="5"/>
-      <c r="B103" s="5"/>
+        <v>260</v>
+      </c>
+    </row>
+    <row r="103" spans="1:8" ht="34" x14ac:dyDescent="0.2">
+      <c r="A103" s="6"/>
+      <c r="B103" s="6"/>
       <c r="C103" t="s">
-        <v>239</v>
+        <v>261</v>
       </c>
       <c r="D103" t="s">
-        <v>240</v>
+        <v>395</v>
       </c>
       <c r="F103" t="s">
         <v>229</v>
       </c>
       <c r="G103" s="2" t="s">
-        <v>241</v>
+        <v>262</v>
       </c>
       <c r="H103" s="2" t="s">
         <v>242</v>
       </c>
     </row>
     <row r="104" spans="1:8" ht="17" x14ac:dyDescent="0.2">
-      <c r="A104" s="5"/>
-      <c r="B104" s="5"/>
-      <c r="C104" t="s">
-        <v>243</v>
-      </c>
-      <c r="D104" t="s">
-        <v>396</v>
+      <c r="A104" s="6"/>
+      <c r="B104" s="6" t="s">
+        <v>231</v>
       </c>
       <c r="F104" t="s">
         <v>229</v>
       </c>
-      <c r="G104" s="2" t="s">
-        <v>244</v>
-      </c>
-    </row>
-    <row r="105" spans="1:8" ht="17" x14ac:dyDescent="0.2">
-      <c r="A105" s="5"/>
-      <c r="B105" s="5"/>
+      <c r="H104" s="2" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="105" spans="1:8" ht="68" x14ac:dyDescent="0.2">
+      <c r="A105" s="6"/>
+      <c r="B105" s="6"/>
       <c r="C105" t="s">
-        <v>245</v>
-      </c>
-      <c r="D105">
-        <v>60</v>
+        <v>233</v>
+      </c>
+      <c r="D105" t="s">
+        <v>155</v>
       </c>
       <c r="E105" s="2" t="s">
-        <v>246</v>
+        <v>63</v>
       </c>
       <c r="F105" t="s">
         <v>229</v>
       </c>
       <c r="G105" s="2" t="s">
-        <v>247</v>
+        <v>234</v>
       </c>
       <c r="H105" s="2" t="s">
-        <v>248</v>
-      </c>
-    </row>
-    <row r="106" spans="1:8" ht="51" x14ac:dyDescent="0.2">
-      <c r="A106" s="5"/>
-      <c r="B106" s="5"/>
+        <v>235</v>
+      </c>
+    </row>
+    <row r="106" spans="1:8" ht="34" x14ac:dyDescent="0.2">
+      <c r="A106" s="6"/>
+      <c r="B106" s="6"/>
       <c r="C106" t="s">
-        <v>249</v>
+        <v>236</v>
       </c>
       <c r="D106" t="s">
-        <v>250</v>
+        <v>155</v>
       </c>
       <c r="E106" s="2" t="s">
-        <v>251</v>
+        <v>63</v>
       </c>
       <c r="F106" t="s">
         <v>229</v>
       </c>
       <c r="G106" s="2" t="s">
-        <v>252</v>
+        <v>237</v>
       </c>
       <c r="H106" s="2" t="s">
-        <v>253</v>
+        <v>238</v>
       </c>
     </row>
     <row r="107" spans="1:8" ht="17" x14ac:dyDescent="0.2">
-      <c r="A107" s="5"/>
-      <c r="B107" s="5"/>
+      <c r="A107" s="6"/>
+      <c r="B107" s="6"/>
       <c r="C107" t="s">
-        <v>254</v>
-      </c>
-      <c r="D107">
-        <v>100</v>
-      </c>
-      <c r="E107" s="2" t="s">
-        <v>78</v>
+        <v>239</v>
+      </c>
+      <c r="D107" t="s">
+        <v>240</v>
       </c>
       <c r="F107" t="s">
         <v>229</v>
       </c>
       <c r="G107" s="2" t="s">
-        <v>255</v>
+        <v>241</v>
+      </c>
+      <c r="H107" s="2" t="s">
+        <v>242</v>
       </c>
     </row>
     <row r="108" spans="1:8" ht="17" x14ac:dyDescent="0.2">
-      <c r="A108" s="5"/>
-      <c r="B108" s="5"/>
+      <c r="A108" s="6"/>
+      <c r="B108" s="6"/>
       <c r="C108" t="s">
-        <v>256</v>
-      </c>
-      <c r="D108">
-        <v>100</v>
-      </c>
-      <c r="E108" s="2" t="s">
-        <v>78</v>
+        <v>243</v>
+      </c>
+      <c r="D108" t="s">
+        <v>396</v>
       </c>
       <c r="F108" t="s">
         <v>229</v>
       </c>
       <c r="G108" s="2" t="s">
-        <v>257</v>
-      </c>
-      <c r="H108" s="2" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="109" spans="1:8" ht="51" x14ac:dyDescent="0.2">
-      <c r="A109" s="5"/>
-      <c r="B109" s="5"/>
+        <v>244</v>
+      </c>
+    </row>
+    <row r="109" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="A109" s="6"/>
+      <c r="B109" s="6"/>
       <c r="C109" t="s">
-        <v>258</v>
-      </c>
-      <c r="D109" t="s">
-        <v>155</v>
+        <v>245</v>
+      </c>
+      <c r="D109">
+        <v>60</v>
       </c>
       <c r="E109" s="2" t="s">
-        <v>63</v>
+        <v>246</v>
       </c>
       <c r="F109" t="s">
         <v>229</v>
       </c>
       <c r="G109" s="2" t="s">
-        <v>259</v>
+        <v>247</v>
       </c>
       <c r="H109" s="2" t="s">
-        <v>260</v>
-      </c>
-    </row>
-    <row r="110" spans="1:8" ht="34" x14ac:dyDescent="0.2">
-      <c r="A110" s="5"/>
-      <c r="B110" s="5"/>
+        <v>248</v>
+      </c>
+    </row>
+    <row r="110" spans="1:8" ht="51" x14ac:dyDescent="0.2">
+      <c r="A110" s="6"/>
+      <c r="B110" s="6"/>
       <c r="C110" t="s">
-        <v>261</v>
+        <v>249</v>
       </c>
       <c r="D110" t="s">
-        <v>395</v>
+        <v>250</v>
+      </c>
+      <c r="E110" s="2" t="s">
+        <v>251</v>
       </c>
       <c r="F110" t="s">
         <v>229</v>
       </c>
       <c r="G110" s="2" t="s">
-        <v>262</v>
+        <v>252</v>
       </c>
       <c r="H110" s="2" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="111" spans="1:8" ht="34" x14ac:dyDescent="0.2">
-      <c r="A111" s="5"/>
-      <c r="B111" s="5" t="s">
-        <v>263</v>
+        <v>253</v>
+      </c>
+    </row>
+    <row r="111" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="A111" s="6"/>
+      <c r="B111" s="6"/>
+      <c r="C111" t="s">
+        <v>254</v>
+      </c>
+      <c r="D111">
+        <v>100</v>
+      </c>
+      <c r="E111" s="2" t="s">
+        <v>78</v>
       </c>
       <c r="F111" t="s">
         <v>229</v>
       </c>
-      <c r="H111" s="2" t="s">
-        <v>264</v>
-      </c>
-    </row>
-    <row r="112" spans="1:8" ht="68" x14ac:dyDescent="0.2">
-      <c r="A112" s="5"/>
-      <c r="B112" s="5"/>
+      <c r="G111" s="2" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="112" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="A112" s="6"/>
+      <c r="B112" s="6"/>
       <c r="C112" t="s">
-        <v>233</v>
-      </c>
-      <c r="D112" t="s">
-        <v>62</v>
+        <v>256</v>
+      </c>
+      <c r="D112">
+        <v>100</v>
       </c>
       <c r="E112" s="2" t="s">
-        <v>63</v>
+        <v>78</v>
       </c>
       <c r="F112" t="s">
         <v>229</v>
       </c>
       <c r="G112" s="2" t="s">
-        <v>265</v>
+        <v>257</v>
       </c>
       <c r="H112" s="2" t="s">
-        <v>266</v>
-      </c>
-    </row>
-    <row r="113" spans="1:8" ht="34" x14ac:dyDescent="0.2">
-      <c r="A113" s="5"/>
-      <c r="B113" s="5"/>
+        <v>144</v>
+      </c>
+    </row>
+    <row r="113" spans="1:8" ht="51" x14ac:dyDescent="0.2">
+      <c r="A113" s="6"/>
+      <c r="B113" s="6"/>
       <c r="C113" t="s">
-        <v>236</v>
+        <v>258</v>
       </c>
       <c r="D113" t="s">
         <v>155</v>
@@ -3906,499 +3933,505 @@
         <v>229</v>
       </c>
       <c r="G113" s="2" t="s">
-        <v>267</v>
+        <v>259</v>
       </c>
       <c r="H113" s="2" t="s">
-        <v>268</v>
-      </c>
-    </row>
-    <row r="114" spans="1:8" ht="17" x14ac:dyDescent="0.2">
-      <c r="A114" s="5"/>
-      <c r="B114" s="5"/>
+        <v>260</v>
+      </c>
+    </row>
+    <row r="114" spans="1:8" ht="34" x14ac:dyDescent="0.2">
+      <c r="A114" s="6"/>
+      <c r="B114" s="6"/>
       <c r="C114" t="s">
-        <v>239</v>
+        <v>261</v>
       </c>
       <c r="D114" t="s">
-        <v>398</v>
+        <v>395</v>
       </c>
       <c r="F114" t="s">
         <v>229</v>
       </c>
       <c r="G114" s="2" t="s">
-        <v>241</v>
+        <v>262</v>
       </c>
       <c r="H114" s="2" t="s">
         <v>242</v>
       </c>
     </row>
     <row r="115" spans="1:8" ht="34" x14ac:dyDescent="0.2">
-      <c r="A115" s="5"/>
-      <c r="B115" s="5"/>
-      <c r="C115" t="s">
-        <v>243</v>
-      </c>
-      <c r="D115" t="s">
-        <v>392</v>
+      <c r="A115" s="6"/>
+      <c r="B115" s="6" t="s">
+        <v>263</v>
       </c>
       <c r="F115" t="s">
         <v>229</v>
       </c>
-      <c r="G115" s="2" t="s">
-        <v>269</v>
-      </c>
       <c r="H115" s="2" t="s">
-        <v>270</v>
-      </c>
-    </row>
-    <row r="116" spans="1:8" ht="17" x14ac:dyDescent="0.2">
-      <c r="A116" s="5"/>
-      <c r="B116" s="5"/>
+        <v>264</v>
+      </c>
+    </row>
+    <row r="116" spans="1:8" ht="68" x14ac:dyDescent="0.2">
+      <c r="A116" s="6"/>
+      <c r="B116" s="6"/>
       <c r="C116" t="s">
-        <v>271</v>
-      </c>
-      <c r="D116">
-        <v>60</v>
+        <v>233</v>
+      </c>
+      <c r="D116" t="s">
+        <v>62</v>
       </c>
       <c r="E116" s="2" t="s">
-        <v>246</v>
+        <v>63</v>
       </c>
       <c r="F116" t="s">
         <v>229</v>
       </c>
       <c r="G116" s="2" t="s">
-        <v>272</v>
-      </c>
-    </row>
-    <row r="117" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A117" s="5" t="s">
-        <v>273</v>
+        <v>265</v>
+      </c>
+      <c r="H116" s="2" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="117" spans="1:8" ht="34" x14ac:dyDescent="0.2">
+      <c r="A117" s="6"/>
+      <c r="B117" s="6"/>
+      <c r="C117" t="s">
+        <v>236</v>
+      </c>
+      <c r="D117" t="s">
+        <v>155</v>
+      </c>
+      <c r="E117" s="2" t="s">
+        <v>63</v>
       </c>
       <c r="F117" t="s">
         <v>229</v>
       </c>
+      <c r="G117" s="2" t="s">
+        <v>267</v>
+      </c>
+      <c r="H117" s="2" t="s">
+        <v>268</v>
+      </c>
     </row>
     <row r="118" spans="1:8" ht="17" x14ac:dyDescent="0.2">
-      <c r="A118" s="5"/>
-      <c r="B118" t="s">
-        <v>233</v>
-      </c>
-      <c r="C118" t="b">
-        <v>0</v>
-      </c>
-      <c r="E118" s="2" t="s">
-        <v>63</v>
+      <c r="A118" s="6"/>
+      <c r="B118" s="6"/>
+      <c r="C118" t="s">
+        <v>239</v>
+      </c>
+      <c r="D118" t="s">
+        <v>398</v>
       </c>
       <c r="F118" t="s">
         <v>229</v>
       </c>
       <c r="G118" s="2" t="s">
-        <v>274</v>
-      </c>
-    </row>
-    <row r="119" spans="1:8" ht="17" x14ac:dyDescent="0.2">
-      <c r="A119" s="5"/>
-      <c r="B119" t="s">
-        <v>239</v>
-      </c>
+        <v>241</v>
+      </c>
+      <c r="H118" s="2" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="119" spans="1:8" ht="34" x14ac:dyDescent="0.2">
+      <c r="A119" s="6"/>
+      <c r="B119" s="6"/>
       <c r="C119" t="s">
-        <v>397</v>
+        <v>243</v>
+      </c>
+      <c r="D119" t="s">
+        <v>392</v>
       </c>
       <c r="F119" t="s">
         <v>229</v>
       </c>
       <c r="G119" s="2" t="s">
-        <v>275</v>
+        <v>269</v>
+      </c>
+      <c r="H119" s="2" t="s">
+        <v>270</v>
       </c>
     </row>
     <row r="120" spans="1:8" ht="17" x14ac:dyDescent="0.2">
-      <c r="A120" s="5"/>
-      <c r="B120" t="s">
-        <v>243</v>
-      </c>
+      <c r="A120" s="6"/>
+      <c r="B120" s="6"/>
       <c r="C120" t="s">
-        <v>276</v>
+        <v>271</v>
+      </c>
+      <c r="D120">
+        <v>60</v>
+      </c>
+      <c r="E120" s="2" t="s">
+        <v>246</v>
       </c>
       <c r="F120" t="s">
         <v>229</v>
       </c>
       <c r="G120" s="2" t="s">
-        <v>277</v>
-      </c>
-    </row>
-    <row r="121" spans="1:8" ht="17" x14ac:dyDescent="0.2">
-      <c r="A121" s="5"/>
-      <c r="B121" t="s">
-        <v>278</v>
-      </c>
-      <c r="C121">
-        <v>0.01</v>
+        <v>272</v>
+      </c>
+    </row>
+    <row r="121" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A121" s="6" t="s">
+        <v>273</v>
       </c>
       <c r="F121" t="s">
         <v>229</v>
       </c>
-      <c r="G121" s="2" t="s">
-        <v>279</v>
-      </c>
-    </row>
-    <row r="122" spans="1:8" ht="34" x14ac:dyDescent="0.2">
-      <c r="A122" s="5"/>
+    </row>
+    <row r="122" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="A122" s="6"/>
       <c r="B122" t="s">
-        <v>280</v>
-      </c>
-      <c r="C122" t="s">
-        <v>281</v>
+        <v>233</v>
+      </c>
+      <c r="C122" t="b">
+        <v>0</v>
       </c>
       <c r="E122" s="2" t="s">
-        <v>282</v>
+        <v>63</v>
       </c>
       <c r="F122" t="s">
         <v>229</v>
       </c>
       <c r="G122" s="2" t="s">
-        <v>283</v>
-      </c>
-      <c r="H122" s="2" t="s">
-        <v>284</v>
-      </c>
-    </row>
-    <row r="123" spans="1:8" ht="34" x14ac:dyDescent="0.2">
-      <c r="A123" s="5"/>
+        <v>274</v>
+      </c>
+    </row>
+    <row r="123" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="A123" s="6"/>
       <c r="B123" t="s">
-        <v>285</v>
-      </c>
-      <c r="C123" t="b">
-        <v>0</v>
+        <v>239</v>
+      </c>
+      <c r="C123" t="s">
+        <v>397</v>
       </c>
       <c r="F123" t="s">
         <v>229</v>
       </c>
       <c r="G123" s="2" t="s">
-        <v>286</v>
-      </c>
-      <c r="H123" s="2" t="s">
-        <v>287</v>
+        <v>275</v>
       </c>
     </row>
     <row r="124" spans="1:8" ht="17" x14ac:dyDescent="0.2">
-      <c r="A124" s="5" t="s">
-        <v>288</v>
+      <c r="A124" s="6"/>
+      <c r="B124" t="s">
+        <v>243</v>
+      </c>
+      <c r="C124" t="s">
+        <v>276</v>
       </c>
       <c r="F124" t="s">
         <v>229</v>
       </c>
-      <c r="H124" s="2" t="s">
-        <v>289</v>
+      <c r="G124" s="2" t="s">
+        <v>277</v>
       </c>
     </row>
     <row r="125" spans="1:8" ht="17" x14ac:dyDescent="0.2">
-      <c r="A125" s="5"/>
+      <c r="A125" s="6"/>
       <c r="B125" t="s">
-        <v>290</v>
-      </c>
-      <c r="D125" t="s">
-        <v>155</v>
-      </c>
-      <c r="E125" s="2" t="s">
-        <v>63</v>
+        <v>278</v>
+      </c>
+      <c r="C125">
+        <v>0.01</v>
       </c>
       <c r="F125" t="s">
         <v>229</v>
       </c>
       <c r="G125" s="2" t="s">
-        <v>291</v>
-      </c>
-      <c r="H125" s="2" t="s">
-        <v>292</v>
+        <v>279</v>
       </c>
     </row>
     <row r="126" spans="1:8" ht="34" x14ac:dyDescent="0.2">
-      <c r="A126" s="5"/>
+      <c r="A126" s="6"/>
       <c r="B126" t="s">
-        <v>293</v>
-      </c>
-      <c r="D126">
-        <v>1</v>
-      </c>
-      <c r="E126" s="3">
-        <v>43922</v>
+        <v>280</v>
+      </c>
+      <c r="C126" t="s">
+        <v>281</v>
+      </c>
+      <c r="E126" s="2" t="s">
+        <v>282</v>
       </c>
       <c r="F126" t="s">
         <v>229</v>
       </c>
       <c r="G126" s="2" t="s">
-        <v>294</v>
+        <v>283</v>
       </c>
       <c r="H126" s="2" t="s">
-        <v>295</v>
-      </c>
-    </row>
-    <row r="127" spans="1:8" ht="17" x14ac:dyDescent="0.2">
-      <c r="A127" s="5"/>
+        <v>284</v>
+      </c>
+    </row>
+    <row r="127" spans="1:8" ht="34" x14ac:dyDescent="0.2">
+      <c r="A127" s="6"/>
       <c r="B127" t="s">
-        <v>296</v>
-      </c>
-      <c r="D127" t="s">
-        <v>297</v>
-      </c>
-      <c r="E127" s="2" t="s">
-        <v>298</v>
+        <v>285</v>
+      </c>
+      <c r="C127" t="b">
+        <v>0</v>
       </c>
       <c r="F127" t="s">
         <v>229</v>
       </c>
       <c r="G127" s="2" t="s">
-        <v>299</v>
+        <v>286</v>
+      </c>
+      <c r="H127" s="2" t="s">
+        <v>287</v>
       </c>
     </row>
     <row r="128" spans="1:8" ht="17" x14ac:dyDescent="0.2">
-      <c r="A128" s="5"/>
-      <c r="B128" t="s">
-        <v>300</v>
-      </c>
-      <c r="D128" s="1">
-        <v>1.0000000000000001E-5</v>
-      </c>
-      <c r="E128" s="2" t="s">
-        <v>86</v>
+      <c r="A128" s="6" t="s">
+        <v>288</v>
       </c>
       <c r="F128" t="s">
         <v>229</v>
       </c>
-      <c r="G128" s="2" t="s">
+      <c r="H128" s="2" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="129" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="A129" s="6"/>
+      <c r="B129" t="s">
+        <v>290</v>
+      </c>
+      <c r="D129" t="s">
+        <v>155</v>
+      </c>
+      <c r="E129" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="F129" t="s">
+        <v>229</v>
+      </c>
+      <c r="G129" s="2" t="s">
+        <v>291</v>
+      </c>
+      <c r="H129" s="2" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="130" spans="1:8" ht="34" x14ac:dyDescent="0.2">
+      <c r="A130" s="6"/>
+      <c r="B130" t="s">
+        <v>293</v>
+      </c>
+      <c r="D130">
+        <v>1</v>
+      </c>
+      <c r="E130" s="3">
+        <v>43922</v>
+      </c>
+      <c r="F130" t="s">
+        <v>229</v>
+      </c>
+      <c r="G130" s="2" t="s">
+        <v>294</v>
+      </c>
+      <c r="H130" s="2" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="131" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="A131" s="6"/>
+      <c r="B131" t="s">
+        <v>296</v>
+      </c>
+      <c r="D131" t="s">
+        <v>297</v>
+      </c>
+      <c r="E131" s="2" t="s">
+        <v>298</v>
+      </c>
+      <c r="F131" t="s">
+        <v>229</v>
+      </c>
+      <c r="G131" s="2" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="132" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="A132" s="6"/>
+      <c r="B132" t="s">
+        <v>300</v>
+      </c>
+      <c r="D132" s="1">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="E132" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="F132" t="s">
+        <v>229</v>
+      </c>
+      <c r="G132" s="2" t="s">
         <v>301</v>
       </c>
     </row>
-    <row r="129" spans="1:8" ht="17" x14ac:dyDescent="0.2">
-      <c r="A129" s="5" t="s">
+    <row r="133" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="A133" s="6" t="s">
         <v>302</v>
       </c>
-      <c r="F129" t="s">
+      <c r="F133" t="s">
         <v>303</v>
       </c>
-      <c r="H129" s="2" t="s">
+      <c r="H133" s="2" t="s">
         <v>304</v>
       </c>
     </row>
-    <row r="130" spans="1:8" ht="34" x14ac:dyDescent="0.2">
-      <c r="A130" s="5"/>
-      <c r="B130" t="s">
+    <row r="134" spans="1:8" ht="34" x14ac:dyDescent="0.2">
+      <c r="A134" s="6"/>
+      <c r="B134" t="s">
         <v>305</v>
       </c>
-      <c r="D130" s="4" t="s">
+      <c r="D134" s="4" t="s">
         <v>391</v>
       </c>
-      <c r="E130" s="2" t="s">
+      <c r="E134" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="F130" t="s">
+      <c r="F134" t="s">
         <v>306</v>
       </c>
-      <c r="G130" s="2" t="s">
+      <c r="G134" s="2" t="s">
         <v>307</v>
       </c>
-      <c r="H130" s="2" t="s">
+      <c r="H134" s="2" t="s">
         <v>308</v>
       </c>
     </row>
-    <row r="131" spans="1:8" ht="51" x14ac:dyDescent="0.2">
-      <c r="A131" s="5"/>
-      <c r="B131" t="s">
+    <row r="135" spans="1:8" ht="51" x14ac:dyDescent="0.2">
+      <c r="A135" s="6"/>
+      <c r="B135" t="s">
         <v>309</v>
       </c>
-      <c r="D131" s="4" t="s">
+      <c r="D135" s="4" t="s">
         <v>364</v>
       </c>
-      <c r="E131" s="2" t="s">
+      <c r="E135" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="F131" t="s">
+      <c r="F135" t="s">
         <v>310</v>
       </c>
-      <c r="G131" s="2" t="s">
+      <c r="G135" s="2" t="s">
         <v>311</v>
       </c>
-      <c r="H131" s="2" t="s">
+      <c r="H135" s="2" t="s">
         <v>312</v>
       </c>
     </row>
-    <row r="132" spans="1:8" ht="34" x14ac:dyDescent="0.2">
-      <c r="A132" s="5" t="s">
+    <row r="136" spans="1:8" ht="34" x14ac:dyDescent="0.2">
+      <c r="A136" s="6" t="s">
         <v>313</v>
-      </c>
-      <c r="F132" t="s">
-        <v>314</v>
-      </c>
-      <c r="H132" s="2" t="s">
-        <v>315</v>
-      </c>
-    </row>
-    <row r="133" spans="1:8" ht="51" x14ac:dyDescent="0.2">
-      <c r="A133" s="5"/>
-      <c r="B133" t="s">
-        <v>316</v>
-      </c>
-      <c r="D133" s="4" t="s">
-        <v>391</v>
-      </c>
-      <c r="E133" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="F133" t="s">
-        <v>314</v>
-      </c>
-      <c r="G133" s="2" t="s">
-        <v>317</v>
-      </c>
-    </row>
-    <row r="134" spans="1:8" ht="51" x14ac:dyDescent="0.2">
-      <c r="A134" s="5"/>
-      <c r="B134" t="s">
-        <v>353</v>
-      </c>
-      <c r="D134" t="s">
-        <v>318</v>
-      </c>
-      <c r="E134" s="2" t="s">
-        <v>319</v>
-      </c>
-      <c r="F134" t="s">
-        <v>314</v>
-      </c>
-      <c r="G134" s="2" t="s">
-        <v>320</v>
-      </c>
-      <c r="H134" s="2" t="s">
-        <v>321</v>
-      </c>
-    </row>
-    <row r="135" spans="1:8" ht="17" x14ac:dyDescent="0.2">
-      <c r="A135" s="5"/>
-      <c r="B135" t="s">
-        <v>322</v>
-      </c>
-      <c r="D135">
-        <v>1</v>
-      </c>
-      <c r="F135" t="s">
-        <v>314</v>
-      </c>
-      <c r="G135" s="2" t="s">
-        <v>323</v>
-      </c>
-      <c r="H135" s="2" t="s">
-        <v>324</v>
-      </c>
-    </row>
-    <row r="136" spans="1:8" ht="17" x14ac:dyDescent="0.2">
-      <c r="A136" s="5"/>
-      <c r="B136" t="s">
-        <v>325</v>
-      </c>
-      <c r="D136">
-        <v>10000</v>
       </c>
       <c r="F136" t="s">
         <v>314</v>
       </c>
-      <c r="G136" s="2" t="s">
-        <v>326</v>
-      </c>
       <c r="H136" s="2" t="s">
-        <v>324</v>
-      </c>
-    </row>
-    <row r="137" spans="1:8" ht="17" x14ac:dyDescent="0.2">
-      <c r="A137" s="5" t="s">
-        <v>314</v>
+        <v>315</v>
+      </c>
+    </row>
+    <row r="137" spans="1:8" ht="51" x14ac:dyDescent="0.2">
+      <c r="A137" s="6"/>
+      <c r="B137" t="s">
+        <v>316</v>
+      </c>
+      <c r="D137" s="4" t="s">
+        <v>391</v>
+      </c>
+      <c r="E137" s="2" t="s">
+        <v>63</v>
       </c>
       <c r="F137" t="s">
         <v>314</v>
       </c>
-      <c r="H137" s="2" t="s">
-        <v>327</v>
-      </c>
-    </row>
-    <row r="138" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A138" s="5"/>
-      <c r="B138" s="6" t="s">
-        <v>415</v>
+      <c r="G137" s="2" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="138" spans="1:8" ht="51" x14ac:dyDescent="0.2">
+      <c r="A138" s="6"/>
+      <c r="B138" t="s">
+        <v>353</v>
+      </c>
+      <c r="D138" t="s">
+        <v>318</v>
+      </c>
+      <c r="E138" s="2" t="s">
+        <v>319</v>
       </c>
       <c r="F138" t="s">
         <v>314</v>
       </c>
+      <c r="G138" s="2" t="s">
+        <v>320</v>
+      </c>
+      <c r="H138" s="2" t="s">
+        <v>321</v>
+      </c>
     </row>
     <row r="139" spans="1:8" ht="17" x14ac:dyDescent="0.2">
-      <c r="A139" s="5"/>
-      <c r="B139" s="6"/>
-      <c r="C139" t="s">
-        <v>233</v>
-      </c>
-      <c r="D139" s="4" t="s">
-        <v>364</v>
-      </c>
-      <c r="E139" s="2" t="s">
-        <v>63</v>
+      <c r="A139" s="6"/>
+      <c r="B139" t="s">
+        <v>322</v>
+      </c>
+      <c r="D139">
+        <v>1</v>
       </c>
       <c r="F139" t="s">
         <v>314</v>
       </c>
-    </row>
-    <row r="140" spans="1:8" ht="34" x14ac:dyDescent="0.2">
-      <c r="A140" s="5"/>
-      <c r="B140" s="6"/>
-      <c r="C140" t="s">
-        <v>333</v>
-      </c>
-      <c r="D140" t="s">
-        <v>334</v>
-      </c>
-      <c r="E140" s="2" t="s">
-        <v>335</v>
+      <c r="G139" s="2" t="s">
+        <v>323</v>
+      </c>
+      <c r="H139" s="2" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="140" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="A140" s="6"/>
+      <c r="B140" t="s">
+        <v>325</v>
+      </c>
+      <c r="D140">
+        <v>10000</v>
       </c>
       <c r="F140" t="s">
         <v>314</v>
       </c>
       <c r="G140" s="2" t="s">
-        <v>336</v>
+        <v>326</v>
       </c>
       <c r="H140" s="2" t="s">
-        <v>337</v>
+        <v>324</v>
       </c>
     </row>
     <row r="141" spans="1:8" ht="17" x14ac:dyDescent="0.2">
-      <c r="A141" s="5"/>
-      <c r="B141" s="6"/>
-      <c r="C141" t="s">
-        <v>412</v>
-      </c>
-      <c r="D141" t="s">
-        <v>413</v>
+      <c r="A141" s="6" t="s">
+        <v>314</v>
       </c>
       <c r="F141" t="s">
         <v>314</v>
       </c>
-      <c r="G141" s="2" t="s">
-        <v>414</v>
-      </c>
       <c r="H141" s="2" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="142" spans="1:8" ht="17" x14ac:dyDescent="0.2">
-      <c r="A142" s="5"/>
-      <c r="B142" s="5" t="s">
-        <v>328</v>
+        <v>327</v>
+      </c>
+    </row>
+    <row r="142" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A142" s="6"/>
+      <c r="B142" s="7" t="s">
+        <v>415</v>
       </c>
       <c r="F142" t="s">
         <v>314</v>
       </c>
-      <c r="H142" s="2" t="s">
-        <v>329</v>
-      </c>
     </row>
     <row r="143" spans="1:8" ht="17" x14ac:dyDescent="0.2">
-      <c r="A143" s="5"/>
-      <c r="B143" s="5"/>
+      <c r="A143" s="6"/>
+      <c r="B143" s="7"/>
       <c r="C143" t="s">
         <v>233</v>
       </c>
@@ -4411,145 +4444,215 @@
       <c r="F143" t="s">
         <v>314</v>
       </c>
-      <c r="G143" s="2" t="s">
-        <v>330</v>
-      </c>
-    </row>
-    <row r="144" spans="1:8" ht="17" x14ac:dyDescent="0.2">
-      <c r="A144" s="5"/>
-      <c r="B144" s="5"/>
+    </row>
+    <row r="144" spans="1:8" ht="34" x14ac:dyDescent="0.2">
+      <c r="A144" s="6"/>
+      <c r="B144" s="7"/>
       <c r="C144" t="s">
-        <v>331</v>
+        <v>333</v>
       </c>
       <c r="D144" t="s">
-        <v>399</v>
+        <v>334</v>
+      </c>
+      <c r="E144" s="2" t="s">
+        <v>335</v>
       </c>
       <c r="F144" t="s">
         <v>314</v>
       </c>
       <c r="G144" s="2" t="s">
-        <v>332</v>
+        <v>336</v>
       </c>
       <c r="H144" s="2" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="145" spans="1:8" ht="34" x14ac:dyDescent="0.2">
-      <c r="A145" s="5"/>
-      <c r="B145" s="5"/>
+        <v>337</v>
+      </c>
+    </row>
+    <row r="145" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="A145" s="6"/>
+      <c r="B145" s="7"/>
       <c r="C145" t="s">
-        <v>333</v>
+        <v>412</v>
       </c>
       <c r="D145" t="s">
-        <v>334</v>
-      </c>
-      <c r="E145" s="2" t="s">
-        <v>335</v>
+        <v>413</v>
       </c>
       <c r="F145" t="s">
         <v>314</v>
       </c>
       <c r="G145" s="2" t="s">
-        <v>336</v>
+        <v>414</v>
       </c>
       <c r="H145" s="2" t="s">
-        <v>337</v>
+        <v>242</v>
       </c>
     </row>
     <row r="146" spans="1:8" ht="17" x14ac:dyDescent="0.2">
-      <c r="A146" s="5"/>
-      <c r="B146" s="5" t="s">
-        <v>338</v>
-      </c>
-      <c r="E146" s="2" t="s">
-        <v>63</v>
+      <c r="A146" s="6"/>
+      <c r="B146" s="6" t="s">
+        <v>328</v>
       </c>
       <c r="F146" t="s">
         <v>314</v>
       </c>
+      <c r="H146" s="2" t="s">
+        <v>329</v>
+      </c>
     </row>
     <row r="147" spans="1:8" ht="17" x14ac:dyDescent="0.2">
-      <c r="A147" s="5"/>
-      <c r="B147" s="5"/>
+      <c r="A147" s="6"/>
+      <c r="B147" s="6"/>
       <c r="C147" t="s">
         <v>233</v>
       </c>
       <c r="D147" s="4" t="s">
-        <v>391</v>
+        <v>364</v>
+      </c>
+      <c r="E147" s="2" t="s">
+        <v>63</v>
       </c>
       <c r="F147" t="s">
         <v>314</v>
       </c>
       <c r="G147" s="2" t="s">
-        <v>339</v>
+        <v>330</v>
       </c>
     </row>
     <row r="148" spans="1:8" ht="17" x14ac:dyDescent="0.2">
-      <c r="A148" s="5"/>
-      <c r="B148" s="5"/>
+      <c r="A148" s="6"/>
+      <c r="B148" s="6"/>
       <c r="C148" t="s">
-        <v>340</v>
+        <v>331</v>
       </c>
       <c r="D148" t="s">
-        <v>281</v>
+        <v>399</v>
       </c>
       <c r="F148" t="s">
         <v>314</v>
       </c>
       <c r="G148" s="2" t="s">
-        <v>341</v>
+        <v>332</v>
       </c>
       <c r="H148" s="2" t="s">
         <v>242</v>
       </c>
     </row>
-    <row r="149" spans="1:8" ht="17" x14ac:dyDescent="0.2">
-      <c r="A149" s="5"/>
-      <c r="B149" t="s">
-        <v>342</v>
-      </c>
-      <c r="D149" s="4" t="s">
-        <v>391</v>
+    <row r="149" spans="1:8" ht="34" x14ac:dyDescent="0.2">
+      <c r="A149" s="6"/>
+      <c r="B149" s="6"/>
+      <c r="C149" t="s">
+        <v>333</v>
+      </c>
+      <c r="D149" t="s">
+        <v>334</v>
       </c>
       <c r="E149" s="2" t="s">
-        <v>63</v>
+        <v>335</v>
       </c>
       <c r="F149" t="s">
         <v>314</v>
       </c>
       <c r="G149" s="2" t="s">
+        <v>336</v>
+      </c>
+      <c r="H149" s="2" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="150" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="A150" s="6"/>
+      <c r="B150" s="6" t="s">
+        <v>338</v>
+      </c>
+      <c r="E150" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="F150" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="151" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="A151" s="6"/>
+      <c r="B151" s="6"/>
+      <c r="C151" t="s">
+        <v>233</v>
+      </c>
+      <c r="D151" s="4" t="s">
+        <v>391</v>
+      </c>
+      <c r="F151" t="s">
+        <v>314</v>
+      </c>
+      <c r="G151" s="2" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="152" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="A152" s="6"/>
+      <c r="B152" s="6"/>
+      <c r="C152" t="s">
+        <v>340</v>
+      </c>
+      <c r="D152" t="s">
+        <v>281</v>
+      </c>
+      <c r="F152" t="s">
+        <v>314</v>
+      </c>
+      <c r="G152" s="2" t="s">
+        <v>341</v>
+      </c>
+      <c r="H152" s="2" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="153" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="A153" s="6"/>
+      <c r="B153" t="s">
+        <v>342</v>
+      </c>
+      <c r="D153" s="4" t="s">
+        <v>391</v>
+      </c>
+      <c r="E153" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="F153" t="s">
+        <v>314</v>
+      </c>
+      <c r="G153" s="2" t="s">
         <v>343</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:H149" xr:uid="{65E3A469-1B8A-364D-8D4D-FD3FF55840DE}"/>
-  <mergeCells count="27">
-    <mergeCell ref="A54:A58"/>
-    <mergeCell ref="B138:B141"/>
+  <autoFilter ref="A1:H153" xr:uid="{65E3A469-1B8A-364D-8D4D-FD3FF55840DE}"/>
+  <mergeCells count="28">
+    <mergeCell ref="A58:A62"/>
     <mergeCell ref="B142:B145"/>
-    <mergeCell ref="B146:B148"/>
-    <mergeCell ref="A60:A75"/>
-    <mergeCell ref="A76:A80"/>
-    <mergeCell ref="A81:A88"/>
-    <mergeCell ref="A89:A116"/>
-    <mergeCell ref="B100:B110"/>
-    <mergeCell ref="B111:B116"/>
-    <mergeCell ref="A117:A123"/>
-    <mergeCell ref="A124:A128"/>
-    <mergeCell ref="A129:A131"/>
-    <mergeCell ref="A132:A136"/>
-    <mergeCell ref="A137:A149"/>
-    <mergeCell ref="B90:B99"/>
+    <mergeCell ref="B50:B52"/>
+    <mergeCell ref="B53:B55"/>
+    <mergeCell ref="B146:B149"/>
+    <mergeCell ref="B150:B152"/>
+    <mergeCell ref="A64:A79"/>
+    <mergeCell ref="A80:A84"/>
+    <mergeCell ref="A85:A92"/>
+    <mergeCell ref="A93:A120"/>
+    <mergeCell ref="B104:B114"/>
+    <mergeCell ref="B115:B120"/>
+    <mergeCell ref="A121:A127"/>
+    <mergeCell ref="A128:A132"/>
+    <mergeCell ref="A133:A135"/>
+    <mergeCell ref="A136:A140"/>
+    <mergeCell ref="A141:A153"/>
+    <mergeCell ref="B94:B103"/>
     <mergeCell ref="A18:A24"/>
     <mergeCell ref="B19:B21"/>
     <mergeCell ref="B22:B24"/>
     <mergeCell ref="A27:A33"/>
-    <mergeCell ref="A34:A52"/>
+    <mergeCell ref="A34:A56"/>
     <mergeCell ref="B35:B37"/>
     <mergeCell ref="B41:B43"/>
     <mergeCell ref="B44:B46"/>
     <mergeCell ref="B47:B49"/>
-    <mergeCell ref="B50:B52"/>
     <mergeCell ref="B38:B40"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
documentation for tax4fun2 and new snakemake additional arguments, fixing #13
</commit_message>
<xml_diff>
--- a/documentation/config_explained.xlsx
+++ b/documentation/config_explained.xlsx
@@ -5,18 +5,18 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/heintzbu/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/heintzbu/Documents/Programs/myOwn/dadasnake/documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{B42F5B3E-750E-3345-9AD7-37C1E53259F1}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1BBF0B63-1997-9D4C-86DE-E457C45C94D6}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="32380" yWindow="800" windowWidth="31000" windowHeight="20240" xr2:uid="{F207B228-D75F-344A-ADB6-4CA41A47821F}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" xr2:uid="{F207B228-D75F-344A-ADB6-4CA41A47821F}"/>
   </bookViews>
   <sheets>
     <sheet name="config_explained" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">config_explained!$A$1:$H$153</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">config_explained!$A$1:$H$159</definedName>
   </definedNames>
   <calcPr calcId="181029"/>
   <extLst>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="774" uniqueCount="423">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="802" uniqueCount="437">
   <si>
     <t xml:space="preserve">email </t>
   </si>
@@ -1297,6 +1297,48 @@
   </si>
   <si>
     <t>useful with Illumina sequencing</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    db</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  tax4fun2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    database_mode</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    normalize_by_copy_number</t>
+  </si>
+  <si>
+    <t>Ref99NR</t>
+  </si>
+  <si>
+    <t>Ref99NR or Ref100NR</t>
+  </si>
+  <si>
+    <t>which tax4fun2 database to use</t>
+  </si>
+  <si>
+    <t>whether tax4fun2 should be run</t>
+  </si>
+  <si>
+    <t>path to tax4fun2 DB</t>
+  </si>
+  <si>
+    <t>whether to normalize tax4fun2 data by copynumber</t>
+  </si>
+  <si>
+    <t>normalization for pathways is no available</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    min_identity_to_reference</t>
+  </si>
+  <si>
+    <t>0.9 to 1.0 or 90 to 100</t>
+  </si>
+  <si>
+    <t>similarity of ASV to DB</t>
   </si>
 </sst>
 </file>
@@ -1332,7 +1374,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1348,10 +1390,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1666,10 +1714,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{61B259DD-FAC6-FB4A-84F8-11B4141970E7}">
-  <dimension ref="A1:H153"/>
+  <dimension ref="A1:H159"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A41" workbookViewId="0">
-      <selection activeCell="H54" sqref="H54"/>
+    <sheetView tabSelected="1" topLeftCell="A135" workbookViewId="0">
+      <selection activeCell="E140" sqref="E140"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2082,7 +2130,7 @@
       </c>
     </row>
     <row r="18" spans="1:8" ht="17" x14ac:dyDescent="0.2">
-      <c r="A18" s="6" t="s">
+      <c r="A18" s="8" t="s">
         <v>36</v>
       </c>
       <c r="B18" t="s">
@@ -2108,8 +2156,8 @@
       </c>
     </row>
     <row r="19" spans="1:8" ht="17" x14ac:dyDescent="0.2">
-      <c r="A19" s="6"/>
-      <c r="B19" s="7" t="s">
+      <c r="A19" s="8"/>
+      <c r="B19" s="9" t="s">
         <v>39</v>
       </c>
       <c r="C19" t="s">
@@ -2132,8 +2180,8 @@
       </c>
     </row>
     <row r="20" spans="1:8" ht="17" x14ac:dyDescent="0.2">
-      <c r="A20" s="6"/>
-      <c r="B20" s="7"/>
+      <c r="A20" s="8"/>
+      <c r="B20" s="9"/>
       <c r="C20" t="s">
         <v>41</v>
       </c>
@@ -2151,8 +2199,8 @@
       </c>
     </row>
     <row r="21" spans="1:8" ht="17" x14ac:dyDescent="0.2">
-      <c r="A21" s="6"/>
-      <c r="B21" s="7"/>
+      <c r="A21" s="8"/>
+      <c r="B21" s="9"/>
       <c r="C21" t="s">
         <v>45</v>
       </c>
@@ -2173,8 +2221,8 @@
       </c>
     </row>
     <row r="22" spans="1:8" ht="17" x14ac:dyDescent="0.2">
-      <c r="A22" s="6"/>
-      <c r="B22" s="6" t="s">
+      <c r="A22" s="8"/>
+      <c r="B22" s="8" t="s">
         <v>50</v>
       </c>
       <c r="C22" t="s">
@@ -2197,8 +2245,8 @@
       </c>
     </row>
     <row r="23" spans="1:8" ht="17" x14ac:dyDescent="0.2">
-      <c r="A23" s="6"/>
-      <c r="B23" s="6"/>
+      <c r="A23" s="8"/>
+      <c r="B23" s="8"/>
       <c r="C23" t="s">
         <v>52</v>
       </c>
@@ -2216,8 +2264,8 @@
       </c>
     </row>
     <row r="24" spans="1:8" ht="17" x14ac:dyDescent="0.2">
-      <c r="A24" s="6"/>
-      <c r="B24" s="6"/>
+      <c r="A24" s="8"/>
+      <c r="B24" s="8"/>
       <c r="C24" t="s">
         <v>57</v>
       </c>
@@ -2278,7 +2326,7 @@
       </c>
     </row>
     <row r="27" spans="1:8" ht="17" x14ac:dyDescent="0.2">
-      <c r="A27" s="6" t="s">
+      <c r="A27" s="8" t="s">
         <v>72</v>
       </c>
       <c r="F27" t="s">
@@ -2289,7 +2337,7 @@
       </c>
     </row>
     <row r="28" spans="1:8" ht="17" x14ac:dyDescent="0.2">
-      <c r="A28" s="6"/>
+      <c r="A28" s="8"/>
       <c r="B28" t="s">
         <v>74</v>
       </c>
@@ -2307,7 +2355,7 @@
       </c>
     </row>
     <row r="29" spans="1:8" ht="34" x14ac:dyDescent="0.2">
-      <c r="A29" s="6"/>
+      <c r="A29" s="8"/>
       <c r="B29" t="s">
         <v>77</v>
       </c>
@@ -2325,7 +2373,7 @@
       </c>
     </row>
     <row r="30" spans="1:8" ht="34" x14ac:dyDescent="0.2">
-      <c r="A30" s="6"/>
+      <c r="A30" s="8"/>
       <c r="B30" t="s">
         <v>80</v>
       </c>
@@ -2346,7 +2394,7 @@
       </c>
     </row>
     <row r="31" spans="1:8" ht="17" x14ac:dyDescent="0.2">
-      <c r="A31" s="6"/>
+      <c r="A31" s="8"/>
       <c r="B31" t="s">
         <v>85</v>
       </c>
@@ -2367,7 +2415,7 @@
       </c>
     </row>
     <row r="32" spans="1:8" ht="34" x14ac:dyDescent="0.2">
-      <c r="A32" s="6"/>
+      <c r="A32" s="8"/>
       <c r="B32" t="s">
         <v>89</v>
       </c>
@@ -2385,7 +2433,7 @@
       </c>
     </row>
     <row r="33" spans="1:8" ht="34" x14ac:dyDescent="0.2">
-      <c r="A33" s="6"/>
+      <c r="A33" s="8"/>
       <c r="B33" t="s">
         <v>93</v>
       </c>
@@ -2406,7 +2454,7 @@
       </c>
     </row>
     <row r="34" spans="1:8" ht="102" x14ac:dyDescent="0.2">
-      <c r="A34" s="6" t="s">
+      <c r="A34" s="8" t="s">
         <v>97</v>
       </c>
       <c r="B34" t="s">
@@ -2432,8 +2480,8 @@
       </c>
     </row>
     <row r="35" spans="1:8" ht="17" x14ac:dyDescent="0.2">
-      <c r="A35" s="6"/>
-      <c r="B35" s="6" t="s">
+      <c r="A35" s="8"/>
+      <c r="B35" s="8" t="s">
         <v>100</v>
       </c>
       <c r="F35" t="s">
@@ -2444,8 +2492,8 @@
       </c>
     </row>
     <row r="36" spans="1:8" ht="34" x14ac:dyDescent="0.2">
-      <c r="A36" s="6"/>
-      <c r="B36" s="6"/>
+      <c r="A36" s="8"/>
+      <c r="B36" s="8"/>
       <c r="C36" t="s">
         <v>103</v>
       </c>
@@ -2466,8 +2514,8 @@
       </c>
     </row>
     <row r="37" spans="1:8" ht="51" x14ac:dyDescent="0.2">
-      <c r="A37" s="6"/>
-      <c r="B37" s="6"/>
+      <c r="A37" s="8"/>
+      <c r="B37" s="8"/>
       <c r="C37" t="s">
         <v>106</v>
       </c>
@@ -2487,9 +2535,9 @@
         <v>108</v>
       </c>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A38" s="6"/>
-      <c r="B38" s="7" t="s">
+    <row r="38" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="A38" s="8"/>
+      <c r="B38" s="9" t="s">
         <v>109</v>
       </c>
       <c r="F38" t="s">
@@ -2500,8 +2548,8 @@
       </c>
     </row>
     <row r="39" spans="1:8" ht="34" x14ac:dyDescent="0.2">
-      <c r="A39" s="6"/>
-      <c r="B39" s="7"/>
+      <c r="A39" s="8"/>
+      <c r="B39" s="9"/>
       <c r="C39" t="s">
         <v>103</v>
       </c>
@@ -2519,8 +2567,8 @@
       </c>
     </row>
     <row r="40" spans="1:8" ht="34" x14ac:dyDescent="0.2">
-      <c r="A40" s="6"/>
-      <c r="B40" s="7"/>
+      <c r="A40" s="8"/>
+      <c r="B40" s="9"/>
       <c r="C40" t="s">
         <v>106</v>
       </c>
@@ -2538,8 +2586,8 @@
       </c>
     </row>
     <row r="41" spans="1:8" ht="51" x14ac:dyDescent="0.2">
-      <c r="A41" s="6"/>
-      <c r="B41" s="6" t="s">
+      <c r="A41" s="8"/>
+      <c r="B41" s="8" t="s">
         <v>112</v>
       </c>
       <c r="F41" t="s">
@@ -2550,8 +2598,8 @@
       </c>
     </row>
     <row r="42" spans="1:8" ht="51" x14ac:dyDescent="0.2">
-      <c r="A42" s="6"/>
-      <c r="B42" s="6"/>
+      <c r="A42" s="8"/>
+      <c r="B42" s="8"/>
       <c r="C42" t="s">
         <v>114</v>
       </c>
@@ -2572,8 +2620,8 @@
       </c>
     </row>
     <row r="43" spans="1:8" ht="68" x14ac:dyDescent="0.2">
-      <c r="A43" s="6"/>
-      <c r="B43" s="6"/>
+      <c r="A43" s="8"/>
+      <c r="B43" s="8"/>
       <c r="C43" t="s">
         <v>106</v>
       </c>
@@ -2594,8 +2642,8 @@
       </c>
     </row>
     <row r="44" spans="1:8" ht="17" x14ac:dyDescent="0.2">
-      <c r="A44" s="6"/>
-      <c r="B44" s="6" t="s">
+      <c r="A44" s="8"/>
+      <c r="B44" s="8" t="s">
         <v>121</v>
       </c>
       <c r="F44" t="s">
@@ -2606,8 +2654,8 @@
       </c>
     </row>
     <row r="45" spans="1:8" ht="51" x14ac:dyDescent="0.2">
-      <c r="A45" s="6"/>
-      <c r="B45" s="6"/>
+      <c r="A45" s="8"/>
+      <c r="B45" s="8"/>
       <c r="C45" t="s">
         <v>103</v>
       </c>
@@ -2628,8 +2676,8 @@
       </c>
     </row>
     <row r="46" spans="1:8" ht="51" x14ac:dyDescent="0.2">
-      <c r="A46" s="6"/>
-      <c r="B46" s="6"/>
+      <c r="A46" s="8"/>
+      <c r="B46" s="8"/>
       <c r="C46" t="s">
         <v>106</v>
       </c>
@@ -2650,8 +2698,8 @@
       </c>
     </row>
     <row r="47" spans="1:8" ht="17" x14ac:dyDescent="0.2">
-      <c r="A47" s="6"/>
-      <c r="B47" s="6" t="s">
+      <c r="A47" s="8"/>
+      <c r="B47" s="8" t="s">
         <v>127</v>
       </c>
       <c r="F47" t="s">
@@ -2662,8 +2710,8 @@
       </c>
     </row>
     <row r="48" spans="1:8" ht="51" x14ac:dyDescent="0.2">
-      <c r="A48" s="6"/>
-      <c r="B48" s="6"/>
+      <c r="A48" s="8"/>
+      <c r="B48" s="8"/>
       <c r="C48" t="s">
         <v>103</v>
       </c>
@@ -2681,8 +2729,8 @@
       </c>
     </row>
     <row r="49" spans="1:8" ht="51" x14ac:dyDescent="0.2">
-      <c r="A49" s="6"/>
-      <c r="B49" s="6"/>
+      <c r="A49" s="8"/>
+      <c r="B49" s="8"/>
       <c r="C49" t="s">
         <v>106</v>
       </c>
@@ -2703,8 +2751,8 @@
       </c>
     </row>
     <row r="50" spans="1:8" ht="17" x14ac:dyDescent="0.2">
-      <c r="A50" s="6"/>
-      <c r="B50" s="6" t="s">
+      <c r="A50" s="8"/>
+      <c r="B50" s="8" t="s">
         <v>134</v>
       </c>
       <c r="F50" t="s">
@@ -2715,8 +2763,8 @@
       </c>
     </row>
     <row r="51" spans="1:8" ht="51" x14ac:dyDescent="0.2">
-      <c r="A51" s="6"/>
-      <c r="B51" s="6"/>
+      <c r="A51" s="8"/>
+      <c r="B51" s="8"/>
       <c r="C51" t="s">
         <v>103</v>
       </c>
@@ -2737,8 +2785,8 @@
       </c>
     </row>
     <row r="52" spans="1:8" ht="51" x14ac:dyDescent="0.2">
-      <c r="A52" s="6"/>
-      <c r="B52" s="6"/>
+      <c r="A52" s="8"/>
+      <c r="B52" s="8"/>
       <c r="C52" t="s">
         <v>106</v>
       </c>
@@ -2759,8 +2807,8 @@
       </c>
     </row>
     <row r="53" spans="1:8" ht="17" x14ac:dyDescent="0.2">
-      <c r="A53" s="6"/>
-      <c r="B53" s="6" t="s">
+      <c r="A53" s="8"/>
+      <c r="B53" s="8" t="s">
         <v>418</v>
       </c>
       <c r="F53" t="s">
@@ -2771,8 +2819,8 @@
       </c>
     </row>
     <row r="54" spans="1:8" ht="34" x14ac:dyDescent="0.2">
-      <c r="A54" s="6"/>
-      <c r="B54" s="6"/>
+      <c r="A54" s="8"/>
+      <c r="B54" s="8"/>
       <c r="C54" t="s">
         <v>103</v>
       </c>
@@ -2788,13 +2836,13 @@
       <c r="G54" s="2" t="s">
         <v>419</v>
       </c>
-      <c r="H54" s="8" t="s">
+      <c r="H54" s="7" t="s">
         <v>421</v>
       </c>
     </row>
     <row r="55" spans="1:8" ht="34" x14ac:dyDescent="0.2">
-      <c r="A55" s="6"/>
-      <c r="B55" s="6"/>
+      <c r="A55" s="8"/>
+      <c r="B55" s="8"/>
       <c r="C55" t="s">
         <v>106</v>
       </c>
@@ -2810,12 +2858,12 @@
       <c r="G55" s="2" t="s">
         <v>420</v>
       </c>
-      <c r="H55" s="8" t="s">
+      <c r="H55" s="7" t="s">
         <v>421</v>
       </c>
     </row>
     <row r="56" spans="1:8" ht="17" x14ac:dyDescent="0.2">
-      <c r="A56" s="6"/>
+      <c r="A56" s="8"/>
       <c r="B56" s="5" t="s">
         <v>416</v>
       </c>
@@ -2856,7 +2904,7 @@
       </c>
     </row>
     <row r="58" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A58" s="6" t="s">
+      <c r="A58" s="8" t="s">
         <v>404</v>
       </c>
       <c r="F58" t="s">
@@ -2864,7 +2912,7 @@
       </c>
     </row>
     <row r="59" spans="1:8" ht="34" x14ac:dyDescent="0.2">
-      <c r="A59" s="6"/>
+      <c r="A59" s="8"/>
       <c r="B59" t="s">
         <v>316</v>
       </c>
@@ -2882,7 +2930,7 @@
       </c>
     </row>
     <row r="60" spans="1:8" ht="17" x14ac:dyDescent="0.2">
-      <c r="A60" s="6"/>
+      <c r="A60" s="8"/>
       <c r="B60" t="s">
         <v>406</v>
       </c>
@@ -2900,7 +2948,7 @@
       </c>
     </row>
     <row r="61" spans="1:8" ht="34" x14ac:dyDescent="0.2">
-      <c r="A61" s="6"/>
+      <c r="A61" s="8"/>
       <c r="B61" t="s">
         <v>408</v>
       </c>
@@ -2921,7 +2969,7 @@
       </c>
     </row>
     <row r="62" spans="1:8" ht="17" x14ac:dyDescent="0.2">
-      <c r="A62" s="6"/>
+      <c r="A62" s="8"/>
       <c r="B62" t="s">
         <v>407</v>
       </c>
@@ -2947,7 +2995,7 @@
       </c>
     </row>
     <row r="64" spans="1:8" ht="34" x14ac:dyDescent="0.2">
-      <c r="A64" s="6"/>
+      <c r="A64" s="8"/>
       <c r="B64" t="s">
         <v>146</v>
       </c>
@@ -2968,7 +3016,7 @@
       </c>
     </row>
     <row r="65" spans="1:8" ht="68" x14ac:dyDescent="0.2">
-      <c r="A65" s="6"/>
+      <c r="A65" s="8"/>
       <c r="B65" t="s">
         <v>149</v>
       </c>
@@ -2989,7 +3037,7 @@
       </c>
     </row>
     <row r="66" spans="1:8" ht="136" x14ac:dyDescent="0.2">
-      <c r="A66" s="6"/>
+      <c r="A66" s="8"/>
       <c r="B66" t="s">
         <v>154</v>
       </c>
@@ -3010,7 +3058,7 @@
       </c>
     </row>
     <row r="67" spans="1:8" ht="51" x14ac:dyDescent="0.2">
-      <c r="A67" s="6"/>
+      <c r="A67" s="8"/>
       <c r="B67" t="s">
         <v>157</v>
       </c>
@@ -3031,7 +3079,7 @@
       </c>
     </row>
     <row r="68" spans="1:8" ht="34" x14ac:dyDescent="0.2">
-      <c r="A68" s="6"/>
+      <c r="A68" s="8"/>
       <c r="B68" t="s">
         <v>161</v>
       </c>
@@ -3052,7 +3100,7 @@
       </c>
     </row>
     <row r="69" spans="1:8" ht="34" x14ac:dyDescent="0.2">
-      <c r="A69" s="6"/>
+      <c r="A69" s="8"/>
       <c r="B69" t="s">
         <v>166</v>
       </c>
@@ -3073,7 +3121,7 @@
       </c>
     </row>
     <row r="70" spans="1:8" ht="34" x14ac:dyDescent="0.2">
-      <c r="A70" s="6"/>
+      <c r="A70" s="8"/>
       <c r="B70" t="s">
         <v>169</v>
       </c>
@@ -3094,7 +3142,7 @@
       </c>
     </row>
     <row r="71" spans="1:8" ht="51" x14ac:dyDescent="0.2">
-      <c r="A71" s="6"/>
+      <c r="A71" s="8"/>
       <c r="B71" t="s">
         <v>171</v>
       </c>
@@ -3115,7 +3163,7 @@
       </c>
     </row>
     <row r="72" spans="1:8" ht="51" x14ac:dyDescent="0.2">
-      <c r="A72" s="6"/>
+      <c r="A72" s="8"/>
       <c r="B72" t="s">
         <v>173</v>
       </c>
@@ -3136,7 +3184,7 @@
       </c>
     </row>
     <row r="73" spans="1:8" ht="51" x14ac:dyDescent="0.2">
-      <c r="A73" s="6"/>
+      <c r="A73" s="8"/>
       <c r="B73" t="s">
         <v>175</v>
       </c>
@@ -3157,7 +3205,7 @@
       </c>
     </row>
     <row r="74" spans="1:8" ht="17" x14ac:dyDescent="0.2">
-      <c r="A74" s="6"/>
+      <c r="A74" s="8"/>
       <c r="B74" t="s">
         <v>180</v>
       </c>
@@ -3178,7 +3226,7 @@
       </c>
     </row>
     <row r="75" spans="1:8" ht="34" x14ac:dyDescent="0.2">
-      <c r="A75" s="6"/>
+      <c r="A75" s="8"/>
       <c r="B75" t="s">
         <v>182</v>
       </c>
@@ -3199,7 +3247,7 @@
       </c>
     </row>
     <row r="76" spans="1:8" ht="51" x14ac:dyDescent="0.2">
-      <c r="A76" s="6"/>
+      <c r="A76" s="8"/>
       <c r="B76" t="s">
         <v>185</v>
       </c>
@@ -3220,7 +3268,7 @@
       </c>
     </row>
     <row r="77" spans="1:8" ht="34" x14ac:dyDescent="0.2">
-      <c r="A77" s="6"/>
+      <c r="A77" s="8"/>
       <c r="B77" t="s">
         <v>188</v>
       </c>
@@ -3241,7 +3289,7 @@
       </c>
     </row>
     <row r="78" spans="1:8" ht="34" x14ac:dyDescent="0.2">
-      <c r="A78" s="6"/>
+      <c r="A78" s="8"/>
       <c r="B78" t="s">
         <v>191</v>
       </c>
@@ -3262,7 +3310,7 @@
       </c>
     </row>
     <row r="79" spans="1:8" ht="68" x14ac:dyDescent="0.2">
-      <c r="A79" s="6"/>
+      <c r="A79" s="8"/>
       <c r="B79" t="s">
         <v>193</v>
       </c>
@@ -3283,7 +3331,7 @@
       </c>
     </row>
     <row r="80" spans="1:8" ht="17" x14ac:dyDescent="0.2">
-      <c r="A80" s="6" t="s">
+      <c r="A80" s="8" t="s">
         <v>195</v>
       </c>
       <c r="F80" t="s">
@@ -3294,7 +3342,7 @@
       </c>
     </row>
     <row r="81" spans="1:8" ht="34" x14ac:dyDescent="0.2">
-      <c r="A81" s="6"/>
+      <c r="A81" s="8"/>
       <c r="B81" t="s">
         <v>197</v>
       </c>
@@ -3315,7 +3363,7 @@
       </c>
     </row>
     <row r="82" spans="1:8" ht="34" x14ac:dyDescent="0.2">
-      <c r="A82" s="6"/>
+      <c r="A82" s="8"/>
       <c r="B82" t="s">
         <v>199</v>
       </c>
@@ -3336,7 +3384,7 @@
       </c>
     </row>
     <row r="83" spans="1:8" ht="68" x14ac:dyDescent="0.2">
-      <c r="A83" s="6"/>
+      <c r="A83" s="8"/>
       <c r="B83" t="s">
         <v>202</v>
       </c>
@@ -3357,7 +3405,7 @@
       </c>
     </row>
     <row r="84" spans="1:8" ht="34" x14ac:dyDescent="0.2">
-      <c r="A84" s="6"/>
+      <c r="A84" s="8"/>
       <c r="B84" t="s">
         <v>205</v>
       </c>
@@ -3378,7 +3426,7 @@
       </c>
     </row>
     <row r="85" spans="1:8" ht="17" x14ac:dyDescent="0.2">
-      <c r="A85" s="6" t="s">
+      <c r="A85" s="8" t="s">
         <v>208</v>
       </c>
       <c r="F85" t="s">
@@ -3389,7 +3437,7 @@
       </c>
     </row>
     <row r="86" spans="1:8" ht="17" x14ac:dyDescent="0.2">
-      <c r="A86" s="6"/>
+      <c r="A86" s="8"/>
       <c r="B86" t="s">
         <v>210</v>
       </c>
@@ -3407,7 +3455,7 @@
       </c>
     </row>
     <row r="87" spans="1:8" ht="85" x14ac:dyDescent="0.2">
-      <c r="A87" s="6"/>
+      <c r="A87" s="8"/>
       <c r="B87" t="s">
         <v>212</v>
       </c>
@@ -3428,7 +3476,7 @@
       </c>
     </row>
     <row r="88" spans="1:8" ht="34" x14ac:dyDescent="0.2">
-      <c r="A88" s="6"/>
+      <c r="A88" s="8"/>
       <c r="B88" t="s">
         <v>217</v>
       </c>
@@ -3449,7 +3497,7 @@
       </c>
     </row>
     <row r="89" spans="1:8" ht="34" x14ac:dyDescent="0.2">
-      <c r="A89" s="6"/>
+      <c r="A89" s="8"/>
       <c r="B89" t="s">
         <v>221</v>
       </c>
@@ -3470,7 +3518,7 @@
       </c>
     </row>
     <row r="90" spans="1:8" ht="34" x14ac:dyDescent="0.2">
-      <c r="A90" s="6"/>
+      <c r="A90" s="8"/>
       <c r="B90" t="s">
         <v>223</v>
       </c>
@@ -3491,7 +3539,7 @@
       </c>
     </row>
     <row r="91" spans="1:8" ht="51" x14ac:dyDescent="0.2">
-      <c r="A91" s="6"/>
+      <c r="A91" s="8"/>
       <c r="B91" t="s">
         <v>225</v>
       </c>
@@ -3512,7 +3560,7 @@
       </c>
     </row>
     <row r="92" spans="1:8" ht="34" x14ac:dyDescent="0.2">
-      <c r="A92" s="6"/>
+      <c r="A92" s="8"/>
       <c r="B92" t="s">
         <v>227</v>
       </c>
@@ -3533,7 +3581,7 @@
       </c>
     </row>
     <row r="93" spans="1:8" ht="17" x14ac:dyDescent="0.2">
-      <c r="A93" s="6" t="s">
+      <c r="A93" s="8" t="s">
         <v>229</v>
       </c>
       <c r="F93" t="s">
@@ -3544,8 +3592,8 @@
       </c>
     </row>
     <row r="94" spans="1:8" ht="17" x14ac:dyDescent="0.2">
-      <c r="A94" s="6"/>
-      <c r="B94" s="6" t="s">
+      <c r="A94" s="8"/>
+      <c r="B94" s="8" t="s">
         <v>101</v>
       </c>
       <c r="F94" t="s">
@@ -3556,8 +3604,8 @@
       </c>
     </row>
     <row r="95" spans="1:8" ht="51" x14ac:dyDescent="0.2">
-      <c r="A95" s="6"/>
-      <c r="B95" s="6"/>
+      <c r="A95" s="8"/>
+      <c r="B95" s="8"/>
       <c r="C95" t="s">
         <v>233</v>
       </c>
@@ -3578,8 +3626,8 @@
       </c>
     </row>
     <row r="96" spans="1:8" ht="51" x14ac:dyDescent="0.2">
-      <c r="A96" s="6"/>
-      <c r="B96" s="6"/>
+      <c r="A96" s="8"/>
+      <c r="B96" s="8"/>
       <c r="C96" t="s">
         <v>236</v>
       </c>
@@ -3600,8 +3648,8 @@
       </c>
     </row>
     <row r="97" spans="1:8" ht="17" x14ac:dyDescent="0.2">
-      <c r="A97" s="6"/>
-      <c r="B97" s="6"/>
+      <c r="A97" s="8"/>
+      <c r="B97" s="8"/>
       <c r="C97" t="s">
         <v>239</v>
       </c>
@@ -3619,8 +3667,8 @@
       </c>
     </row>
     <row r="98" spans="1:8" ht="17" x14ac:dyDescent="0.2">
-      <c r="A98" s="6"/>
-      <c r="B98" s="6"/>
+      <c r="A98" s="8"/>
+      <c r="B98" s="8"/>
       <c r="C98" t="s">
         <v>385</v>
       </c>
@@ -3635,8 +3683,8 @@
       </c>
     </row>
     <row r="99" spans="1:8" ht="34" x14ac:dyDescent="0.2">
-      <c r="A99" s="6"/>
-      <c r="B99" s="6"/>
+      <c r="A99" s="8"/>
+      <c r="B99" s="8"/>
       <c r="C99" t="s">
         <v>386</v>
       </c>
@@ -3657,8 +3705,8 @@
       </c>
     </row>
     <row r="100" spans="1:8" ht="51" x14ac:dyDescent="0.2">
-      <c r="A100" s="6"/>
-      <c r="B100" s="6"/>
+      <c r="A100" s="8"/>
+      <c r="B100" s="8"/>
       <c r="C100" t="s">
         <v>387</v>
       </c>
@@ -3679,8 +3727,8 @@
       </c>
     </row>
     <row r="101" spans="1:8" ht="34" x14ac:dyDescent="0.2">
-      <c r="A101" s="6"/>
-      <c r="B101" s="6"/>
+      <c r="A101" s="8"/>
+      <c r="B101" s="8"/>
       <c r="C101" t="s">
         <v>256</v>
       </c>
@@ -3701,8 +3749,8 @@
       </c>
     </row>
     <row r="102" spans="1:8" ht="51" x14ac:dyDescent="0.2">
-      <c r="A102" s="6"/>
-      <c r="B102" s="6"/>
+      <c r="A102" s="8"/>
+      <c r="B102" s="8"/>
       <c r="C102" t="s">
         <v>258</v>
       </c>
@@ -3723,8 +3771,8 @@
       </c>
     </row>
     <row r="103" spans="1:8" ht="34" x14ac:dyDescent="0.2">
-      <c r="A103" s="6"/>
-      <c r="B103" s="6"/>
+      <c r="A103" s="8"/>
+      <c r="B103" s="8"/>
       <c r="C103" t="s">
         <v>261</v>
       </c>
@@ -3742,8 +3790,8 @@
       </c>
     </row>
     <row r="104" spans="1:8" ht="17" x14ac:dyDescent="0.2">
-      <c r="A104" s="6"/>
-      <c r="B104" s="6" t="s">
+      <c r="A104" s="8"/>
+      <c r="B104" s="8" t="s">
         <v>231</v>
       </c>
       <c r="F104" t="s">
@@ -3754,8 +3802,8 @@
       </c>
     </row>
     <row r="105" spans="1:8" ht="68" x14ac:dyDescent="0.2">
-      <c r="A105" s="6"/>
-      <c r="B105" s="6"/>
+      <c r="A105" s="8"/>
+      <c r="B105" s="8"/>
       <c r="C105" t="s">
         <v>233</v>
       </c>
@@ -3776,8 +3824,8 @@
       </c>
     </row>
     <row r="106" spans="1:8" ht="34" x14ac:dyDescent="0.2">
-      <c r="A106" s="6"/>
-      <c r="B106" s="6"/>
+      <c r="A106" s="8"/>
+      <c r="B106" s="8"/>
       <c r="C106" t="s">
         <v>236</v>
       </c>
@@ -3798,8 +3846,8 @@
       </c>
     </row>
     <row r="107" spans="1:8" ht="17" x14ac:dyDescent="0.2">
-      <c r="A107" s="6"/>
-      <c r="B107" s="6"/>
+      <c r="A107" s="8"/>
+      <c r="B107" s="8"/>
       <c r="C107" t="s">
         <v>239</v>
       </c>
@@ -3817,8 +3865,8 @@
       </c>
     </row>
     <row r="108" spans="1:8" ht="17" x14ac:dyDescent="0.2">
-      <c r="A108" s="6"/>
-      <c r="B108" s="6"/>
+      <c r="A108" s="8"/>
+      <c r="B108" s="8"/>
       <c r="C108" t="s">
         <v>243</v>
       </c>
@@ -3833,8 +3881,8 @@
       </c>
     </row>
     <row r="109" spans="1:8" ht="17" x14ac:dyDescent="0.2">
-      <c r="A109" s="6"/>
-      <c r="B109" s="6"/>
+      <c r="A109" s="8"/>
+      <c r="B109" s="8"/>
       <c r="C109" t="s">
         <v>245</v>
       </c>
@@ -3855,8 +3903,8 @@
       </c>
     </row>
     <row r="110" spans="1:8" ht="51" x14ac:dyDescent="0.2">
-      <c r="A110" s="6"/>
-      <c r="B110" s="6"/>
+      <c r="A110" s="8"/>
+      <c r="B110" s="8"/>
       <c r="C110" t="s">
         <v>249</v>
       </c>
@@ -3877,8 +3925,8 @@
       </c>
     </row>
     <row r="111" spans="1:8" ht="17" x14ac:dyDescent="0.2">
-      <c r="A111" s="6"/>
-      <c r="B111" s="6"/>
+      <c r="A111" s="8"/>
+      <c r="B111" s="8"/>
       <c r="C111" t="s">
         <v>254</v>
       </c>
@@ -3896,8 +3944,8 @@
       </c>
     </row>
     <row r="112" spans="1:8" ht="17" x14ac:dyDescent="0.2">
-      <c r="A112" s="6"/>
-      <c r="B112" s="6"/>
+      <c r="A112" s="8"/>
+      <c r="B112" s="8"/>
       <c r="C112" t="s">
         <v>256</v>
       </c>
@@ -3918,8 +3966,8 @@
       </c>
     </row>
     <row r="113" spans="1:8" ht="51" x14ac:dyDescent="0.2">
-      <c r="A113" s="6"/>
-      <c r="B113" s="6"/>
+      <c r="A113" s="8"/>
+      <c r="B113" s="8"/>
       <c r="C113" t="s">
         <v>258</v>
       </c>
@@ -3940,8 +3988,8 @@
       </c>
     </row>
     <row r="114" spans="1:8" ht="34" x14ac:dyDescent="0.2">
-      <c r="A114" s="6"/>
-      <c r="B114" s="6"/>
+      <c r="A114" s="8"/>
+      <c r="B114" s="8"/>
       <c r="C114" t="s">
         <v>261</v>
       </c>
@@ -3959,8 +4007,8 @@
       </c>
     </row>
     <row r="115" spans="1:8" ht="34" x14ac:dyDescent="0.2">
-      <c r="A115" s="6"/>
-      <c r="B115" s="6" t="s">
+      <c r="A115" s="8"/>
+      <c r="B115" s="8" t="s">
         <v>263</v>
       </c>
       <c r="F115" t="s">
@@ -3971,8 +4019,8 @@
       </c>
     </row>
     <row r="116" spans="1:8" ht="68" x14ac:dyDescent="0.2">
-      <c r="A116" s="6"/>
-      <c r="B116" s="6"/>
+      <c r="A116" s="8"/>
+      <c r="B116" s="8"/>
       <c r="C116" t="s">
         <v>233</v>
       </c>
@@ -3993,8 +4041,8 @@
       </c>
     </row>
     <row r="117" spans="1:8" ht="34" x14ac:dyDescent="0.2">
-      <c r="A117" s="6"/>
-      <c r="B117" s="6"/>
+      <c r="A117" s="8"/>
+      <c r="B117" s="8"/>
       <c r="C117" t="s">
         <v>236</v>
       </c>
@@ -4015,8 +4063,8 @@
       </c>
     </row>
     <row r="118" spans="1:8" ht="17" x14ac:dyDescent="0.2">
-      <c r="A118" s="6"/>
-      <c r="B118" s="6"/>
+      <c r="A118" s="8"/>
+      <c r="B118" s="8"/>
       <c r="C118" t="s">
         <v>239</v>
       </c>
@@ -4034,8 +4082,8 @@
       </c>
     </row>
     <row r="119" spans="1:8" ht="34" x14ac:dyDescent="0.2">
-      <c r="A119" s="6"/>
-      <c r="B119" s="6"/>
+      <c r="A119" s="8"/>
+      <c r="B119" s="8"/>
       <c r="C119" t="s">
         <v>243</v>
       </c>
@@ -4053,8 +4101,8 @@
       </c>
     </row>
     <row r="120" spans="1:8" ht="17" x14ac:dyDescent="0.2">
-      <c r="A120" s="6"/>
-      <c r="B120" s="6"/>
+      <c r="A120" s="8"/>
+      <c r="B120" s="8"/>
       <c r="C120" t="s">
         <v>271</v>
       </c>
@@ -4072,7 +4120,7 @@
       </c>
     </row>
     <row r="121" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A121" s="6" t="s">
+      <c r="A121" s="8" t="s">
         <v>273</v>
       </c>
       <c r="F121" t="s">
@@ -4080,7 +4128,7 @@
       </c>
     </row>
     <row r="122" spans="1:8" ht="17" x14ac:dyDescent="0.2">
-      <c r="A122" s="6"/>
+      <c r="A122" s="8"/>
       <c r="B122" t="s">
         <v>233</v>
       </c>
@@ -4098,7 +4146,7 @@
       </c>
     </row>
     <row r="123" spans="1:8" ht="17" x14ac:dyDescent="0.2">
-      <c r="A123" s="6"/>
+      <c r="A123" s="8"/>
       <c r="B123" t="s">
         <v>239</v>
       </c>
@@ -4113,7 +4161,7 @@
       </c>
     </row>
     <row r="124" spans="1:8" ht="17" x14ac:dyDescent="0.2">
-      <c r="A124" s="6"/>
+      <c r="A124" s="8"/>
       <c r="B124" t="s">
         <v>243</v>
       </c>
@@ -4128,7 +4176,7 @@
       </c>
     </row>
     <row r="125" spans="1:8" ht="17" x14ac:dyDescent="0.2">
-      <c r="A125" s="6"/>
+      <c r="A125" s="8"/>
       <c r="B125" t="s">
         <v>278</v>
       </c>
@@ -4143,7 +4191,7 @@
       </c>
     </row>
     <row r="126" spans="1:8" ht="34" x14ac:dyDescent="0.2">
-      <c r="A126" s="6"/>
+      <c r="A126" s="8"/>
       <c r="B126" t="s">
         <v>280</v>
       </c>
@@ -4164,7 +4212,7 @@
       </c>
     </row>
     <row r="127" spans="1:8" ht="34" x14ac:dyDescent="0.2">
-      <c r="A127" s="6"/>
+      <c r="A127" s="8"/>
       <c r="B127" t="s">
         <v>285</v>
       </c>
@@ -4182,7 +4230,7 @@
       </c>
     </row>
     <row r="128" spans="1:8" ht="17" x14ac:dyDescent="0.2">
-      <c r="A128" s="6" t="s">
+      <c r="A128" s="8" t="s">
         <v>288</v>
       </c>
       <c r="F128" t="s">
@@ -4193,7 +4241,7 @@
       </c>
     </row>
     <row r="129" spans="1:8" ht="17" x14ac:dyDescent="0.2">
-      <c r="A129" s="6"/>
+      <c r="A129" s="8"/>
       <c r="B129" t="s">
         <v>290</v>
       </c>
@@ -4214,7 +4262,7 @@
       </c>
     </row>
     <row r="130" spans="1:8" ht="34" x14ac:dyDescent="0.2">
-      <c r="A130" s="6"/>
+      <c r="A130" s="8"/>
       <c r="B130" t="s">
         <v>293</v>
       </c>
@@ -4235,7 +4283,7 @@
       </c>
     </row>
     <row r="131" spans="1:8" ht="17" x14ac:dyDescent="0.2">
-      <c r="A131" s="6"/>
+      <c r="A131" s="8"/>
       <c r="B131" t="s">
         <v>296</v>
       </c>
@@ -4253,7 +4301,7 @@
       </c>
     </row>
     <row r="132" spans="1:8" ht="17" x14ac:dyDescent="0.2">
-      <c r="A132" s="6"/>
+      <c r="A132" s="8"/>
       <c r="B132" t="s">
         <v>300</v>
       </c>
@@ -4271,7 +4319,7 @@
       </c>
     </row>
     <row r="133" spans="1:8" ht="17" x14ac:dyDescent="0.2">
-      <c r="A133" s="6" t="s">
+      <c r="A133" s="8" t="s">
         <v>302</v>
       </c>
       <c r="F133" t="s">
@@ -4282,7 +4330,7 @@
       </c>
     </row>
     <row r="134" spans="1:8" ht="34" x14ac:dyDescent="0.2">
-      <c r="A134" s="6"/>
+      <c r="A134" s="8"/>
       <c r="B134" t="s">
         <v>305</v>
       </c>
@@ -4303,7 +4351,7 @@
       </c>
     </row>
     <row r="135" spans="1:8" ht="51" x14ac:dyDescent="0.2">
-      <c r="A135" s="6"/>
+      <c r="A135" s="8"/>
       <c r="B135" t="s">
         <v>309</v>
       </c>
@@ -4324,7 +4372,7 @@
       </c>
     </row>
     <row r="136" spans="1:8" ht="34" x14ac:dyDescent="0.2">
-      <c r="A136" s="6" t="s">
+      <c r="A136" s="8" t="s">
         <v>313</v>
       </c>
       <c r="F136" t="s">
@@ -4335,7 +4383,7 @@
       </c>
     </row>
     <row r="137" spans="1:8" ht="51" x14ac:dyDescent="0.2">
-      <c r="A137" s="6"/>
+      <c r="A137" s="8"/>
       <c r="B137" t="s">
         <v>316</v>
       </c>
@@ -4353,7 +4401,7 @@
       </c>
     </row>
     <row r="138" spans="1:8" ht="51" x14ac:dyDescent="0.2">
-      <c r="A138" s="6"/>
+      <c r="A138" s="8"/>
       <c r="B138" t="s">
         <v>353</v>
       </c>
@@ -4374,7 +4422,7 @@
       </c>
     </row>
     <row r="139" spans="1:8" ht="17" x14ac:dyDescent="0.2">
-      <c r="A139" s="6"/>
+      <c r="A139" s="8"/>
       <c r="B139" t="s">
         <v>322</v>
       </c>
@@ -4392,7 +4440,7 @@
       </c>
     </row>
     <row r="140" spans="1:8" ht="17" x14ac:dyDescent="0.2">
-      <c r="A140" s="6"/>
+      <c r="A140" s="8"/>
       <c r="B140" t="s">
         <v>325</v>
       </c>
@@ -4410,7 +4458,7 @@
       </c>
     </row>
     <row r="141" spans="1:8" ht="17" x14ac:dyDescent="0.2">
-      <c r="A141" s="6" t="s">
+      <c r="A141" s="10" t="s">
         <v>314</v>
       </c>
       <c r="F141" t="s">
@@ -4421,8 +4469,8 @@
       </c>
     </row>
     <row r="142" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A142" s="6"/>
-      <c r="B142" s="7" t="s">
+      <c r="A142" s="10"/>
+      <c r="B142" s="9" t="s">
         <v>415</v>
       </c>
       <c r="F142" t="s">
@@ -4430,8 +4478,8 @@
       </c>
     </row>
     <row r="143" spans="1:8" ht="17" x14ac:dyDescent="0.2">
-      <c r="A143" s="6"/>
-      <c r="B143" s="7"/>
+      <c r="A143" s="10"/>
+      <c r="B143" s="9"/>
       <c r="C143" t="s">
         <v>233</v>
       </c>
@@ -4446,8 +4494,8 @@
       </c>
     </row>
     <row r="144" spans="1:8" ht="34" x14ac:dyDescent="0.2">
-      <c r="A144" s="6"/>
-      <c r="B144" s="7"/>
+      <c r="A144" s="10"/>
+      <c r="B144" s="9"/>
       <c r="C144" t="s">
         <v>333</v>
       </c>
@@ -4468,8 +4516,8 @@
       </c>
     </row>
     <row r="145" spans="1:8" ht="17" x14ac:dyDescent="0.2">
-      <c r="A145" s="6"/>
-      <c r="B145" s="7"/>
+      <c r="A145" s="10"/>
+      <c r="B145" s="9"/>
       <c r="C145" t="s">
         <v>412</v>
       </c>
@@ -4487,8 +4535,8 @@
       </c>
     </row>
     <row r="146" spans="1:8" ht="17" x14ac:dyDescent="0.2">
-      <c r="A146" s="6"/>
-      <c r="B146" s="6" t="s">
+      <c r="A146" s="10"/>
+      <c r="B146" s="8" t="s">
         <v>328</v>
       </c>
       <c r="F146" t="s">
@@ -4499,8 +4547,8 @@
       </c>
     </row>
     <row r="147" spans="1:8" ht="17" x14ac:dyDescent="0.2">
-      <c r="A147" s="6"/>
-      <c r="B147" s="6"/>
+      <c r="A147" s="10"/>
+      <c r="B147" s="8"/>
       <c r="C147" t="s">
         <v>233</v>
       </c>
@@ -4518,8 +4566,8 @@
       </c>
     </row>
     <row r="148" spans="1:8" ht="17" x14ac:dyDescent="0.2">
-      <c r="A148" s="6"/>
-      <c r="B148" s="6"/>
+      <c r="A148" s="10"/>
+      <c r="B148" s="8"/>
       <c r="C148" t="s">
         <v>331</v>
       </c>
@@ -4537,8 +4585,8 @@
       </c>
     </row>
     <row r="149" spans="1:8" ht="34" x14ac:dyDescent="0.2">
-      <c r="A149" s="6"/>
-      <c r="B149" s="6"/>
+      <c r="A149" s="10"/>
+      <c r="B149" s="8"/>
       <c r="C149" t="s">
         <v>333</v>
       </c>
@@ -4559,79 +4607,194 @@
       </c>
     </row>
     <row r="150" spans="1:8" ht="17" x14ac:dyDescent="0.2">
-      <c r="A150" s="6"/>
-      <c r="B150" s="6" t="s">
-        <v>338</v>
-      </c>
-      <c r="E150" s="2" t="s">
-        <v>63</v>
+      <c r="A150" s="10"/>
+      <c r="B150" s="9" t="s">
+        <v>424</v>
       </c>
       <c r="F150" t="s">
         <v>314</v>
       </c>
+      <c r="H150" s="2" t="s">
+        <v>329</v>
+      </c>
     </row>
     <row r="151" spans="1:8" ht="17" x14ac:dyDescent="0.2">
-      <c r="A151" s="6"/>
-      <c r="B151" s="6"/>
+      <c r="A151" s="10"/>
+      <c r="B151" s="9"/>
       <c r="C151" t="s">
         <v>233</v>
       </c>
       <c r="D151" s="4" t="s">
-        <v>391</v>
+        <v>364</v>
+      </c>
+      <c r="E151" s="2" t="s">
+        <v>63</v>
       </c>
       <c r="F151" t="s">
         <v>314</v>
       </c>
       <c r="G151" s="2" t="s">
-        <v>339</v>
+        <v>430</v>
       </c>
     </row>
     <row r="152" spans="1:8" ht="17" x14ac:dyDescent="0.2">
-      <c r="A152" s="6"/>
-      <c r="B152" s="6"/>
+      <c r="A152" s="10"/>
+      <c r="B152" s="9"/>
       <c r="C152" t="s">
-        <v>340</v>
+        <v>423</v>
       </c>
       <c r="D152" t="s">
-        <v>281</v>
+        <v>399</v>
       </c>
       <c r="F152" t="s">
         <v>314</v>
       </c>
       <c r="G152" s="2" t="s">
-        <v>341</v>
+        <v>431</v>
       </c>
       <c r="H152" s="2" t="s">
         <v>242</v>
       </c>
     </row>
     <row r="153" spans="1:8" ht="17" x14ac:dyDescent="0.2">
-      <c r="A153" s="6"/>
-      <c r="B153" t="s">
-        <v>342</v>
-      </c>
-      <c r="D153" s="4" t="s">
-        <v>391</v>
+      <c r="A153" s="10"/>
+      <c r="B153" s="9"/>
+      <c r="C153" t="s">
+        <v>425</v>
+      </c>
+      <c r="D153" t="s">
+        <v>427</v>
       </c>
       <c r="E153" s="2" t="s">
-        <v>63</v>
+        <v>428</v>
       </c>
       <c r="F153" t="s">
         <v>314</v>
       </c>
       <c r="G153" s="2" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="154" spans="1:8" ht="34" x14ac:dyDescent="0.2">
+      <c r="A154" s="10"/>
+      <c r="B154" s="9"/>
+      <c r="C154" t="s">
+        <v>426</v>
+      </c>
+      <c r="D154" s="4" t="s">
+        <v>391</v>
+      </c>
+      <c r="E154" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="F154" t="s">
+        <v>314</v>
+      </c>
+      <c r="G154" s="2" t="s">
+        <v>432</v>
+      </c>
+      <c r="H154" s="2" t="s">
+        <v>433</v>
+      </c>
+    </row>
+    <row r="155" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="A155" s="10"/>
+      <c r="B155" s="9"/>
+      <c r="C155" t="s">
+        <v>434</v>
+      </c>
+      <c r="D155">
+        <v>0.97</v>
+      </c>
+      <c r="E155" s="2" t="s">
+        <v>435</v>
+      </c>
+      <c r="F155" t="s">
+        <v>314</v>
+      </c>
+      <c r="G155" s="2" t="s">
+        <v>436</v>
+      </c>
+    </row>
+    <row r="156" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="A156" s="6"/>
+      <c r="B156" s="8" t="s">
+        <v>338</v>
+      </c>
+      <c r="E156" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="F156" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="157" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="A157" s="6"/>
+      <c r="B157" s="8"/>
+      <c r="C157" t="s">
+        <v>233</v>
+      </c>
+      <c r="D157" s="4" t="s">
+        <v>391</v>
+      </c>
+      <c r="F157" t="s">
+        <v>314</v>
+      </c>
+      <c r="G157" s="2" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="158" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="A158" s="6"/>
+      <c r="B158" s="8"/>
+      <c r="C158" t="s">
+        <v>340</v>
+      </c>
+      <c r="D158" t="s">
+        <v>281</v>
+      </c>
+      <c r="F158" t="s">
+        <v>314</v>
+      </c>
+      <c r="G158" s="2" t="s">
+        <v>341</v>
+      </c>
+      <c r="H158" s="2" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="159" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="A159" s="6"/>
+      <c r="B159" t="s">
+        <v>342</v>
+      </c>
+      <c r="D159" s="4" t="s">
+        <v>391</v>
+      </c>
+      <c r="E159" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="F159" t="s">
+        <v>314</v>
+      </c>
+      <c r="G159" s="2" t="s">
         <v>343</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:H153" xr:uid="{65E3A469-1B8A-364D-8D4D-FD3FF55840DE}"/>
-  <mergeCells count="28">
-    <mergeCell ref="A58:A62"/>
-    <mergeCell ref="B142:B145"/>
-    <mergeCell ref="B50:B52"/>
-    <mergeCell ref="B53:B55"/>
-    <mergeCell ref="B146:B149"/>
-    <mergeCell ref="B150:B152"/>
+  <autoFilter ref="A1:H159" xr:uid="{65E3A469-1B8A-364D-8D4D-FD3FF55840DE}"/>
+  <mergeCells count="29">
+    <mergeCell ref="A18:A24"/>
+    <mergeCell ref="B19:B21"/>
+    <mergeCell ref="B22:B24"/>
+    <mergeCell ref="A27:A33"/>
+    <mergeCell ref="A34:A56"/>
+    <mergeCell ref="B35:B37"/>
+    <mergeCell ref="B41:B43"/>
+    <mergeCell ref="B44:B46"/>
+    <mergeCell ref="B47:B49"/>
+    <mergeCell ref="B38:B40"/>
+    <mergeCell ref="B156:B158"/>
     <mergeCell ref="A64:A79"/>
     <mergeCell ref="A80:A84"/>
     <mergeCell ref="A85:A92"/>
@@ -4642,18 +4805,14 @@
     <mergeCell ref="A128:A132"/>
     <mergeCell ref="A133:A135"/>
     <mergeCell ref="A136:A140"/>
-    <mergeCell ref="A141:A153"/>
     <mergeCell ref="B94:B103"/>
-    <mergeCell ref="A18:A24"/>
-    <mergeCell ref="B19:B21"/>
-    <mergeCell ref="B22:B24"/>
-    <mergeCell ref="A27:A33"/>
-    <mergeCell ref="A34:A56"/>
-    <mergeCell ref="B35:B37"/>
-    <mergeCell ref="B41:B43"/>
-    <mergeCell ref="B44:B46"/>
-    <mergeCell ref="B47:B49"/>
-    <mergeCell ref="B38:B40"/>
+    <mergeCell ref="B150:B155"/>
+    <mergeCell ref="A141:A155"/>
+    <mergeCell ref="A58:A62"/>
+    <mergeCell ref="B142:B145"/>
+    <mergeCell ref="B50:B52"/>
+    <mergeCell ref="B53:B55"/>
+    <mergeCell ref="B146:B149"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>